<commit_message>
delete some unuseful .swp and add hdu6319,hdu6321,hdu6335,hdu6336,hdu6338,hdu6342
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="827">
   <si>
     <t>OJ</t>
   </si>
@@ -9985,6 +9985,234 @@
       </rPr>
       <t>;dp</t>
     </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Euler Function</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ascending Rating</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>单调队列</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic Graph Matching</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>状压</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grab The Tree</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>博弈论</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interstellar Travel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>思维;计算几何</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Visual Cube</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>大模拟</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nothing is Impossible</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matrix from Arrays</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>思维</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Depth-First Search</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>树型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>动态开点线段树</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expression in Memories</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -10059,7 +10287,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top"/>
     </xf>
@@ -10074,6 +10302,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -10416,8 +10656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -11108,7 +11348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A234" workbookViewId="0">
       <selection activeCell="A269" sqref="A269"/>
     </sheetView>
   </sheetViews>
@@ -16356,17 +16596,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="22.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="55.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="22.28515625" style="1"/>
   </cols>
@@ -16809,10 +17049,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="5"/>
+      <c r="D26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="9"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -16830,10 +17070,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="5"/>
+      <c r="D27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -16851,10 +17091,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="5"/>
+      <c r="D28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="9"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -16872,10 +17112,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="5"/>
+      <c r="D29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -16893,10 +17133,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="5"/>
+      <c r="D30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="9"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -16911,10 +17151,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="5"/>
+      <c r="D31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="9"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -16929,10 +17169,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="5"/>
+      <c r="D32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="9"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -16947,10 +17187,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="D33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="9"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -16968,10 +17208,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="9">
         <v>97</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="9"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -16986,10 +17226,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="5"/>
+      <c r="D35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="9"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -17004,10 +17244,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="5"/>
+      <c r="D36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -17022,10 +17262,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="5"/>
+      <c r="D37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="9"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -17040,10 +17280,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="5"/>
+      <c r="D38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -17061,10 +17301,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="5"/>
+      <c r="D39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -17082,10 +17322,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="5"/>
+      <c r="D40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -17100,10 +17340,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="5"/>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -17121,10 +17361,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="5"/>
+      <c r="D42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -17139,10 +17379,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="5"/>
+      <c r="D43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -17160,10 +17400,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="5"/>
+      <c r="D44" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -17178,10 +17418,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="5"/>
+      <c r="D45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -17196,10 +17436,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="5"/>
+      <c r="D46" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -17214,10 +17454,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="5"/>
+      <c r="D47" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="9"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -17235,10 +17475,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="5"/>
+      <c r="D48" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="9"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -17253,10 +17493,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="5"/>
+      <c r="D49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="9"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -17274,10 +17514,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="5"/>
+      <c r="D50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="9"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -17295,10 +17535,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="5"/>
+      <c r="D51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="9"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -17313,10 +17553,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="5"/>
+      <c r="D52" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="9"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -17331,10 +17571,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="5"/>
+      <c r="D53" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="9"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -17349,10 +17589,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="5"/>
+      <c r="D54" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="9"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -17367,10 +17607,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="5"/>
+      <c r="D55" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="9"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -17385,10 +17625,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="5"/>
+      <c r="D56" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="9"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -17403,10 +17643,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="5"/>
+      <c r="D57" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="9"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -17421,10 +17661,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="5"/>
+      <c r="D58" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="9"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -17439,10 +17679,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="5"/>
+      <c r="D59" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="9"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -17460,10 +17700,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="5"/>
+      <c r="D60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="9"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -17478,10 +17718,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="5"/>
+      <c r="D61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="9"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -17499,181 +17739,391 @@
       <c r="C62" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="9" t="s">
         <v>799</v>
       </c>
-      <c r="E62" s="5"/>
+      <c r="E62" s="9"/>
       <c r="F62" s="1" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1">
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
+      <c r="A63" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6322</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="E63" s="9"/>
+      <c r="F63" s="5" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1">
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="4:5" ht="18" customHeight="1">
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="4:5" ht="18" customHeight="1">
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="4:5" ht="18" customHeight="1">
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="4:5" ht="18" customHeight="1">
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-    </row>
-    <row r="69" spans="4:5" ht="18" customHeight="1">
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="4:5" ht="18" customHeight="1">
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="4:5" ht="18" customHeight="1">
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="4:5" ht="18" customHeight="1">
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="4:5" ht="18" customHeight="1">
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="4:5" ht="18" customHeight="1">
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-    </row>
-    <row r="75" spans="4:5" ht="18" customHeight="1">
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-    </row>
-    <row r="76" spans="4:5" ht="18" customHeight="1">
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-    </row>
-    <row r="77" spans="4:5" ht="18" customHeight="1">
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-    </row>
-    <row r="78" spans="4:5" ht="18" customHeight="1">
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="4:5" ht="18" customHeight="1">
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" spans="4:5" ht="18" customHeight="1">
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
+      <c r="A64" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="B64" s="1">
+        <v>6319</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="E64" s="9"/>
+      <c r="F64" s="8" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="18" customHeight="1">
+      <c r="A65" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="B65" s="1">
+        <v>6321</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="E65" s="9"/>
+      <c r="F65" s="6" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="18" customHeight="1">
+      <c r="A66" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="B66" s="1">
+        <v>6324</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="E66" s="9"/>
+      <c r="F66" s="6" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="18" customHeight="1">
+      <c r="A67" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="B67" s="1">
+        <v>6325</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="E67" s="9"/>
+      <c r="F67" s="6" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="18" customHeight="1">
+      <c r="A68" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="B68" s="1">
+        <v>6330</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>815</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="8" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="18" customHeight="1">
+      <c r="A69" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="B69" s="1">
+        <v>6335</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="E69" s="9"/>
+      <c r="F69" s="7" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="18" customHeight="1">
+      <c r="A70" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="B70" s="1">
+        <v>6336</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="8" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="18" customHeight="1">
+      <c r="A71" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="B71" s="1">
+        <v>6338</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="7" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="18" customHeight="1">
+      <c r="A72" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="B72" s="1">
+        <v>6342</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="8" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="18" customHeight="1">
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+    </row>
+    <row r="74" spans="1:6" ht="18" customHeight="1">
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+    </row>
+    <row r="75" spans="1:6" ht="18" customHeight="1">
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+    </row>
+    <row r="76" spans="1:6" ht="18" customHeight="1">
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="1:6" ht="18" customHeight="1">
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78" spans="1:6" ht="18" customHeight="1">
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="1:6" ht="18" customHeight="1">
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+    </row>
+    <row r="80" spans="1:6" ht="18" customHeight="1">
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
     </row>
     <row r="81" spans="4:5" ht="18" customHeight="1">
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
     </row>
     <row r="82" spans="4:5" ht="18" customHeight="1">
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
     </row>
     <row r="83" spans="4:5" ht="18" customHeight="1">
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
     </row>
     <row r="84" spans="4:5" ht="18" customHeight="1">
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
     </row>
     <row r="85" spans="4:5" ht="18" customHeight="1">
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
     </row>
     <row r="86" spans="4:5" ht="18" customHeight="1">
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
     </row>
     <row r="87" spans="4:5" ht="18" customHeight="1">
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
     </row>
     <row r="88" spans="4:5" ht="18" customHeight="1">
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
     </row>
     <row r="89" spans="4:5" ht="18" customHeight="1">
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
     </row>
     <row r="90" spans="4:5" ht="18" customHeight="1">
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
     </row>
     <row r="91" spans="4:5" ht="18" customHeight="1">
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
     </row>
     <row r="92" spans="4:5" ht="18" customHeight="1">
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
     </row>
     <row r="93" spans="4:5" ht="18" customHeight="1">
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
     </row>
     <row r="94" spans="4:5" ht="18" customHeight="1">
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
     </row>
     <row r="95" spans="4:5" ht="18" customHeight="1">
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
     </row>
     <row r="96" spans="4:5" ht="18" customHeight="1">
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
     </row>
     <row r="97" spans="4:5" ht="18" customHeight="1">
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
     </row>
     <row r="98" spans="4:5" ht="18" customHeight="1">
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
     </row>
     <row r="99" spans="4:5" ht="18" customHeight="1">
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
     </row>
     <row r="100" spans="4:5" ht="18" customHeight="1">
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
     </row>
     <row r="101" spans="4:5" ht="18" customHeight="1">
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
     </row>
     <row r="102" spans="4:5" ht="18" customHeight="1">
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
     </row>
     <row r="103" spans="4:5" ht="18" customHeight="1">
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G61"/>
   <mergeCells count="78">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
     <mergeCell ref="D101:E101"/>
     <mergeCell ref="D102:E102"/>
     <mergeCell ref="D103:E103"/>
@@ -17682,76 +18132,6 @@
     <mergeCell ref="D98:E98"/>
     <mergeCell ref="D99:E99"/>
     <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
merge the programmes before into the repository
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="904">
   <si>
     <t>OJ</t>
   </si>
@@ -10628,6 +10628,423 @@
   </si>
   <si>
     <t>Photos of The Sky</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BestCoder</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>百度之星</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>资格赛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>百度之星</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>2019</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>资格赛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>百度之星</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>2020</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>资格赛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>百度之星</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>2021</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>资格赛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>百度之星</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>资格赛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>调查问卷</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>子串查询</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>字符串</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数规划</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分图最大权匹配</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列计数</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp;BIT</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>三原色图</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最小生成树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>贪心</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016A</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016B</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016C</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016D</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016E</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016F</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Death Note</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Segment Occurences</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vasya And The Mushrooms</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vasya And The Matrix</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rest In The Shade</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Road Projects</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>二分</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>思维</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>构造</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二分</t>
+    </r>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -10718,7 +11135,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -10739,6 +11156,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -17023,15 +17443,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="22.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
@@ -17478,10 +17899,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="8"/>
+      <c r="D26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="9"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -17499,10 +17920,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="8"/>
+      <c r="D27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -17520,10 +17941,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="8"/>
+      <c r="D28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="9"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -17541,10 +17962,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="8"/>
+      <c r="D29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -17562,10 +17983,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="8"/>
+      <c r="D30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="9"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -17580,10 +18001,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="8"/>
+      <c r="D31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="9"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -17598,10 +18019,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="8"/>
+      <c r="D32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="9"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -17616,10 +18037,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="8"/>
+      <c r="D33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="9"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -17637,10 +18058,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="9">
         <v>97</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="9"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -17655,10 +18076,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="8"/>
+      <c r="D35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="9"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -17673,10 +18094,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="8"/>
+      <c r="D36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -17691,10 +18112,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="8"/>
+      <c r="D37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="9"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -17709,10 +18130,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="8"/>
+      <c r="D38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -17730,10 +18151,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="8"/>
+      <c r="D39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -17751,10 +18172,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="8"/>
+      <c r="D40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -17769,10 +18190,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="8"/>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -17790,10 +18211,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="8"/>
+      <c r="D42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -17808,10 +18229,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="8"/>
+      <c r="D43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -17829,10 +18250,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="8"/>
+      <c r="D44" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -17847,10 +18268,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="8"/>
+      <c r="D45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -17865,10 +18286,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="8"/>
+      <c r="D46" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -17883,10 +18304,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="8"/>
+      <c r="D47" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="9"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -17904,10 +18325,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="8"/>
+      <c r="D48" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="9"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -17922,10 +18343,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="8"/>
+      <c r="D49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="9"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -17943,10 +18364,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="8"/>
+      <c r="D50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="9"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -17964,10 +18385,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="8"/>
+      <c r="D51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="9"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -17982,10 +18403,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="8"/>
+      <c r="D52" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="9"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -18000,10 +18421,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="8"/>
+      <c r="D53" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="9"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -18018,10 +18439,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="8"/>
+      <c r="D54" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="9"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -18036,10 +18457,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="8"/>
+      <c r="D55" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="9"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -18054,10 +18475,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="8"/>
+      <c r="D56" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="9"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -18072,10 +18493,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="8"/>
+      <c r="D57" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="9"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -18090,10 +18511,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="8"/>
+      <c r="D58" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="9"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -18108,10 +18529,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="8"/>
+      <c r="D59" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="9"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -18129,10 +18550,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="8"/>
+      <c r="D60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="9"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -18147,10 +18568,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="8"/>
+      <c r="D61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="9"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -18168,10 +18589,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="8"/>
+      <c r="D62" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="9"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -18186,10 +18607,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="8"/>
+      <c r="D63" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="9"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -18204,10 +18625,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="8"/>
+      <c r="D64" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="9"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -18222,10 +18643,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="8"/>
+      <c r="D65" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="9"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -18240,10 +18661,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="8"/>
+      <c r="D66" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="9"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -18258,10 +18679,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="8"/>
+      <c r="D67" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="9"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -18276,10 +18697,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="8"/>
+      <c r="D68" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="9"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -18294,10 +18715,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="8"/>
+      <c r="D69" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="9"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -18312,10 +18733,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="8"/>
+      <c r="D70" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="9"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -18330,10 +18751,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="8"/>
+      <c r="D71" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="9"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -18348,10 +18769,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="8"/>
+      <c r="D72" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="9"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -18366,10 +18787,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="8"/>
+      <c r="D73" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="9"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -18384,10 +18805,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="8"/>
+      <c r="D74" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="9"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -18402,10 +18823,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="8"/>
+      <c r="D75" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="9"/>
       <c r="F75" s="4" t="s">
         <v>821</v>
       </c>
@@ -18420,10 +18841,10 @@
       <c r="C76" s="7" t="s">
         <v>832</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E76" s="8"/>
+      <c r="E76" s="9"/>
       <c r="F76" s="7" t="s">
         <v>833</v>
       </c>
@@ -18438,10 +18859,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="9" t="s">
         <v>824</v>
       </c>
-      <c r="E77" s="8"/>
+      <c r="E77" s="9"/>
       <c r="F77" s="1" t="s">
         <v>825</v>
       </c>
@@ -18456,10 +18877,10 @@
       <c r="C78" s="7" t="s">
         <v>827</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E78" s="8"/>
+      <c r="E78" s="9"/>
       <c r="F78" s="7" t="s">
         <v>829</v>
       </c>
@@ -18474,10 +18895,10 @@
       <c r="C79" s="7" t="s">
         <v>834</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D79" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E79" s="8"/>
+      <c r="E79" s="9"/>
       <c r="F79" s="7" t="s">
         <v>835</v>
       </c>
@@ -18492,10 +18913,10 @@
       <c r="C80" s="7" t="s">
         <v>836</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E80" s="8"/>
+      <c r="E80" s="9"/>
       <c r="F80" s="3" t="s">
         <v>837</v>
       </c>
@@ -18510,10 +18931,10 @@
       <c r="C81" s="7" t="s">
         <v>838</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E81" s="8"/>
+      <c r="E81" s="9"/>
       <c r="F81" s="3" t="s">
         <v>839</v>
       </c>
@@ -18528,10 +18949,10 @@
       <c r="C82" s="7" t="s">
         <v>840</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E82" s="8"/>
+      <c r="E82" s="9"/>
       <c r="F82" s="3" t="s">
         <v>841</v>
       </c>
@@ -18546,10 +18967,10 @@
       <c r="C83" s="7" t="s">
         <v>842</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D83" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E83" s="8"/>
+      <c r="E83" s="9"/>
       <c r="F83" s="7" t="s">
         <v>843</v>
       </c>
@@ -18564,10 +18985,10 @@
       <c r="C84" s="7" t="s">
         <v>844</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D84" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E84" s="8"/>
+      <c r="E84" s="9"/>
       <c r="F84" s="3" t="s">
         <v>845</v>
       </c>
@@ -18582,10 +19003,10 @@
       <c r="C85" s="7" t="s">
         <v>846</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D85" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E85" s="8"/>
+      <c r="E85" s="9"/>
       <c r="F85" s="7" t="s">
         <v>847</v>
       </c>
@@ -18600,10 +19021,10 @@
       <c r="C86" s="7" t="s">
         <v>848</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D86" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E86" s="8"/>
+      <c r="E86" s="9"/>
       <c r="F86" s="7" t="s">
         <v>849</v>
       </c>
@@ -18618,10 +19039,10 @@
       <c r="C87" s="7" t="s">
         <v>850</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E87" s="8"/>
+      <c r="E87" s="9"/>
       <c r="F87" s="3" t="s">
         <v>851</v>
       </c>
@@ -18636,10 +19057,10 @@
       <c r="C88" s="7" t="s">
         <v>852</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D88" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E88" s="8"/>
+      <c r="E88" s="9"/>
       <c r="F88" s="3" t="s">
         <v>853</v>
       </c>
@@ -18654,10 +19075,10 @@
       <c r="C89" s="7" t="s">
         <v>854</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D89" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E89" s="8"/>
+      <c r="E89" s="9"/>
       <c r="F89" s="7" t="s">
         <v>855</v>
       </c>
@@ -18672,10 +19093,10 @@
       <c r="C90" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="D90" s="8" t="s">
+      <c r="D90" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E90" s="8"/>
+      <c r="E90" s="9"/>
       <c r="F90" s="7" t="s">
         <v>857</v>
       </c>
@@ -18690,10 +19111,10 @@
       <c r="C91" s="7" t="s">
         <v>863</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D91" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E91" s="8"/>
+      <c r="E91" s="9"/>
       <c r="F91" s="3" t="s">
         <v>845</v>
       </c>
@@ -18708,10 +19129,10 @@
       <c r="C92" s="7" t="s">
         <v>864</v>
       </c>
-      <c r="D92" s="8" t="s">
+      <c r="D92" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E92" s="8"/>
+      <c r="E92" s="9"/>
       <c r="F92" s="3" t="s">
         <v>845</v>
       </c>
@@ -18726,10 +19147,10 @@
       <c r="C93" s="7" t="s">
         <v>869</v>
       </c>
-      <c r="D93" s="8" t="s">
+      <c r="D93" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E93" s="8"/>
+      <c r="E93" s="9"/>
       <c r="F93" s="3" t="s">
         <v>839</v>
       </c>
@@ -18744,10 +19165,10 @@
       <c r="C94" s="7" t="s">
         <v>867</v>
       </c>
-      <c r="D94" s="8" t="s">
+      <c r="D94" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E94" s="8"/>
+      <c r="E94" s="9"/>
       <c r="F94" s="7" t="s">
         <v>868</v>
       </c>
@@ -18762,53 +19183,545 @@
       <c r="C95" s="7" t="s">
         <v>865</v>
       </c>
-      <c r="D95" s="8" t="s">
+      <c r="D95" s="9" t="s">
         <v>828</v>
       </c>
-      <c r="E95" s="8"/>
+      <c r="E95" s="9"/>
       <c r="F95" s="7" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="18" customHeight="1">
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-    </row>
-    <row r="97" spans="4:5" ht="18" customHeight="1">
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-    </row>
-    <row r="98" spans="4:5" ht="18" customHeight="1">
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-    </row>
-    <row r="99" spans="4:5" ht="18" customHeight="1">
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-    </row>
-    <row r="100" spans="4:5" ht="18" customHeight="1">
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-    </row>
-    <row r="101" spans="4:5" ht="18" customHeight="1">
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-    </row>
-    <row r="102" spans="4:5" ht="18" customHeight="1">
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-    </row>
-    <row r="103" spans="4:5" ht="18" customHeight="1">
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-    </row>
-    <row r="104" spans="4:5" ht="18" customHeight="1">
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
+      <c r="A96" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E96" s="9"/>
+      <c r="F96" s="3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="18" customHeight="1">
+      <c r="A97" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>872</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E97" s="9"/>
+      <c r="F97" s="8" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="18" customHeight="1">
+      <c r="A98" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>873</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E98" s="9"/>
+      <c r="F98" s="3" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="18" customHeight="1">
+      <c r="A99" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>874</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E99" s="9"/>
+      <c r="F99" s="8" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="18" customHeight="1">
+      <c r="A100" s="8" t="s">
+        <v>870</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E100" s="9"/>
+      <c r="F100" s="8" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="18" customHeight="1">
+      <c r="A101" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>888</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>894</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E101" s="9"/>
+      <c r="F101" s="3" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="18" customHeight="1">
+      <c r="A102" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>889</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>895</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E102" s="9"/>
+      <c r="F102" s="3" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="18" customHeight="1">
+      <c r="A103" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>890</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>896</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E103" s="9"/>
+      <c r="F103" s="3" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="18" customHeight="1">
+      <c r="A104" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>891</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>897</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E104" s="9"/>
+      <c r="F104" s="8" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="18" customHeight="1">
+      <c r="A105" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>892</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>898</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E105" s="9"/>
+      <c r="F105" s="8" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="18" customHeight="1">
+      <c r="A106" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>893</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>899</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E106" s="9"/>
+      <c r="F106" s="3" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="18" customHeight="1">
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+    </row>
+    <row r="108" spans="1:6" ht="18" customHeight="1">
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+    </row>
+    <row r="109" spans="1:6" ht="18" customHeight="1">
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+    </row>
+    <row r="110" spans="1:6" ht="18" customHeight="1">
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+    </row>
+    <row r="111" spans="1:6" ht="18" customHeight="1">
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+    </row>
+    <row r="112" spans="1:6" ht="18" customHeight="1">
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+    </row>
+    <row r="113" spans="4:5" ht="18" customHeight="1">
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+    </row>
+    <row r="114" spans="4:5" ht="18" customHeight="1">
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+    </row>
+    <row r="115" spans="4:5" ht="18" customHeight="1">
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+    </row>
+    <row r="116" spans="4:5" ht="18" customHeight="1">
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+    </row>
+    <row r="117" spans="4:5" ht="18" customHeight="1">
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+    </row>
+    <row r="118" spans="4:5" ht="18" customHeight="1">
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+    </row>
+    <row r="119" spans="4:5" ht="18" customHeight="1">
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+    </row>
+    <row r="120" spans="4:5" ht="18" customHeight="1">
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+    </row>
+    <row r="121" spans="4:5" ht="18" customHeight="1">
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+    </row>
+    <row r="122" spans="4:5" ht="18" customHeight="1">
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+    </row>
+    <row r="123" spans="4:5" ht="18" customHeight="1">
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+    </row>
+    <row r="124" spans="4:5" ht="18" customHeight="1">
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+    </row>
+    <row r="125" spans="4:5" ht="18" customHeight="1">
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+    </row>
+    <row r="126" spans="4:5" ht="18" customHeight="1">
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+    </row>
+    <row r="127" spans="4:5" ht="18" customHeight="1">
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+    </row>
+    <row r="128" spans="4:5" ht="18" customHeight="1">
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+    </row>
+    <row r="129" spans="4:5" ht="18" customHeight="1">
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+    </row>
+    <row r="130" spans="4:5" ht="18" customHeight="1">
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+    </row>
+    <row r="131" spans="4:5" ht="18" customHeight="1">
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+    </row>
+    <row r="132" spans="4:5" ht="18" customHeight="1">
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+    </row>
+    <row r="133" spans="4:5" ht="18" customHeight="1">
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+    </row>
+    <row r="134" spans="4:5" ht="18" customHeight="1">
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+    </row>
+    <row r="135" spans="4:5" ht="18" customHeight="1">
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+    </row>
+    <row r="136" spans="4:5" ht="18" customHeight="1">
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+    </row>
+    <row r="137" spans="4:5" ht="18" customHeight="1">
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+    </row>
+    <row r="138" spans="4:5" ht="18" customHeight="1">
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+    </row>
+    <row r="139" spans="4:5" ht="18" customHeight="1">
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+    </row>
+    <row r="140" spans="4:5" ht="18" customHeight="1">
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+    </row>
+    <row r="141" spans="4:5" ht="18" customHeight="1">
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+    </row>
+    <row r="142" spans="4:5" ht="18" customHeight="1">
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+    </row>
+    <row r="143" spans="4:5" ht="18" customHeight="1">
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+    </row>
+    <row r="144" spans="4:5" ht="18" customHeight="1">
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+    </row>
+    <row r="145" spans="4:5" ht="18" customHeight="1">
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+    </row>
+    <row r="146" spans="4:5" ht="18" customHeight="1">
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+    </row>
+    <row r="147" spans="4:5" ht="18" customHeight="1">
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+    </row>
+    <row r="148" spans="4:5" ht="18" customHeight="1">
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+    </row>
+    <row r="149" spans="4:5" ht="18" customHeight="1">
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+    </row>
+    <row r="150" spans="4:5" ht="18" customHeight="1">
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+    </row>
+    <row r="151" spans="4:5" ht="18" customHeight="1">
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+    </row>
+    <row r="152" spans="4:5" ht="18" customHeight="1">
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+    </row>
+    <row r="153" spans="4:5" ht="18" customHeight="1">
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+    </row>
+    <row r="154" spans="4:5" ht="18" customHeight="1">
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+    </row>
+    <row r="155" spans="4:5" ht="18" customHeight="1">
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+    </row>
+    <row r="156" spans="4:5" ht="18" customHeight="1">
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+    </row>
+    <row r="157" spans="4:5" ht="18" customHeight="1">
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+    </row>
+    <row r="158" spans="4:5" ht="18" customHeight="1">
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+    </row>
+    <row r="159" spans="4:5" ht="18" customHeight="1">
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G74"/>
-  <mergeCells count="79">
+  <mergeCells count="134">
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
@@ -18825,69 +19738,6 @@
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
add hdu6171,6364,6370,6373 and agc006d
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="937">
   <si>
     <t>OJ</t>
   </si>
@@ -11036,6 +11036,166 @@
   </si>
   <si>
     <t>Finished</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>oval-and-rectangle</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ringland</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Werewolf</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pinball</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>积分</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>思维</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Admiral</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGC</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>066D</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median Pyramid Hard</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二分</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>双向搜索</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>剪枝</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>哈希</t>
+    </r>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -11126,7 +11286,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -11147,6 +11307,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -17445,8 +17611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
@@ -17899,10 +18065,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="12"/>
+      <c r="D26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="14"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -17920,10 +18086,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="12"/>
+      <c r="D27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -17941,10 +18107,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="12"/>
+      <c r="D28" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="14"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -17962,10 +18128,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="12"/>
+      <c r="D29" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="14"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -17983,10 +18149,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="12"/>
+      <c r="D30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="14"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -18001,10 +18167,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="12"/>
+      <c r="D31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="14"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -18019,10 +18185,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="12"/>
+      <c r="D32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="14"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -18037,10 +18203,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="12"/>
+      <c r="D33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="14"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -18058,10 +18224,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="14">
         <v>97</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -18076,10 +18242,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="12"/>
+      <c r="D35" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="14"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -18094,10 +18260,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="12"/>
+      <c r="D36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="14"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -18112,10 +18278,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="12"/>
+      <c r="D37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="14"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -18130,10 +18296,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="12"/>
+      <c r="D38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="14"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -18151,10 +18317,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="12"/>
+      <c r="D39" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="14"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -18172,10 +18338,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="12"/>
+      <c r="D40" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="14"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -18190,10 +18356,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="12"/>
+      <c r="D41" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="14"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -18211,10 +18377,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="12"/>
+      <c r="D42" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="14"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -18229,10 +18395,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="12"/>
+      <c r="D43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="14"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -18250,10 +18416,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="12"/>
+      <c r="D44" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="14"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -18268,10 +18434,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="12"/>
+      <c r="D45" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="14"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -18286,10 +18452,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="12"/>
+      <c r="D46" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="14"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -18304,10 +18470,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="12"/>
+      <c r="D47" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="14"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -18325,10 +18491,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="12"/>
+      <c r="D48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="14"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -18343,10 +18509,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="12"/>
+      <c r="D49" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="14"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -18364,10 +18530,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="12"/>
+      <c r="D50" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="14"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -18385,10 +18551,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="12"/>
+      <c r="D51" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="14"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -18403,10 +18569,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="12"/>
+      <c r="D52" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="14"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -18421,10 +18587,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="12"/>
+      <c r="D53" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="14"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -18439,10 +18605,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="12"/>
+      <c r="D54" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="14"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -18457,10 +18623,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="12"/>
+      <c r="D55" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="14"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -18475,10 +18641,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="12"/>
+      <c r="D56" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="14"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -18493,10 +18659,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="12"/>
+      <c r="D57" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="14"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -18511,10 +18677,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="12"/>
+      <c r="D58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="14"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -18529,10 +18695,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="12"/>
+      <c r="D59" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="14"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -18550,10 +18716,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="12"/>
+      <c r="D60" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="14"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -18568,10 +18734,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="12"/>
+      <c r="D61" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="14"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -18589,10 +18755,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="12"/>
+      <c r="D62" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="14"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -18607,10 +18773,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="12"/>
+      <c r="D63" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="14"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -18625,10 +18791,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="12"/>
+      <c r="D64" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="14"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -18643,10 +18809,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="12"/>
+      <c r="D65" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="14"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -18661,10 +18827,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="12"/>
+      <c r="D66" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="14"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -18679,10 +18845,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="12"/>
+      <c r="D67" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="14"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -18697,10 +18863,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="12"/>
+      <c r="D68" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="14"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -18715,10 +18881,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="12"/>
+      <c r="D69" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="14"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -18733,10 +18899,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="12"/>
+      <c r="D70" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="14"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -18751,10 +18917,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="12"/>
+      <c r="D71" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="14"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -18769,10 +18935,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="12"/>
+      <c r="D72" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="14"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -18787,10 +18953,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="12"/>
+      <c r="D73" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="14"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -18805,10 +18971,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="12"/>
+      <c r="D74" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="14"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -18823,10 +18989,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="12"/>
+      <c r="D75" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="14"/>
       <c r="F75" s="4" t="s">
         <v>821</v>
       </c>
@@ -18841,10 +19007,10 @@
       <c r="C76" s="7" t="s">
         <v>832</v>
       </c>
-      <c r="D76" s="12" t="s">
+      <c r="D76" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E76" s="12"/>
+      <c r="E76" s="14"/>
       <c r="F76" s="7" t="s">
         <v>833</v>
       </c>
@@ -18859,10 +19025,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="14" t="s">
         <v>824</v>
       </c>
-      <c r="E77" s="12"/>
+      <c r="E77" s="14"/>
       <c r="F77" s="1" t="s">
         <v>825</v>
       </c>
@@ -18877,10 +19043,10 @@
       <c r="C78" s="7" t="s">
         <v>827</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E78" s="12"/>
+      <c r="E78" s="14"/>
       <c r="F78" s="7" t="s">
         <v>829</v>
       </c>
@@ -18895,10 +19061,10 @@
       <c r="C79" s="7" t="s">
         <v>834</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E79" s="12"/>
+      <c r="E79" s="14"/>
       <c r="F79" s="7" t="s">
         <v>835</v>
       </c>
@@ -18913,10 +19079,10 @@
       <c r="C80" s="7" t="s">
         <v>836</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E80" s="12"/>
+      <c r="E80" s="14"/>
       <c r="F80" s="3" t="s">
         <v>837</v>
       </c>
@@ -18931,10 +19097,10 @@
       <c r="C81" s="7" t="s">
         <v>838</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E81" s="12"/>
+      <c r="E81" s="14"/>
       <c r="F81" s="3" t="s">
         <v>839</v>
       </c>
@@ -18949,10 +19115,10 @@
       <c r="C82" s="7" t="s">
         <v>840</v>
       </c>
-      <c r="D82" s="12" t="s">
+      <c r="D82" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E82" s="12"/>
+      <c r="E82" s="14"/>
       <c r="F82" s="3" t="s">
         <v>841</v>
       </c>
@@ -18967,10 +19133,10 @@
       <c r="C83" s="7" t="s">
         <v>842</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D83" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E83" s="12"/>
+      <c r="E83" s="14"/>
       <c r="F83" s="7" t="s">
         <v>843</v>
       </c>
@@ -18985,10 +19151,10 @@
       <c r="C84" s="7" t="s">
         <v>844</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E84" s="12"/>
+      <c r="E84" s="14"/>
       <c r="F84" s="3" t="s">
         <v>845</v>
       </c>
@@ -19003,10 +19169,10 @@
       <c r="C85" s="7" t="s">
         <v>846</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E85" s="12"/>
+      <c r="E85" s="14"/>
       <c r="F85" s="7" t="s">
         <v>847</v>
       </c>
@@ -19021,10 +19187,10 @@
       <c r="C86" s="7" t="s">
         <v>848</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E86" s="12"/>
+      <c r="E86" s="14"/>
       <c r="F86" s="7" t="s">
         <v>849</v>
       </c>
@@ -19039,10 +19205,10 @@
       <c r="C87" s="7" t="s">
         <v>850</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D87" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E87" s="12"/>
+      <c r="E87" s="14"/>
       <c r="F87" s="3" t="s">
         <v>851</v>
       </c>
@@ -19057,10 +19223,10 @@
       <c r="C88" s="7" t="s">
         <v>852</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E88" s="12"/>
+      <c r="E88" s="14"/>
       <c r="F88" s="3" t="s">
         <v>853</v>
       </c>
@@ -19075,10 +19241,10 @@
       <c r="C89" s="7" t="s">
         <v>854</v>
       </c>
-      <c r="D89" s="12" t="s">
+      <c r="D89" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E89" s="12"/>
+      <c r="E89" s="14"/>
       <c r="F89" s="7" t="s">
         <v>855</v>
       </c>
@@ -19093,10 +19259,10 @@
       <c r="C90" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D90" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E90" s="12"/>
+      <c r="E90" s="14"/>
       <c r="F90" s="7" t="s">
         <v>857</v>
       </c>
@@ -19111,10 +19277,10 @@
       <c r="C91" s="7" t="s">
         <v>863</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D91" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E91" s="12"/>
+      <c r="E91" s="14"/>
       <c r="F91" s="3" t="s">
         <v>845</v>
       </c>
@@ -19129,10 +19295,10 @@
       <c r="C92" s="7" t="s">
         <v>864</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D92" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E92" s="12"/>
+      <c r="E92" s="14"/>
       <c r="F92" s="3" t="s">
         <v>845</v>
       </c>
@@ -19147,10 +19313,10 @@
       <c r="C93" s="7" t="s">
         <v>869</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E93" s="12"/>
+      <c r="E93" s="14"/>
       <c r="F93" s="3" t="s">
         <v>839</v>
       </c>
@@ -19165,10 +19331,10 @@
       <c r="C94" s="7" t="s">
         <v>867</v>
       </c>
-      <c r="D94" s="12" t="s">
+      <c r="D94" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E94" s="12"/>
+      <c r="E94" s="14"/>
       <c r="F94" s="7" t="s">
         <v>868</v>
       </c>
@@ -19183,10 +19349,10 @@
       <c r="C95" s="7" t="s">
         <v>865</v>
       </c>
-      <c r="D95" s="12" t="s">
+      <c r="D95" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E95" s="12"/>
+      <c r="E95" s="14"/>
       <c r="F95" s="7" t="s">
         <v>866</v>
       </c>
@@ -19201,10 +19367,10 @@
       <c r="C96" s="3" t="s">
         <v>872</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E96" s="12"/>
+      <c r="E96" s="14"/>
       <c r="F96" s="3" t="s">
         <v>871</v>
       </c>
@@ -19219,10 +19385,10 @@
       <c r="C97" s="3" t="s">
         <v>873</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D97" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E97" s="12"/>
+      <c r="E97" s="14"/>
       <c r="F97" s="8" t="s">
         <v>874</v>
       </c>
@@ -19237,10 +19403,10 @@
       <c r="C98" s="3" t="s">
         <v>875</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="D98" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E98" s="12"/>
+      <c r="E98" s="14"/>
       <c r="F98" s="3" t="s">
         <v>876</v>
       </c>
@@ -19255,10 +19421,10 @@
       <c r="C99" s="3" t="s">
         <v>877</v>
       </c>
-      <c r="D99" s="12" t="s">
+      <c r="D99" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E99" s="12"/>
+      <c r="E99" s="14"/>
       <c r="F99" s="8" t="s">
         <v>878</v>
       </c>
@@ -19273,10 +19439,10 @@
       <c r="C100" s="3" t="s">
         <v>879</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E100" s="12"/>
+      <c r="E100" s="14"/>
       <c r="F100" s="8" t="s">
         <v>880</v>
       </c>
@@ -19291,10 +19457,10 @@
       <c r="C101" s="8" t="s">
         <v>888</v>
       </c>
-      <c r="D101" s="12" t="s">
+      <c r="D101" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E101" s="12"/>
+      <c r="E101" s="14"/>
       <c r="F101" s="3" t="s">
         <v>871</v>
       </c>
@@ -19312,10 +19478,10 @@
       <c r="C102" s="8" t="s">
         <v>889</v>
       </c>
-      <c r="D102" s="12" t="s">
+      <c r="D102" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E102" s="12"/>
+      <c r="E102" s="14"/>
       <c r="F102" s="3" t="s">
         <v>894</v>
       </c>
@@ -19333,10 +19499,10 @@
       <c r="C103" s="8" t="s">
         <v>890</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D103" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E103" s="12"/>
+      <c r="E103" s="14"/>
       <c r="F103" s="3" t="s">
         <v>895</v>
       </c>
@@ -19351,10 +19517,10 @@
       <c r="C104" s="8" t="s">
         <v>891</v>
       </c>
-      <c r="D104" s="12" t="s">
+      <c r="D104" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E104" s="12"/>
+      <c r="E104" s="14"/>
       <c r="F104" s="8" t="s">
         <v>896</v>
       </c>
@@ -19369,10 +19535,10 @@
       <c r="C105" s="8" t="s">
         <v>892</v>
       </c>
-      <c r="D105" s="12" t="s">
+      <c r="D105" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E105" s="12"/>
+      <c r="E105" s="14"/>
       <c r="F105" s="8" t="s">
         <v>897</v>
       </c>
@@ -19387,10 +19553,10 @@
       <c r="C106" s="8" t="s">
         <v>893</v>
       </c>
-      <c r="D106" s="12" t="s">
+      <c r="D106" s="14" t="s">
         <v>870</v>
       </c>
-      <c r="E106" s="12"/>
+      <c r="E106" s="14"/>
       <c r="F106" s="3" t="s">
         <v>895</v>
       </c>
@@ -19405,10 +19571,10 @@
       <c r="C107" s="9" t="s">
         <v>900</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="14" t="s">
         <v>901</v>
       </c>
-      <c r="E107" s="12"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="3" t="s">
         <v>905</v>
       </c>
@@ -19423,10 +19589,10 @@
       <c r="C108" s="9" t="s">
         <v>902</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="14" t="s">
         <v>901</v>
       </c>
-      <c r="E108" s="12"/>
+      <c r="E108" s="14"/>
       <c r="F108" s="9" t="s">
         <v>906</v>
       </c>
@@ -19441,10 +19607,10 @@
       <c r="C109" s="9" t="s">
         <v>903</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D109" s="14" t="s">
         <v>901</v>
       </c>
-      <c r="E109" s="12"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="9" t="s">
         <v>907</v>
       </c>
@@ -19459,10 +19625,10 @@
       <c r="C110" s="9" t="s">
         <v>904</v>
       </c>
-      <c r="D110" s="12" t="s">
+      <c r="D110" s="14" t="s">
         <v>901</v>
       </c>
-      <c r="E110" s="12"/>
+      <c r="E110" s="14"/>
       <c r="F110" s="9" t="s">
         <v>908</v>
       </c>
@@ -19477,10 +19643,10 @@
       <c r="C111" s="10" t="s">
         <v>912</v>
       </c>
-      <c r="D111" s="12" t="s">
+      <c r="D111" s="14" t="s">
         <v>913</v>
       </c>
-      <c r="E111" s="12"/>
+      <c r="E111" s="14"/>
       <c r="F111" s="3" t="s">
         <v>914</v>
       </c>
@@ -19495,10 +19661,10 @@
       <c r="C112" s="11" t="s">
         <v>916</v>
       </c>
-      <c r="D112" s="12" t="s">
+      <c r="D112" s="14" t="s">
         <v>917</v>
       </c>
-      <c r="E112" s="12"/>
+      <c r="E112" s="14"/>
       <c r="F112" s="11" t="s">
         <v>918</v>
       </c>
@@ -19506,193 +19672,277 @@
         <v>919</v>
       </c>
     </row>
-    <row r="113" spans="4:5" ht="18" customHeight="1">
-      <c r="D113" s="12"/>
-      <c r="E113" s="12"/>
-    </row>
-    <row r="114" spans="4:5" ht="18" customHeight="1">
-      <c r="D114" s="12"/>
-      <c r="E114" s="12"/>
-    </row>
-    <row r="115" spans="4:5" ht="18" customHeight="1">
-      <c r="D115" s="12"/>
-      <c r="E115" s="12"/>
-    </row>
-    <row r="116" spans="4:5" ht="18" customHeight="1">
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-    </row>
-    <row r="117" spans="4:5" ht="18" customHeight="1">
-      <c r="D117" s="12"/>
-      <c r="E117" s="12"/>
-    </row>
-    <row r="118" spans="4:5" ht="18" customHeight="1">
-      <c r="D118" s="12"/>
-      <c r="E118" s="12"/>
-    </row>
-    <row r="119" spans="4:5" ht="18" customHeight="1">
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-    </row>
-    <row r="120" spans="4:5" ht="18" customHeight="1">
-      <c r="D120" s="12"/>
-      <c r="E120" s="12"/>
-    </row>
-    <row r="121" spans="4:5" ht="18" customHeight="1">
-      <c r="D121" s="12"/>
-      <c r="E121" s="12"/>
-    </row>
-    <row r="122" spans="4:5" ht="18" customHeight="1">
-      <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
-    </row>
-    <row r="123" spans="4:5" ht="18" customHeight="1">
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-    </row>
-    <row r="124" spans="4:5" ht="18" customHeight="1">
-      <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
-    </row>
-    <row r="125" spans="4:5" ht="18" customHeight="1">
-      <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
-    </row>
-    <row r="126" spans="4:5" ht="18" customHeight="1">
-      <c r="D126" s="12"/>
-      <c r="E126" s="12"/>
-    </row>
-    <row r="127" spans="4:5" ht="18" customHeight="1">
-      <c r="D127" s="12"/>
-      <c r="E127" s="12"/>
-    </row>
-    <row r="128" spans="4:5" ht="18" customHeight="1">
-      <c r="D128" s="12"/>
-      <c r="E128" s="12"/>
+    <row r="113" spans="1:6" ht="18" customHeight="1">
+      <c r="A113" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="B113" s="1">
+        <v>6362</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>921</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>922</v>
+      </c>
+      <c r="E113" s="14"/>
+      <c r="F113" s="12" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="18" customHeight="1">
+      <c r="A114" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="B114" s="1">
+        <v>6364</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>923</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>922</v>
+      </c>
+      <c r="E114" s="14"/>
+      <c r="F114" s="3" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="18" customHeight="1">
+      <c r="A115" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="B115" s="1">
+        <v>6370</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>924</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>922</v>
+      </c>
+      <c r="E115" s="14"/>
+      <c r="F115" s="3" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="18" customHeight="1">
+      <c r="A116" s="12" t="s">
+        <v>920</v>
+      </c>
+      <c r="B116" s="1">
+        <v>6373</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>925</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>922</v>
+      </c>
+      <c r="E116" s="14"/>
+      <c r="F116" s="3" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="18" customHeight="1">
+      <c r="A117" s="13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>933</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>934</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>931</v>
+      </c>
+      <c r="E117" s="14"/>
+      <c r="F117" s="13" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="18" customHeight="1">
+      <c r="A118" s="13" t="s">
+        <v>929</v>
+      </c>
+      <c r="B118" s="1">
+        <v>6171</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>930</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>931</v>
+      </c>
+      <c r="E118" s="14"/>
+      <c r="F118" s="13" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="18" customHeight="1">
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+    </row>
+    <row r="120" spans="1:6" ht="18" customHeight="1">
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+    </row>
+    <row r="121" spans="1:6" ht="18" customHeight="1">
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+    </row>
+    <row r="122" spans="1:6" ht="18" customHeight="1">
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+    </row>
+    <row r="123" spans="1:6" ht="18" customHeight="1">
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+    </row>
+    <row r="124" spans="1:6" ht="18" customHeight="1">
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+    </row>
+    <row r="125" spans="1:6" ht="18" customHeight="1">
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+    </row>
+    <row r="126" spans="1:6" ht="18" customHeight="1">
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+    </row>
+    <row r="127" spans="1:6" ht="18" customHeight="1">
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+    </row>
+    <row r="128" spans="1:6" ht="18" customHeight="1">
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
     </row>
     <row r="129" spans="4:5" ht="18" customHeight="1">
-      <c r="D129" s="12"/>
-      <c r="E129" s="12"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
     </row>
     <row r="130" spans="4:5" ht="18" customHeight="1">
-      <c r="D130" s="12"/>
-      <c r="E130" s="12"/>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
     </row>
     <row r="131" spans="4:5" ht="18" customHeight="1">
-      <c r="D131" s="12"/>
-      <c r="E131" s="12"/>
+      <c r="D131" s="14"/>
+      <c r="E131" s="14"/>
     </row>
     <row r="132" spans="4:5" ht="18" customHeight="1">
-      <c r="D132" s="12"/>
-      <c r="E132" s="12"/>
+      <c r="D132" s="14"/>
+      <c r="E132" s="14"/>
     </row>
     <row r="133" spans="4:5" ht="18" customHeight="1">
-      <c r="D133" s="12"/>
-      <c r="E133" s="12"/>
+      <c r="D133" s="14"/>
+      <c r="E133" s="14"/>
     </row>
     <row r="134" spans="4:5" ht="18" customHeight="1">
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
+      <c r="D134" s="14"/>
+      <c r="E134" s="14"/>
     </row>
     <row r="135" spans="4:5" ht="18" customHeight="1">
-      <c r="D135" s="12"/>
-      <c r="E135" s="12"/>
+      <c r="D135" s="14"/>
+      <c r="E135" s="14"/>
     </row>
     <row r="136" spans="4:5" ht="18" customHeight="1">
-      <c r="D136" s="12"/>
-      <c r="E136" s="12"/>
+      <c r="D136" s="14"/>
+      <c r="E136" s="14"/>
     </row>
     <row r="137" spans="4:5" ht="18" customHeight="1">
-      <c r="D137" s="12"/>
-      <c r="E137" s="12"/>
+      <c r="D137" s="14"/>
+      <c r="E137" s="14"/>
     </row>
     <row r="138" spans="4:5" ht="18" customHeight="1">
-      <c r="D138" s="12"/>
-      <c r="E138" s="12"/>
+      <c r="D138" s="14"/>
+      <c r="E138" s="14"/>
     </row>
     <row r="139" spans="4:5" ht="18" customHeight="1">
-      <c r="D139" s="12"/>
-      <c r="E139" s="12"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
     </row>
     <row r="140" spans="4:5" ht="18" customHeight="1">
-      <c r="D140" s="12"/>
-      <c r="E140" s="12"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
     </row>
     <row r="141" spans="4:5" ht="18" customHeight="1">
-      <c r="D141" s="12"/>
-      <c r="E141" s="12"/>
+      <c r="D141" s="14"/>
+      <c r="E141" s="14"/>
     </row>
     <row r="142" spans="4:5" ht="18" customHeight="1">
-      <c r="D142" s="12"/>
-      <c r="E142" s="12"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="14"/>
     </row>
     <row r="143" spans="4:5" ht="18" customHeight="1">
-      <c r="D143" s="12"/>
-      <c r="E143" s="12"/>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
     </row>
     <row r="144" spans="4:5" ht="18" customHeight="1">
-      <c r="D144" s="12"/>
-      <c r="E144" s="12"/>
+      <c r="D144" s="14"/>
+      <c r="E144" s="14"/>
     </row>
     <row r="145" spans="4:5" ht="18" customHeight="1">
-      <c r="D145" s="12"/>
-      <c r="E145" s="12"/>
+      <c r="D145" s="14"/>
+      <c r="E145" s="14"/>
     </row>
     <row r="146" spans="4:5" ht="18" customHeight="1">
-      <c r="D146" s="12"/>
-      <c r="E146" s="12"/>
+      <c r="D146" s="14"/>
+      <c r="E146" s="14"/>
     </row>
     <row r="147" spans="4:5" ht="18" customHeight="1">
-      <c r="D147" s="12"/>
-      <c r="E147" s="12"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
     </row>
     <row r="148" spans="4:5" ht="18" customHeight="1">
-      <c r="D148" s="12"/>
-      <c r="E148" s="12"/>
+      <c r="D148" s="14"/>
+      <c r="E148" s="14"/>
     </row>
     <row r="149" spans="4:5" ht="18" customHeight="1">
-      <c r="D149" s="12"/>
-      <c r="E149" s="12"/>
+      <c r="D149" s="14"/>
+      <c r="E149" s="14"/>
     </row>
     <row r="150" spans="4:5" ht="18" customHeight="1">
-      <c r="D150" s="12"/>
-      <c r="E150" s="12"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
     </row>
     <row r="151" spans="4:5" ht="18" customHeight="1">
-      <c r="D151" s="12"/>
-      <c r="E151" s="12"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="14"/>
     </row>
     <row r="152" spans="4:5" ht="18" customHeight="1">
-      <c r="D152" s="12"/>
-      <c r="E152" s="12"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="14"/>
     </row>
     <row r="153" spans="4:5" ht="18" customHeight="1">
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
     </row>
     <row r="154" spans="4:5" ht="18" customHeight="1">
-      <c r="D154" s="12"/>
-      <c r="E154" s="12"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
     </row>
     <row r="155" spans="4:5" ht="18" customHeight="1">
-      <c r="D155" s="12"/>
-      <c r="E155" s="12"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
     </row>
     <row r="156" spans="4:5" ht="18" customHeight="1">
-      <c r="D156" s="12"/>
-      <c r="E156" s="12"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14"/>
     </row>
     <row r="157" spans="4:5" ht="18" customHeight="1">
-      <c r="D157" s="12"/>
-      <c r="E157" s="12"/>
+      <c r="D157" s="14"/>
+      <c r="E157" s="14"/>
     </row>
     <row r="158" spans="4:5" ht="18" customHeight="1">
-      <c r="D158" s="12"/>
-      <c r="E158" s="12"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
     </row>
     <row r="159" spans="4:5" ht="18" customHeight="1">
-      <c r="D159" s="12"/>
-      <c r="E159" s="12"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G74"/>

</xml_diff>

<commit_message>
add hdu6409,6410,6411,6412,64156,6416,6418,6425 and cf983d(std)
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="990">
   <si>
     <t>OJ</t>
   </si>
@@ -11365,10 +11365,160 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>983D</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>扫描线</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>堆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>扫描线</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>堆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t>Arkady and Rectangles</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
+    <t>Arkady and Rectangles(std)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swordsman</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t>Accepted</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -11380,40 +11530,6 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>扫描线</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Apple Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>线段树</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Apple Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
       <t>堆</t>
     </r>
     <r>
@@ -11433,6 +11549,367 @@
       </rPr>
       <t>思维</t>
     </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character Encoding</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>容斥</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parentheses Matrix</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>构造</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic Square</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Card Game</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>图论</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taotao Picks Apples</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二分</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pop the Balloon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pop the Balloon(std)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>状压</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>三进制状态</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>状压</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二进制状态</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有兄弟的舞会</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列期望</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>带劲的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>公共子序列</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>树型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>dp</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>DSU;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rikka with Nash Equilibrium</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rikka with Stone-Paper-Scissors</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>博弈论</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rikka with Badminton</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类讨论</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rikka with Seam</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -11535,7 +12012,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -11556,6 +12033,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -11901,7 +12381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -12593,7 +13073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
+    <sheetView topLeftCell="A250" workbookViewId="0">
       <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
@@ -17841,8 +18321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142:E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
@@ -18295,10 +18775,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="7"/>
+      <c r="D26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="8"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -18316,10 +18796,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7"/>
+      <c r="D27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -18337,10 +18817,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="D28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="8"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -18358,10 +18838,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="7"/>
+      <c r="D29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="8"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -18379,10 +18859,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="7"/>
+      <c r="D30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="8"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -18397,10 +18877,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="7"/>
+      <c r="D31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -18415,10 +18895,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="7"/>
+      <c r="D32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -18433,10 +18913,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="7"/>
+      <c r="D33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -18454,10 +18934,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="8">
         <v>97</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -18472,10 +18952,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="7"/>
+      <c r="D35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="8"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -18490,10 +18970,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="7"/>
+      <c r="D36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="8"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -18508,10 +18988,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="7"/>
+      <c r="D37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="8"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -18526,10 +19006,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="7"/>
+      <c r="D38" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="8"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -18547,10 +19027,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="7"/>
+      <c r="D39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="8"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -18568,10 +19048,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="7"/>
+      <c r="D40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="8"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -18586,10 +19066,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="7"/>
+      <c r="D41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="8"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -18607,10 +19087,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="7"/>
+      <c r="D42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="8"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -18625,10 +19105,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="7"/>
+      <c r="D43" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="8"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -18646,10 +19126,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="7"/>
+      <c r="D44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="8"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -18664,10 +19144,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="7"/>
+      <c r="D45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="8"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -18682,10 +19162,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="7"/>
+      <c r="D46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="8"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -18700,10 +19180,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="7"/>
+      <c r="D47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="8"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -18721,10 +19201,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="7"/>
+      <c r="D48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="8"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -18739,10 +19219,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="7"/>
+      <c r="D49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="8"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -18760,10 +19240,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="7"/>
+      <c r="D50" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="8"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -18781,10 +19261,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="7"/>
+      <c r="D51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="8"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -18799,10 +19279,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="7"/>
+      <c r="D52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="8"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -18817,10 +19297,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="7"/>
+      <c r="D53" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="8"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -18835,10 +19315,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="7"/>
+      <c r="D54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="8"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -18853,10 +19333,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="7"/>
+      <c r="D55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="8"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -18871,10 +19351,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="7"/>
+      <c r="D56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="8"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -18889,10 +19369,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="7"/>
+      <c r="D57" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="8"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -18907,10 +19387,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="7"/>
+      <c r="D58" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="8"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -18925,10 +19405,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="7"/>
+      <c r="D59" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="8"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -18946,10 +19426,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="7"/>
+      <c r="D60" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="8"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -18964,10 +19444,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="7"/>
+      <c r="D61" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="8"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -18985,10 +19465,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="7"/>
+      <c r="D62" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="8"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -19003,10 +19483,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="7"/>
+      <c r="D63" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="8"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -19021,10 +19501,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="7"/>
+      <c r="D64" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="8"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -19039,10 +19519,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="7"/>
+      <c r="D65" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="8"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -19057,10 +19537,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="7"/>
+      <c r="D66" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="8"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -19075,10 +19555,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="7"/>
+      <c r="D67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="8"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -19093,10 +19573,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="7"/>
+      <c r="D68" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="8"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -19111,10 +19591,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="7"/>
+      <c r="D69" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="8"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -19129,10 +19609,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="7"/>
+      <c r="D70" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="8"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -19147,10 +19627,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="7"/>
+      <c r="D71" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="8"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -19165,10 +19645,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="7"/>
+      <c r="D72" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="8"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -19183,10 +19663,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="7"/>
+      <c r="D73" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="8"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -19201,10 +19681,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="7"/>
+      <c r="D74" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="8"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -19219,10 +19699,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="7"/>
+      <c r="D75" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="8"/>
       <c r="F75" s="3" t="s">
         <v>821</v>
       </c>
@@ -19237,10 +19717,10 @@
       <c r="C76" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="7"/>
+      <c r="D76" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="8"/>
       <c r="F76" s="1" t="s">
         <v>822</v>
       </c>
@@ -19255,10 +19735,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="7"/>
+      <c r="D77" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="8"/>
       <c r="F77" s="1" t="s">
         <v>824</v>
       </c>
@@ -19273,10 +19753,10 @@
       <c r="C78" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="7"/>
+      <c r="D78" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="8"/>
       <c r="F78" s="1" t="s">
         <v>826</v>
       </c>
@@ -19291,10 +19771,10 @@
       <c r="C79" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="7"/>
+      <c r="D79" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="8"/>
       <c r="F79" s="1" t="s">
         <v>818</v>
       </c>
@@ -19309,10 +19789,10 @@
       <c r="C80" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="7"/>
+      <c r="D80" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="8"/>
       <c r="F80" s="3" t="s">
         <v>566</v>
       </c>
@@ -19327,10 +19807,10 @@
       <c r="C81" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="7"/>
+      <c r="D81" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="8"/>
       <c r="F81" s="3" t="s">
         <v>14</v>
       </c>
@@ -19345,10 +19825,10 @@
       <c r="C82" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="7"/>
+      <c r="D82" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="8"/>
       <c r="F82" s="3" t="s">
         <v>831</v>
       </c>
@@ -19363,10 +19843,10 @@
       <c r="C83" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="7"/>
+      <c r="D83" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="8"/>
       <c r="F83" s="1" t="s">
         <v>833</v>
       </c>
@@ -19381,10 +19861,10 @@
       <c r="C84" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="7"/>
+      <c r="D84" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="8"/>
       <c r="F84" s="3" t="s">
         <v>568</v>
       </c>
@@ -19399,10 +19879,10 @@
       <c r="C85" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="D85" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="7"/>
+      <c r="D85" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="8"/>
       <c r="F85" s="1" t="s">
         <v>836</v>
       </c>
@@ -19417,10 +19897,10 @@
       <c r="C86" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="7"/>
+      <c r="D86" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="8"/>
       <c r="F86" s="1" t="s">
         <v>806</v>
       </c>
@@ -19435,10 +19915,10 @@
       <c r="C87" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="7"/>
+      <c r="D87" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="8"/>
       <c r="F87" s="3" t="s">
         <v>839</v>
       </c>
@@ -19453,10 +19933,10 @@
       <c r="C88" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="7"/>
+      <c r="D88" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="8"/>
       <c r="F88" s="3" t="s">
         <v>841</v>
       </c>
@@ -19471,10 +19951,10 @@
       <c r="C89" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="D89" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="7"/>
+      <c r="D89" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="8"/>
       <c r="F89" s="1" t="s">
         <v>843</v>
       </c>
@@ -19489,10 +19969,10 @@
       <c r="C90" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="7"/>
+      <c r="D90" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="8"/>
       <c r="F90" s="1" t="s">
         <v>845</v>
       </c>
@@ -19507,10 +19987,10 @@
       <c r="C91" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="7"/>
+      <c r="D91" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="8"/>
       <c r="F91" s="3" t="s">
         <v>568</v>
       </c>
@@ -19525,10 +20005,10 @@
       <c r="C92" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="7"/>
+      <c r="D92" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="8"/>
       <c r="F92" s="3" t="s">
         <v>568</v>
       </c>
@@ -19543,10 +20023,10 @@
       <c r="C93" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="7"/>
+      <c r="D93" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="8"/>
       <c r="F93" s="3" t="s">
         <v>14</v>
       </c>
@@ -19561,10 +20041,10 @@
       <c r="C94" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D94" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="7"/>
+      <c r="D94" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="8"/>
       <c r="F94" s="1" t="s">
         <v>854</v>
       </c>
@@ -19579,10 +20059,10 @@
       <c r="C95" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="D95" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="7"/>
+      <c r="D95" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="8"/>
       <c r="F95" s="1" t="s">
         <v>162</v>
       </c>
@@ -19597,10 +20077,10 @@
       <c r="C96" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="D96" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="7"/>
+      <c r="D96" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="8"/>
       <c r="F96" s="3" t="s">
         <v>568</v>
       </c>
@@ -19615,10 +20095,10 @@
       <c r="C97" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="D97" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="7"/>
+      <c r="D97" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="8"/>
       <c r="F97" s="1" t="s">
         <v>859</v>
       </c>
@@ -19633,10 +20113,10 @@
       <c r="C98" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="7"/>
+      <c r="D98" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="8"/>
       <c r="F98" s="3" t="s">
         <v>861</v>
       </c>
@@ -19651,10 +20131,10 @@
       <c r="C99" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="D99" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="7"/>
+      <c r="D99" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="8"/>
       <c r="F99" s="1" t="s">
         <v>863</v>
       </c>
@@ -19669,10 +20149,10 @@
       <c r="C100" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="7"/>
+      <c r="D100" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="8"/>
       <c r="F100" s="1" t="s">
         <v>865</v>
       </c>
@@ -19687,10 +20167,10 @@
       <c r="C101" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="D101" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="7"/>
+      <c r="D101" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="8"/>
       <c r="F101" s="3" t="s">
         <v>568</v>
       </c>
@@ -19708,10 +20188,10 @@
       <c r="C102" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="7"/>
+      <c r="D102" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="8"/>
       <c r="F102" s="3" t="s">
         <v>870</v>
       </c>
@@ -19729,10 +20209,10 @@
       <c r="C103" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="7"/>
+      <c r="D103" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="8"/>
       <c r="F103" s="3" t="s">
         <v>14</v>
       </c>
@@ -19747,10 +20227,10 @@
       <c r="C104" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="7"/>
+      <c r="D104" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="8"/>
       <c r="F104" s="1" t="s">
         <v>875</v>
       </c>
@@ -19765,10 +20245,10 @@
       <c r="C105" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="7"/>
+      <c r="D105" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="8"/>
       <c r="F105" s="1" t="s">
         <v>878</v>
       </c>
@@ -19783,10 +20263,10 @@
       <c r="C106" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="7"/>
+      <c r="D106" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="8"/>
       <c r="F106" s="3" t="s">
         <v>14</v>
       </c>
@@ -19801,10 +20281,10 @@
       <c r="C107" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D107" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="7"/>
+      <c r="D107" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="8"/>
       <c r="F107" s="3" t="s">
         <v>882</v>
       </c>
@@ -19819,10 +20299,10 @@
       <c r="C108" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="D108" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="7"/>
+      <c r="D108" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="8"/>
       <c r="F108" s="1" t="s">
         <v>884</v>
       </c>
@@ -19837,10 +20317,10 @@
       <c r="C109" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="D109" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="7"/>
+      <c r="D109" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="8"/>
       <c r="F109" s="1" t="s">
         <v>886</v>
       </c>
@@ -19855,10 +20335,10 @@
       <c r="C110" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D110" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="7"/>
+      <c r="D110" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="8"/>
       <c r="F110" s="1" t="s">
         <v>162</v>
       </c>
@@ -19873,10 +20353,10 @@
       <c r="C111" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="D111" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="7"/>
+      <c r="D111" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="8"/>
       <c r="F111" s="3" t="s">
         <v>171</v>
       </c>
@@ -19891,10 +20371,10 @@
       <c r="C112" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D112" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="7"/>
+      <c r="D112" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="8"/>
       <c r="F112" s="1" t="s">
         <v>891</v>
       </c>
@@ -19912,10 +20392,10 @@
       <c r="C113" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="7"/>
+      <c r="D113" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="8"/>
       <c r="F113" s="1" t="s">
         <v>893</v>
       </c>
@@ -19930,10 +20410,10 @@
       <c r="C114" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="7"/>
+      <c r="D114" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="8"/>
       <c r="F114" s="3" t="s">
         <v>14</v>
       </c>
@@ -19948,10 +20428,10 @@
       <c r="C115" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="D115" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" s="7"/>
+      <c r="D115" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="8"/>
       <c r="F115" s="3" t="s">
         <v>14</v>
       </c>
@@ -19966,10 +20446,10 @@
       <c r="C116" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="D116" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" s="7"/>
+      <c r="D116" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="8"/>
       <c r="F116" s="3" t="s">
         <v>897</v>
       </c>
@@ -19984,10 +20464,10 @@
       <c r="C117" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="D117" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="7"/>
+      <c r="D117" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" s="8"/>
       <c r="F117" s="1" t="s">
         <v>900</v>
       </c>
@@ -20002,10 +20482,10 @@
       <c r="C118" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="D118" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="7"/>
+      <c r="D118" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="8"/>
       <c r="F118" s="1" t="s">
         <v>902</v>
       </c>
@@ -20020,10 +20500,10 @@
       <c r="C119" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="D119" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="7"/>
+      <c r="D119" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="8"/>
       <c r="F119" s="1" t="s">
         <v>905</v>
       </c>
@@ -20038,10 +20518,10 @@
       <c r="C120" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="D120" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E120" s="7"/>
+      <c r="D120" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="8"/>
       <c r="F120" s="2" t="s">
         <v>411</v>
       </c>
@@ -20056,10 +20536,10 @@
       <c r="C121" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="D121" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="7"/>
+      <c r="D121" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="8"/>
       <c r="F121" s="2" t="s">
         <v>234</v>
       </c>
@@ -20074,10 +20554,10 @@
       <c r="C122" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="D122" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="7"/>
+      <c r="D122" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="8"/>
       <c r="F122" s="3" t="s">
         <v>912</v>
       </c>
@@ -20092,10 +20572,10 @@
       <c r="C123" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="D123" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="7"/>
+      <c r="D123" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="8"/>
       <c r="F123" s="3" t="s">
         <v>915</v>
       </c>
@@ -20110,10 +20590,10 @@
       <c r="C124" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="D124" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="7"/>
+      <c r="D124" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="8"/>
       <c r="F124" s="1" t="s">
         <v>918</v>
       </c>
@@ -20128,10 +20608,10 @@
       <c r="C125" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="D125" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="7"/>
+      <c r="D125" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="8"/>
       <c r="F125" s="3" t="s">
         <v>422</v>
       </c>
@@ -20146,10 +20626,10 @@
       <c r="C126" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="D126" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="7"/>
+      <c r="D126" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="8"/>
       <c r="F126" s="3" t="s">
         <v>882</v>
       </c>
@@ -20164,10 +20644,10 @@
       <c r="C127" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D127" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E127" s="7"/>
+      <c r="D127" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E127" s="8"/>
       <c r="F127" s="1" t="s">
         <v>925</v>
       </c>
@@ -20182,10 +20662,10 @@
       <c r="C128" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D128" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E128" s="7"/>
+      <c r="D128" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="8"/>
       <c r="F128" s="3" t="s">
         <v>168</v>
       </c>
@@ -20200,10 +20680,10 @@
       <c r="C129" s="3" t="s">
         <v>926</v>
       </c>
-      <c r="D129" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E129" s="7"/>
+      <c r="D129" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="8"/>
       <c r="F129" s="1" t="s">
         <v>927</v>
       </c>
@@ -20218,10 +20698,10 @@
       <c r="C130" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="D130" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E130" s="7"/>
+      <c r="D130" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" s="8"/>
       <c r="F130" s="3" t="s">
         <v>171</v>
       </c>
@@ -20236,10 +20716,10 @@
       <c r="C131" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="D131" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" s="7"/>
+      <c r="D131" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="8"/>
       <c r="F131" s="3" t="s">
         <v>566</v>
       </c>
@@ -20254,10 +20734,10 @@
       <c r="C132" s="3" t="s">
         <v>930</v>
       </c>
-      <c r="D132" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E132" s="7"/>
+      <c r="D132" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="8"/>
       <c r="F132" s="1" t="s">
         <v>162</v>
       </c>
@@ -20272,10 +20752,10 @@
       <c r="C133" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="D133" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133" s="7"/>
+      <c r="D133" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="8"/>
       <c r="F133" s="1" t="s">
         <v>933</v>
       </c>
@@ -20290,10 +20770,10 @@
       <c r="C134" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="D134" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="7"/>
+      <c r="D134" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="8"/>
       <c r="F134" s="1" t="s">
         <v>936</v>
       </c>
@@ -20311,10 +20791,10 @@
       <c r="C135" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="D135" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="7"/>
+      <c r="D135" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" s="8"/>
       <c r="F135" s="1" t="s">
         <v>938</v>
       </c>
@@ -20329,10 +20809,10 @@
       <c r="C136" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D136" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" s="7"/>
+      <c r="D136" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" s="8"/>
       <c r="F136" s="1" t="s">
         <v>940</v>
       </c>
@@ -20347,10 +20827,10 @@
       <c r="C137" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D137" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E137" s="7"/>
+      <c r="D137" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" s="8"/>
       <c r="F137" s="1" t="s">
         <v>942</v>
       </c>
@@ -20365,10 +20845,10 @@
       <c r="C138" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D138" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="7"/>
+      <c r="D138" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="8"/>
       <c r="F138" s="1" t="s">
         <v>943</v>
       </c>
@@ -20383,10 +20863,10 @@
       <c r="C139" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="D139" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="7"/>
+      <c r="D139" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="8"/>
       <c r="F139" s="1" t="s">
         <v>826</v>
       </c>
@@ -20401,10 +20881,10 @@
       <c r="C140" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="D140" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E140" s="7"/>
+      <c r="D140" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" s="8"/>
       <c r="F140" s="4" t="s">
         <v>947</v>
       </c>
@@ -20416,96 +20896,469 @@
       <c r="B141" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="D141" s="8" t="s">
         <v>950</v>
       </c>
-      <c r="D141" s="7" t="s">
+      <c r="E141" s="8"/>
+      <c r="F141" s="7" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="18" customHeight="1">
+      <c r="A142" s="7" t="s">
         <v>951</v>
       </c>
-      <c r="E141" s="7"/>
-      <c r="F141" s="1" t="s">
+      <c r="B142" s="7" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="18" customHeight="1">
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
+      <c r="C142" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E142" s="8"/>
+      <c r="F142" s="7" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="143" spans="1:7" ht="18" customHeight="1">
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
+      <c r="A143" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B143" s="1">
+        <v>6396</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="D143" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E143" s="8"/>
+      <c r="F143" s="7" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="144" spans="1:7" ht="18" customHeight="1">
-      <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
-    </row>
-    <row r="145" spans="4:5" ht="18" customHeight="1">
-      <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
-    </row>
-    <row r="146" spans="4:5" ht="18" customHeight="1">
-      <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-    </row>
-    <row r="147" spans="4:5" ht="18" customHeight="1">
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-    </row>
-    <row r="148" spans="4:5" ht="18" customHeight="1">
-      <c r="D148" s="7"/>
-      <c r="E148" s="7"/>
-    </row>
-    <row r="149" spans="4:5" ht="18" customHeight="1">
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
-    </row>
-    <row r="150" spans="4:5" ht="18" customHeight="1">
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-    </row>
-    <row r="151" spans="4:5" ht="18" customHeight="1">
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-    </row>
-    <row r="152" spans="4:5" ht="18" customHeight="1">
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
-    </row>
-    <row r="153" spans="4:5" ht="18" customHeight="1">
-      <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
-    </row>
-    <row r="154" spans="4:5" ht="18" customHeight="1">
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-    </row>
-    <row r="155" spans="4:5" ht="18" customHeight="1">
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
-    </row>
-    <row r="156" spans="4:5" ht="18" customHeight="1">
-      <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
-    </row>
-    <row r="157" spans="4:5" ht="18" customHeight="1">
-      <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
-    </row>
-    <row r="158" spans="4:5" ht="18" customHeight="1">
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="4:5" ht="18" customHeight="1">
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-    </row>
-    <row r="160" spans="4:5" ht="18" customHeight="1">
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
+      <c r="A144" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B144" s="1">
+        <v>6397</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E144" s="8"/>
+      <c r="F144" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="G144" s="7" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="18" customHeight="1">
+      <c r="A145" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B145" s="1">
+        <v>6400</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="D145" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E145" s="8"/>
+      <c r="F145" s="3" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="18" customHeight="1">
+      <c r="A146" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B146" s="1">
+        <v>6401</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>966</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E146" s="8"/>
+      <c r="F146" s="3" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="18" customHeight="1">
+      <c r="A147" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B147" s="1">
+        <v>6403</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>968</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E147" s="8"/>
+      <c r="F147" s="7" t="s">
+        <v>969</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="18" customHeight="1">
+      <c r="A148" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B148" s="1">
+        <v>6406</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E148" s="8"/>
+      <c r="F148" s="7" t="s">
+        <v>971</v>
+      </c>
+      <c r="G148" s="7" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="18" customHeight="1">
+      <c r="A149" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B149" s="1">
+        <v>6407</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E149" s="8"/>
+      <c r="F149" s="7" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="18" customHeight="1">
+      <c r="A150" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B150" s="1">
+        <v>6407</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E150" s="8"/>
+      <c r="F150" s="7" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="18" customHeight="1">
+      <c r="A151" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B151" s="1">
+        <v>6409</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="D151" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E151" s="8"/>
+      <c r="F151" s="7" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="18" customHeight="1">
+      <c r="A152" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B152" s="1">
+        <v>6410</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E152" s="8"/>
+      <c r="F152" s="7" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="18" customHeight="1">
+      <c r="A153" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B153" s="1">
+        <v>6411</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E153" s="8"/>
+      <c r="F153" s="7" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="18" customHeight="1">
+      <c r="A154" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B154" s="1">
+        <v>6412</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E154" s="8"/>
+      <c r="F154" s="7" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="18" customHeight="1">
+      <c r="A155" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B155" s="1">
+        <v>6415</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="D155" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E155" s="8"/>
+      <c r="F155" s="7" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="18" customHeight="1">
+      <c r="A156" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B156" s="1">
+        <v>6418</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>985</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E156" s="8"/>
+      <c r="F156" s="7" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="18" customHeight="1">
+      <c r="A157" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B157" s="1">
+        <v>6425</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="D157" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E157" s="8"/>
+      <c r="F157" s="3" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="18" customHeight="1">
+      <c r="A158" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B158" s="1">
+        <v>6416</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>989</v>
+      </c>
+      <c r="D158" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="E158" s="8"/>
+      <c r="F158" s="7" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="18" customHeight="1">
+      <c r="D159" s="8"/>
+      <c r="E159" s="8"/>
+    </row>
+    <row r="160" spans="1:7" ht="18" customHeight="1">
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G139"/>
   <mergeCells count="135">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
     <mergeCell ref="D152:E152"/>
     <mergeCell ref="D153:E153"/>
     <mergeCell ref="D154:E154"/>
@@ -20515,132 +21368,6 @@
     <mergeCell ref="D158:E158"/>
     <mergeCell ref="D159:E159"/>
     <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
add hdu6427 and hdu6430
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -14,14 +14,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$139</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$169</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="1018">
   <si>
     <t>OJ</t>
   </si>
@@ -12090,6 +12090,158 @@
       </rPr>
       <t>欧拉函数</t>
     </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beeds</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Pollard_Rho;Burnside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>引理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;Polya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>定理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>TLE</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树合并</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>TeaTree</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>TeaTree</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>哈希表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>启发式合并</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>思维;堆</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -12192,7 +12344,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -12213,6 +12365,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -18504,8 +18659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G167" sqref="G167"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
@@ -18958,10 +19113,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="9"/>
+      <c r="D26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -18979,10 +19134,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="9"/>
+      <c r="D27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -19000,10 +19155,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="9"/>
+      <c r="D28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="10"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -19021,10 +19176,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="9"/>
+      <c r="D29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="10"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -19042,10 +19197,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="9"/>
+      <c r="D30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -19060,10 +19215,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="9"/>
+      <c r="D31" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="10"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -19078,10 +19233,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="9"/>
+      <c r="D32" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="10"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -19096,10 +19251,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="9"/>
+      <c r="D33" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="10"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -19117,10 +19272,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="10">
         <v>97</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -19135,10 +19290,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="9"/>
+      <c r="D35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -19153,10 +19308,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="9"/>
+      <c r="D36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -19171,10 +19326,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="9"/>
+      <c r="D37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="10"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -19189,10 +19344,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="9"/>
+      <c r="D38" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="10"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -19210,10 +19365,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="9"/>
+      <c r="D39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="10"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -19231,10 +19386,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="9"/>
+      <c r="D40" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="10"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -19249,10 +19404,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="9"/>
+      <c r="D41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="10"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -19270,10 +19425,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="9"/>
+      <c r="D42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="10"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -19288,10 +19443,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="9"/>
+      <c r="D43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="10"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -19309,10 +19464,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="9"/>
+      <c r="D44" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="10"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -19327,10 +19482,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="9"/>
+      <c r="D45" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="10"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -19345,10 +19500,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="9"/>
+      <c r="D46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="10"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -19363,10 +19518,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="9"/>
+      <c r="D47" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="10"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -19384,10 +19539,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="9"/>
+      <c r="D48" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="10"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -19402,10 +19557,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="9"/>
+      <c r="D49" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="10"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -19423,10 +19578,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="9"/>
+      <c r="D50" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -19444,10 +19599,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="9"/>
+      <c r="D51" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="10"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -19462,10 +19617,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="9"/>
+      <c r="D52" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="10"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -19480,10 +19635,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="9"/>
+      <c r="D53" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="10"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -19498,10 +19653,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="9"/>
+      <c r="D54" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="10"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -19516,10 +19671,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="9"/>
+      <c r="D55" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="10"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -19534,10 +19689,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="9"/>
+      <c r="D56" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="10"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -19552,10 +19707,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="9"/>
+      <c r="D57" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="10"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -19570,10 +19725,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="9"/>
+      <c r="D58" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="10"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -19588,10 +19743,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="9"/>
+      <c r="D59" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="10"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -19609,10 +19764,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="9"/>
+      <c r="D60" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="10"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -19627,10 +19782,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="9"/>
+      <c r="D61" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="10"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -19648,10 +19803,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="9"/>
+      <c r="D62" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="10"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -19666,10 +19821,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="9"/>
+      <c r="D63" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="10"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -19684,10 +19839,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="9"/>
+      <c r="D64" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="10"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -19702,10 +19857,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="9"/>
+      <c r="D65" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="10"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -19720,10 +19875,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="9"/>
+      <c r="D66" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="10"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -19738,10 +19893,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="9"/>
+      <c r="D67" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="10"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -19756,10 +19911,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="9"/>
+      <c r="D68" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="10"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -19774,10 +19929,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="9"/>
+      <c r="D69" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="10"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -19792,10 +19947,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="9"/>
+      <c r="D70" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="10"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -19810,10 +19965,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="9"/>
+      <c r="D71" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="10"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -19828,10 +19983,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="9"/>
+      <c r="D72" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="10"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -19846,10 +20001,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="9"/>
+      <c r="D73" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="10"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -19864,10 +20019,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="9"/>
+      <c r="D74" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="10"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -19882,10 +20037,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="9"/>
+      <c r="D75" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="10"/>
       <c r="F75" s="3" t="s">
         <v>821</v>
       </c>
@@ -19900,10 +20055,10 @@
       <c r="C76" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D76" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="9"/>
+      <c r="D76" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="10"/>
       <c r="F76" s="1" t="s">
         <v>822</v>
       </c>
@@ -19918,10 +20073,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="9"/>
+      <c r="D77" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="10"/>
       <c r="F77" s="1" t="s">
         <v>824</v>
       </c>
@@ -19936,10 +20091,10 @@
       <c r="C78" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="D78" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="9"/>
+      <c r="D78" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="10"/>
       <c r="F78" s="1" t="s">
         <v>826</v>
       </c>
@@ -19954,10 +20109,10 @@
       <c r="C79" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="9"/>
+      <c r="D79" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="10"/>
       <c r="F79" s="1" t="s">
         <v>818</v>
       </c>
@@ -19972,10 +20127,10 @@
       <c r="C80" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="9"/>
+      <c r="D80" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="10"/>
       <c r="F80" s="3" t="s">
         <v>566</v>
       </c>
@@ -19990,10 +20145,10 @@
       <c r="C81" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="9"/>
+      <c r="D81" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="10"/>
       <c r="F81" s="3" t="s">
         <v>14</v>
       </c>
@@ -20008,10 +20163,10 @@
       <c r="C82" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="D82" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="9"/>
+      <c r="D82" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="10"/>
       <c r="F82" s="3" t="s">
         <v>831</v>
       </c>
@@ -20026,10 +20181,10 @@
       <c r="C83" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="D83" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="9"/>
+      <c r="D83" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="10"/>
       <c r="F83" s="1" t="s">
         <v>833</v>
       </c>
@@ -20044,10 +20199,10 @@
       <c r="C84" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D84" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="9"/>
+      <c r="D84" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="10"/>
       <c r="F84" s="3" t="s">
         <v>568</v>
       </c>
@@ -20062,10 +20217,10 @@
       <c r="C85" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="9"/>
+      <c r="D85" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="10"/>
       <c r="F85" s="1" t="s">
         <v>836</v>
       </c>
@@ -20080,10 +20235,10 @@
       <c r="C86" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="D86" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="9"/>
+      <c r="D86" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="10"/>
       <c r="F86" s="1" t="s">
         <v>806</v>
       </c>
@@ -20098,10 +20253,10 @@
       <c r="C87" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D87" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="9"/>
+      <c r="D87" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="10"/>
       <c r="F87" s="3" t="s">
         <v>839</v>
       </c>
@@ -20116,10 +20271,10 @@
       <c r="C88" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="9"/>
+      <c r="D88" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="10"/>
       <c r="F88" s="3" t="s">
         <v>841</v>
       </c>
@@ -20134,10 +20289,10 @@
       <c r="C89" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="D89" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="9"/>
+      <c r="D89" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="10"/>
       <c r="F89" s="1" t="s">
         <v>843</v>
       </c>
@@ -20152,10 +20307,10 @@
       <c r="C90" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="9"/>
+      <c r="D90" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="10"/>
       <c r="F90" s="1" t="s">
         <v>845</v>
       </c>
@@ -20170,10 +20325,10 @@
       <c r="C91" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="D91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9"/>
+      <c r="D91" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="10"/>
       <c r="F91" s="3" t="s">
         <v>568</v>
       </c>
@@ -20188,10 +20343,10 @@
       <c r="C92" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="D92" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="9"/>
+      <c r="D92" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="10"/>
       <c r="F92" s="3" t="s">
         <v>568</v>
       </c>
@@ -20206,10 +20361,10 @@
       <c r="C93" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="D93" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="9"/>
+      <c r="D93" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="10"/>
       <c r="F93" s="3" t="s">
         <v>14</v>
       </c>
@@ -20224,10 +20379,10 @@
       <c r="C94" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D94" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="9"/>
+      <c r="D94" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="10"/>
       <c r="F94" s="1" t="s">
         <v>854</v>
       </c>
@@ -20242,10 +20397,10 @@
       <c r="C95" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="9"/>
+      <c r="D95" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="10"/>
       <c r="F95" s="1" t="s">
         <v>162</v>
       </c>
@@ -20260,10 +20415,10 @@
       <c r="C96" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="D96" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="9"/>
+      <c r="D96" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="10"/>
       <c r="F96" s="3" t="s">
         <v>568</v>
       </c>
@@ -20278,10 +20433,10 @@
       <c r="C97" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="D97" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="9"/>
+      <c r="D97" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="10"/>
       <c r="F97" s="1" t="s">
         <v>859</v>
       </c>
@@ -20296,10 +20451,10 @@
       <c r="C98" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="D98" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="9"/>
+      <c r="D98" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="10"/>
       <c r="F98" s="3" t="s">
         <v>861</v>
       </c>
@@ -20314,10 +20469,10 @@
       <c r="C99" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="D99" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="9"/>
+      <c r="D99" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="10"/>
       <c r="F99" s="1" t="s">
         <v>863</v>
       </c>
@@ -20332,10 +20487,10 @@
       <c r="C100" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="D100" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="9"/>
+      <c r="D100" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="10"/>
       <c r="F100" s="1" t="s">
         <v>865</v>
       </c>
@@ -20350,10 +20505,10 @@
       <c r="C101" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="D101" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="9"/>
+      <c r="D101" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="10"/>
       <c r="F101" s="3" t="s">
         <v>568</v>
       </c>
@@ -20371,10 +20526,10 @@
       <c r="C102" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="D102" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="9"/>
+      <c r="D102" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="10"/>
       <c r="F102" s="3" t="s">
         <v>870</v>
       </c>
@@ -20392,10 +20547,10 @@
       <c r="C103" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D103" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="9"/>
+      <c r="D103" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="10"/>
       <c r="F103" s="3" t="s">
         <v>14</v>
       </c>
@@ -20410,10 +20565,10 @@
       <c r="C104" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="D104" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="9"/>
+      <c r="D104" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="10"/>
       <c r="F104" s="1" t="s">
         <v>875</v>
       </c>
@@ -20428,10 +20583,10 @@
       <c r="C105" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="D105" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="9"/>
+      <c r="D105" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="10"/>
       <c r="F105" s="1" t="s">
         <v>878</v>
       </c>
@@ -20446,10 +20601,10 @@
       <c r="C106" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="D106" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="9"/>
+      <c r="D106" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="10"/>
       <c r="F106" s="3" t="s">
         <v>14</v>
       </c>
@@ -20464,10 +20619,10 @@
       <c r="C107" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D107" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="9"/>
+      <c r="D107" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="10"/>
       <c r="F107" s="3" t="s">
         <v>882</v>
       </c>
@@ -20482,10 +20637,10 @@
       <c r="C108" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="D108" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="9"/>
+      <c r="D108" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="10"/>
       <c r="F108" s="1" t="s">
         <v>884</v>
       </c>
@@ -20500,10 +20655,10 @@
       <c r="C109" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="D109" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="9"/>
+      <c r="D109" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="10"/>
       <c r="F109" s="1" t="s">
         <v>886</v>
       </c>
@@ -20518,10 +20673,10 @@
       <c r="C110" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D110" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="9"/>
+      <c r="D110" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="10"/>
       <c r="F110" s="1" t="s">
         <v>162</v>
       </c>
@@ -20536,10 +20691,10 @@
       <c r="C111" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="D111" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="9"/>
+      <c r="D111" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="10"/>
       <c r="F111" s="3" t="s">
         <v>171</v>
       </c>
@@ -20554,10 +20709,10 @@
       <c r="C112" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D112" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="9"/>
+      <c r="D112" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="10"/>
       <c r="F112" s="1" t="s">
         <v>891</v>
       </c>
@@ -20575,10 +20730,10 @@
       <c r="C113" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="D113" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="9"/>
+      <c r="D113" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="10"/>
       <c r="F113" s="1" t="s">
         <v>893</v>
       </c>
@@ -20593,10 +20748,10 @@
       <c r="C114" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="D114" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="9"/>
+      <c r="D114" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="10"/>
       <c r="F114" s="3" t="s">
         <v>14</v>
       </c>
@@ -20611,10 +20766,10 @@
       <c r="C115" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="D115" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" s="9"/>
+      <c r="D115" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="10"/>
       <c r="F115" s="3" t="s">
         <v>14</v>
       </c>
@@ -20629,10 +20784,10 @@
       <c r="C116" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="D116" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" s="9"/>
+      <c r="D116" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="10"/>
       <c r="F116" s="3" t="s">
         <v>897</v>
       </c>
@@ -20647,10 +20802,10 @@
       <c r="C117" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="D117" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="9"/>
+      <c r="D117" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" s="10"/>
       <c r="F117" s="1" t="s">
         <v>900</v>
       </c>
@@ -20665,10 +20820,10 @@
       <c r="C118" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="D118" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="9"/>
+      <c r="D118" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="10"/>
       <c r="F118" s="1" t="s">
         <v>902</v>
       </c>
@@ -20683,10 +20838,10 @@
       <c r="C119" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="D119" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="9"/>
+      <c r="D119" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="10"/>
       <c r="F119" s="1" t="s">
         <v>905</v>
       </c>
@@ -20701,10 +20856,10 @@
       <c r="C120" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="D120" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E120" s="9"/>
+      <c r="D120" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="10"/>
       <c r="F120" s="2" t="s">
         <v>411</v>
       </c>
@@ -20719,10 +20874,10 @@
       <c r="C121" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="D121" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="9"/>
+      <c r="D121" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="10"/>
       <c r="F121" s="2" t="s">
         <v>234</v>
       </c>
@@ -20737,10 +20892,10 @@
       <c r="C122" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="D122" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="9"/>
+      <c r="D122" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="10"/>
       <c r="F122" s="3" t="s">
         <v>912</v>
       </c>
@@ -20755,10 +20910,10 @@
       <c r="C123" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="D123" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="9"/>
+      <c r="D123" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="10"/>
       <c r="F123" s="3" t="s">
         <v>915</v>
       </c>
@@ -20773,10 +20928,10 @@
       <c r="C124" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="D124" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="9"/>
+      <c r="D124" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="10"/>
       <c r="F124" s="1" t="s">
         <v>918</v>
       </c>
@@ -20791,10 +20946,10 @@
       <c r="C125" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="D125" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="9"/>
+      <c r="D125" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="10"/>
       <c r="F125" s="3" t="s">
         <v>422</v>
       </c>
@@ -20809,10 +20964,10 @@
       <c r="C126" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="D126" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="9"/>
+      <c r="D126" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="10"/>
       <c r="F126" s="3" t="s">
         <v>882</v>
       </c>
@@ -20827,10 +20982,10 @@
       <c r="C127" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D127" s="9" t="s">
+      <c r="D127" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E127" s="9"/>
+      <c r="E127" s="10"/>
       <c r="F127" s="1" t="s">
         <v>925</v>
       </c>
@@ -20845,10 +21000,10 @@
       <c r="C128" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D128" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E128" s="9"/>
+      <c r="D128" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="10"/>
       <c r="F128" s="3" t="s">
         <v>168</v>
       </c>
@@ -20863,10 +21018,10 @@
       <c r="C129" s="3" t="s">
         <v>926</v>
       </c>
-      <c r="D129" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E129" s="9"/>
+      <c r="D129" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="10"/>
       <c r="F129" s="1" t="s">
         <v>927</v>
       </c>
@@ -20881,10 +21036,10 @@
       <c r="C130" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="D130" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E130" s="9"/>
+      <c r="D130" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" s="10"/>
       <c r="F130" s="3" t="s">
         <v>171</v>
       </c>
@@ -20899,10 +21054,10 @@
       <c r="C131" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="D131" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" s="9"/>
+      <c r="D131" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="10"/>
       <c r="F131" s="3" t="s">
         <v>566</v>
       </c>
@@ -20917,10 +21072,10 @@
       <c r="C132" s="3" t="s">
         <v>930</v>
       </c>
-      <c r="D132" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E132" s="9"/>
+      <c r="D132" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="10"/>
       <c r="F132" s="1" t="s">
         <v>162</v>
       </c>
@@ -20935,10 +21090,10 @@
       <c r="C133" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="D133" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133" s="9"/>
+      <c r="D133" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="10"/>
       <c r="F133" s="1" t="s">
         <v>933</v>
       </c>
@@ -20953,10 +21108,10 @@
       <c r="C134" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="D134" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="9"/>
+      <c r="D134" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="10"/>
       <c r="F134" s="1" t="s">
         <v>936</v>
       </c>
@@ -20974,10 +21129,10 @@
       <c r="C135" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="D135" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="9"/>
+      <c r="D135" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" s="10"/>
       <c r="F135" s="1" t="s">
         <v>938</v>
       </c>
@@ -20992,10 +21147,10 @@
       <c r="C136" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D136" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" s="9"/>
+      <c r="D136" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" s="10"/>
       <c r="F136" s="1" t="s">
         <v>940</v>
       </c>
@@ -21010,10 +21165,10 @@
       <c r="C137" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D137" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E137" s="9"/>
+      <c r="D137" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" s="10"/>
       <c r="F137" s="1" t="s">
         <v>942</v>
       </c>
@@ -21028,10 +21183,10 @@
       <c r="C138" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D138" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="9"/>
+      <c r="D138" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="10"/>
       <c r="F138" s="1" t="s">
         <v>943</v>
       </c>
@@ -21046,10 +21201,10 @@
       <c r="C139" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="D139" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="9"/>
+      <c r="D139" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="10"/>
       <c r="F139" s="1" t="s">
         <v>826</v>
       </c>
@@ -21064,10 +21219,10 @@
       <c r="C140" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="D140" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E140" s="9"/>
+      <c r="D140" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" s="10"/>
       <c r="F140" s="4" t="s">
         <v>947</v>
       </c>
@@ -21082,10 +21237,10 @@
       <c r="C141" s="7" t="s">
         <v>955</v>
       </c>
-      <c r="D141" s="9" t="s">
+      <c r="D141" s="10" t="s">
         <v>950</v>
       </c>
-      <c r="E141" s="9"/>
+      <c r="E141" s="10"/>
       <c r="F141" s="7" t="s">
         <v>954</v>
       </c>
@@ -21100,10 +21255,10 @@
       <c r="C142" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="D142" s="9" t="s">
+      <c r="D142" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E142" s="9"/>
+      <c r="E142" s="10"/>
       <c r="F142" s="7" t="s">
         <v>953</v>
       </c>
@@ -21118,10 +21273,10 @@
       <c r="C143" s="7" t="s">
         <v>958</v>
       </c>
-      <c r="D143" s="9" t="s">
+      <c r="D143" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E143" s="9"/>
+      <c r="E143" s="10"/>
       <c r="F143" s="7" t="s">
         <v>960</v>
       </c>
@@ -21136,10 +21291,10 @@
       <c r="C144" s="7" t="s">
         <v>961</v>
       </c>
-      <c r="D144" s="9" t="s">
+      <c r="D144" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E144" s="9"/>
+      <c r="E144" s="10"/>
       <c r="F144" s="7" t="s">
         <v>962</v>
       </c>
@@ -21157,10 +21312,10 @@
       <c r="C145" s="7" t="s">
         <v>964</v>
       </c>
-      <c r="D145" s="9" t="s">
+      <c r="D145" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E145" s="9"/>
+      <c r="E145" s="10"/>
       <c r="F145" s="3" t="s">
         <v>965</v>
       </c>
@@ -21175,10 +21330,10 @@
       <c r="C146" s="7" t="s">
         <v>966</v>
       </c>
-      <c r="D146" s="9" t="s">
+      <c r="D146" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E146" s="9"/>
+      <c r="E146" s="10"/>
       <c r="F146" s="3" t="s">
         <v>967</v>
       </c>
@@ -21193,10 +21348,10 @@
       <c r="C147" s="7" t="s">
         <v>968</v>
       </c>
-      <c r="D147" s="9" t="s">
+      <c r="D147" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E147" s="9"/>
+      <c r="E147" s="10"/>
       <c r="F147" s="7" t="s">
         <v>969</v>
       </c>
@@ -21214,10 +21369,10 @@
       <c r="C148" s="7" t="s">
         <v>970</v>
       </c>
-      <c r="D148" s="9" t="s">
+      <c r="D148" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E148" s="9"/>
+      <c r="E148" s="10"/>
       <c r="F148" s="7" t="s">
         <v>971</v>
       </c>
@@ -21235,10 +21390,10 @@
       <c r="C149" s="7" t="s">
         <v>972</v>
       </c>
-      <c r="D149" s="9" t="s">
+      <c r="D149" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E149" s="9"/>
+      <c r="E149" s="10"/>
       <c r="F149" s="7" t="s">
         <v>974</v>
       </c>
@@ -21253,10 +21408,10 @@
       <c r="C150" s="7" t="s">
         <v>973</v>
       </c>
-      <c r="D150" s="9" t="s">
+      <c r="D150" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E150" s="9"/>
+      <c r="E150" s="10"/>
       <c r="F150" s="7" t="s">
         <v>975</v>
       </c>
@@ -21271,10 +21426,10 @@
       <c r="C151" s="3" t="s">
         <v>976</v>
       </c>
-      <c r="D151" s="9" t="s">
+      <c r="D151" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E151" s="9"/>
+      <c r="E151" s="10"/>
       <c r="F151" s="7" t="s">
         <v>980</v>
       </c>
@@ -21289,10 +21444,10 @@
       <c r="C152" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="D152" s="9" t="s">
+      <c r="D152" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E152" s="9"/>
+      <c r="E152" s="10"/>
       <c r="F152" s="7" t="s">
         <v>981</v>
       </c>
@@ -21307,10 +21462,10 @@
       <c r="C153" s="7" t="s">
         <v>978</v>
       </c>
-      <c r="D153" s="9" t="s">
+      <c r="D153" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E153" s="9"/>
+      <c r="E153" s="10"/>
       <c r="F153" s="7" t="s">
         <v>982</v>
       </c>
@@ -21325,10 +21480,10 @@
       <c r="C154" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="D154" s="9" t="s">
+      <c r="D154" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E154" s="9"/>
+      <c r="E154" s="10"/>
       <c r="F154" s="7" t="s">
         <v>983</v>
       </c>
@@ -21343,10 +21498,10 @@
       <c r="C155" s="7" t="s">
         <v>984</v>
       </c>
-      <c r="D155" s="9" t="s">
+      <c r="D155" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E155" s="9"/>
+      <c r="E155" s="10"/>
       <c r="F155" s="7" t="s">
         <v>981</v>
       </c>
@@ -21361,10 +21516,10 @@
       <c r="C156" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="D156" s="9" t="s">
+      <c r="D156" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E156" s="9"/>
+      <c r="E156" s="10"/>
       <c r="F156" s="7" t="s">
         <v>986</v>
       </c>
@@ -21379,10 +21534,10 @@
       <c r="C157" s="7" t="s">
         <v>987</v>
       </c>
-      <c r="D157" s="9" t="s">
+      <c r="D157" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E157" s="9"/>
+      <c r="E157" s="10"/>
       <c r="F157" s="3" t="s">
         <v>988</v>
       </c>
@@ -21397,10 +21552,10 @@
       <c r="C158" s="7" t="s">
         <v>989</v>
       </c>
-      <c r="D158" s="9" t="s">
+      <c r="D158" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="E158" s="9"/>
+      <c r="E158" s="10"/>
       <c r="F158" s="7" t="s">
         <v>983</v>
       </c>
@@ -21415,10 +21570,10 @@
       <c r="C159" s="8" t="s">
         <v>991</v>
       </c>
-      <c r="D159" s="9" t="s">
+      <c r="D159" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E159" s="9"/>
+      <c r="E159" s="10"/>
       <c r="F159" s="3" t="s">
         <v>995</v>
       </c>
@@ -21436,10 +21591,10 @@
       <c r="C160" s="8" t="s">
         <v>993</v>
       </c>
-      <c r="D160" s="9" t="s">
+      <c r="D160" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E160" s="9"/>
+      <c r="E160" s="10"/>
       <c r="F160" s="3" t="s">
         <v>996</v>
       </c>
@@ -21454,10 +21609,10 @@
       <c r="C161" s="8" t="s">
         <v>994</v>
       </c>
-      <c r="D161" s="9" t="s">
+      <c r="D161" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E161" s="9"/>
+      <c r="E161" s="10"/>
       <c r="F161" s="8" t="s">
         <v>997</v>
       </c>
@@ -21472,10 +21627,10 @@
       <c r="C162" s="8" t="s">
         <v>998</v>
       </c>
-      <c r="D162" s="9" t="s">
+      <c r="D162" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E162" s="9"/>
+      <c r="E162" s="10"/>
       <c r="F162" s="3" t="s">
         <v>999</v>
       </c>
@@ -21490,10 +21645,10 @@
       <c r="C163" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="D163" s="9" t="s">
+      <c r="D163" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E163" s="9"/>
+      <c r="E163" s="10"/>
       <c r="F163" s="8" t="s">
         <v>1001</v>
       </c>
@@ -21508,10 +21663,10 @@
       <c r="C164" s="8" t="s">
         <v>1002</v>
       </c>
-      <c r="D164" s="9" t="s">
+      <c r="D164" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E164" s="9"/>
+      <c r="E164" s="10"/>
       <c r="F164" s="8" t="s">
         <v>1003</v>
       </c>
@@ -21526,12 +21681,12 @@
       <c r="C165" s="8" t="s">
         <v>1005</v>
       </c>
-      <c r="D165" s="9" t="s">
+      <c r="D165" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E165" s="9"/>
-      <c r="F165" s="3" t="s">
-        <v>996</v>
+      <c r="E165" s="10"/>
+      <c r="F165" s="9" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="18" customHeight="1">
@@ -21544,11 +21699,11 @@
       <c r="C166" s="8" t="s">
         <v>1006</v>
       </c>
-      <c r="D166" s="9" t="s">
+      <c r="D166" s="10" t="s">
         <v>992</v>
       </c>
-      <c r="E166" s="9"/>
-      <c r="F166" s="8" t="s">
+      <c r="E166" s="10"/>
+      <c r="F166" s="9" t="s">
         <v>1007</v>
       </c>
       <c r="G166" s="8" t="s">
@@ -21556,100 +21711,295 @@
       </c>
     </row>
     <row r="167" spans="1:7" ht="18" customHeight="1">
-      <c r="D167" s="9"/>
-      <c r="E167" s="9"/>
+      <c r="A167" s="9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B167" s="1">
+        <v>6430</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D167" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E167" s="10"/>
+      <c r="F167" s="9" t="s">
+        <v>1013</v>
+      </c>
     </row>
     <row r="168" spans="1:7" ht="18" customHeight="1">
-      <c r="D168" s="9"/>
-      <c r="E168" s="9"/>
+      <c r="A168" s="9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B168" s="1">
+        <v>6430</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D168" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E168" s="10"/>
+      <c r="F168" s="9" t="s">
+        <v>1016</v>
+      </c>
     </row>
     <row r="169" spans="1:7" ht="18" customHeight="1">
-      <c r="D169" s="9"/>
-      <c r="E169" s="9"/>
+      <c r="A169" s="9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B169" s="1">
+        <v>6427</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D169" s="10" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E169" s="10"/>
+      <c r="F169" s="9" t="s">
+        <v>1011</v>
+      </c>
     </row>
     <row r="170" spans="1:7" ht="18" customHeight="1">
-      <c r="D170" s="9"/>
-      <c r="E170" s="9"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="10"/>
     </row>
     <row r="171" spans="1:7" ht="18" customHeight="1">
-      <c r="D171" s="9"/>
-      <c r="E171" s="9"/>
+      <c r="D171" s="10"/>
+      <c r="E171" s="10"/>
     </row>
     <row r="172" spans="1:7" ht="18" customHeight="1">
-      <c r="D172" s="9"/>
-      <c r="E172" s="9"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
     </row>
     <row r="173" spans="1:7" ht="18" customHeight="1">
-      <c r="D173" s="9"/>
-      <c r="E173" s="9"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="10"/>
     </row>
     <row r="174" spans="1:7" ht="18" customHeight="1">
-      <c r="D174" s="9"/>
-      <c r="E174" s="9"/>
+      <c r="D174" s="10"/>
+      <c r="E174" s="10"/>
     </row>
     <row r="175" spans="1:7" ht="18" customHeight="1">
-      <c r="D175" s="9"/>
-      <c r="E175" s="9"/>
+      <c r="D175" s="10"/>
+      <c r="E175" s="10"/>
     </row>
     <row r="176" spans="1:7" ht="18" customHeight="1">
-      <c r="D176" s="9"/>
-      <c r="E176" s="9"/>
+      <c r="D176" s="10"/>
+      <c r="E176" s="10"/>
     </row>
     <row r="177" spans="4:5" ht="18" customHeight="1">
-      <c r="D177" s="9"/>
-      <c r="E177" s="9"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="10"/>
     </row>
     <row r="178" spans="4:5" ht="18" customHeight="1">
-      <c r="D178" s="9"/>
-      <c r="E178" s="9"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
     </row>
     <row r="179" spans="4:5" ht="18" customHeight="1">
-      <c r="D179" s="9"/>
-      <c r="E179" s="9"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
     </row>
     <row r="180" spans="4:5" ht="18" customHeight="1">
-      <c r="D180" s="9"/>
-      <c r="E180" s="9"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
     </row>
     <row r="181" spans="4:5" ht="18" customHeight="1">
-      <c r="D181" s="9"/>
-      <c r="E181" s="9"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
     </row>
     <row r="182" spans="4:5" ht="18" customHeight="1">
-      <c r="D182" s="9"/>
-      <c r="E182" s="9"/>
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
     </row>
     <row r="183" spans="4:5" ht="18" customHeight="1">
-      <c r="D183" s="9"/>
-      <c r="E183" s="9"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
     </row>
     <row r="184" spans="4:5" ht="18" customHeight="1">
-      <c r="D184" s="9"/>
-      <c r="E184" s="9"/>
+      <c r="D184" s="10"/>
+      <c r="E184" s="10"/>
     </row>
     <row r="185" spans="4:5" ht="18" customHeight="1">
-      <c r="D185" s="9"/>
-      <c r="E185" s="9"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
     </row>
     <row r="186" spans="4:5" ht="18" customHeight="1">
-      <c r="D186" s="9"/>
-      <c r="E186" s="9"/>
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
     </row>
     <row r="187" spans="4:5" ht="18" customHeight="1">
-      <c r="D187" s="9"/>
-      <c r="E187" s="9"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
     </row>
     <row r="188" spans="4:5" ht="18" customHeight="1">
-      <c r="D188" s="9"/>
-      <c r="E188" s="9"/>
+      <c r="D188" s="10"/>
+      <c r="E188" s="10"/>
     </row>
     <row r="189" spans="4:5" ht="18" customHeight="1">
-      <c r="D189" s="9"/>
-      <c r="E189" s="9"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G139"/>
+  <autoFilter ref="A1:G169"/>
   <mergeCells count="164">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -21661,159 +22011,6 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
add hdu6428 and hdu6429
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="1027">
   <si>
     <t>OJ</t>
   </si>
@@ -12242,6 +12242,83 @@
   </si>
   <si>
     <t>思维;堆</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calculate</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>莫比乌斯反演</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Permutations</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp</t>
+    </r>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -12344,7 +12421,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -12365,6 +12442,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -18660,7 +18743,7 @@
   <dimension ref="A1:G189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F166" sqref="F166"/>
+      <selection activeCell="F171" sqref="F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
@@ -19113,10 +19196,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="10"/>
+      <c r="D26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -19134,10 +19217,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="10"/>
+      <c r="D27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="12"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -19155,10 +19238,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="10"/>
+      <c r="D28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="12"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -19176,10 +19259,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="10"/>
+      <c r="D29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="12"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -19197,10 +19280,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="10"/>
+      <c r="D30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="12"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -19215,10 +19298,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="10"/>
+      <c r="D31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="12"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -19233,10 +19316,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="10"/>
+      <c r="D32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="12"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -19251,10 +19334,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="10"/>
+      <c r="D33" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="12"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -19272,10 +19355,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="12">
         <v>97</v>
       </c>
-      <c r="E34" s="10"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -19290,10 +19373,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="10"/>
+      <c r="D35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="12"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -19308,10 +19391,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="10"/>
+      <c r="D36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="12"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -19326,10 +19409,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="10"/>
+      <c r="D37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="12"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -19344,10 +19427,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="10"/>
+      <c r="D38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="12"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -19365,10 +19448,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="10"/>
+      <c r="D39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="12"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -19386,10 +19469,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="10"/>
+      <c r="D40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="12"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -19404,10 +19487,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="10"/>
+      <c r="D41" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="12"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -19425,10 +19508,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="10"/>
+      <c r="D42" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="12"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -19443,10 +19526,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="10"/>
+      <c r="D43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="12"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -19464,10 +19547,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="10"/>
+      <c r="D44" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="12"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -19482,10 +19565,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="10"/>
+      <c r="D45" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="12"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -19500,10 +19583,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="10"/>
+      <c r="D46" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="12"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -19518,10 +19601,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="10"/>
+      <c r="D47" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="12"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -19539,10 +19622,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="10"/>
+      <c r="D48" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="12"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -19557,10 +19640,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="10"/>
+      <c r="D49" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="12"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -19578,10 +19661,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="10"/>
+      <c r="D50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="12"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -19599,10 +19682,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="10"/>
+      <c r="D51" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="12"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -19617,10 +19700,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="10"/>
+      <c r="D52" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="12"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -19635,10 +19718,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="10"/>
+      <c r="D53" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="12"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -19653,10 +19736,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="10"/>
+      <c r="D54" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="12"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -19671,10 +19754,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="10"/>
+      <c r="D55" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="12"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -19689,10 +19772,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="10"/>
+      <c r="D56" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="12"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -19707,10 +19790,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="10"/>
+      <c r="D57" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="12"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -19725,10 +19808,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="10"/>
+      <c r="D58" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="12"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -19743,10 +19826,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="10"/>
+      <c r="D59" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="12"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -19764,10 +19847,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="10"/>
+      <c r="D60" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="12"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -19782,10 +19865,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="10"/>
+      <c r="D61" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="12"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -19803,10 +19886,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="10"/>
+      <c r="D62" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="12"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -19821,10 +19904,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="10"/>
+      <c r="D63" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="12"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -19839,10 +19922,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="10"/>
+      <c r="D64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="12"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -19857,10 +19940,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="10"/>
+      <c r="D65" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="12"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -19875,10 +19958,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="10"/>
+      <c r="D66" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="12"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -19893,10 +19976,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="10"/>
+      <c r="D67" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="12"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -19911,10 +19994,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="10"/>
+      <c r="D68" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="12"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -19929,10 +20012,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="10"/>
+      <c r="D69" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="12"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -19947,10 +20030,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="10"/>
+      <c r="D70" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="12"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -19965,10 +20048,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="10"/>
+      <c r="D71" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="12"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -19983,10 +20066,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="10"/>
+      <c r="D72" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="12"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -20001,10 +20084,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="10"/>
+      <c r="D73" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="12"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -20019,10 +20102,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="10"/>
+      <c r="D74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="12"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -20037,10 +20120,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="10"/>
+      <c r="D75" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="12"/>
       <c r="F75" s="3" t="s">
         <v>821</v>
       </c>
@@ -20055,10 +20138,10 @@
       <c r="C76" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="10"/>
+      <c r="D76" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="12"/>
       <c r="F76" s="1" t="s">
         <v>822</v>
       </c>
@@ -20073,10 +20156,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="10"/>
+      <c r="D77" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="12"/>
       <c r="F77" s="1" t="s">
         <v>824</v>
       </c>
@@ -20091,10 +20174,10 @@
       <c r="C78" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="D78" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="10"/>
+      <c r="D78" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="12"/>
       <c r="F78" s="1" t="s">
         <v>826</v>
       </c>
@@ -20109,10 +20192,10 @@
       <c r="C79" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="D79" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="10"/>
+      <c r="D79" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="12"/>
       <c r="F79" s="1" t="s">
         <v>818</v>
       </c>
@@ -20127,10 +20210,10 @@
       <c r="C80" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="D80" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="10"/>
+      <c r="D80" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="12"/>
       <c r="F80" s="3" t="s">
         <v>566</v>
       </c>
@@ -20145,10 +20228,10 @@
       <c r="C81" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="10"/>
+      <c r="D81" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="12"/>
       <c r="F81" s="3" t="s">
         <v>14</v>
       </c>
@@ -20163,10 +20246,10 @@
       <c r="C82" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="10"/>
+      <c r="D82" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="12"/>
       <c r="F82" s="3" t="s">
         <v>831</v>
       </c>
@@ -20181,10 +20264,10 @@
       <c r="C83" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="D83" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="10"/>
+      <c r="D83" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="12"/>
       <c r="F83" s="1" t="s">
         <v>833</v>
       </c>
@@ -20199,10 +20282,10 @@
       <c r="C84" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D84" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="10"/>
+      <c r="D84" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="12"/>
       <c r="F84" s="3" t="s">
         <v>568</v>
       </c>
@@ -20217,10 +20300,10 @@
       <c r="C85" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="D85" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="10"/>
+      <c r="D85" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="12"/>
       <c r="F85" s="1" t="s">
         <v>836</v>
       </c>
@@ -20235,10 +20318,10 @@
       <c r="C86" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="D86" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="10"/>
+      <c r="D86" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="12"/>
       <c r="F86" s="1" t="s">
         <v>806</v>
       </c>
@@ -20253,10 +20336,10 @@
       <c r="C87" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D87" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="10"/>
+      <c r="D87" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="12"/>
       <c r="F87" s="3" t="s">
         <v>839</v>
       </c>
@@ -20271,10 +20354,10 @@
       <c r="C88" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="D88" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="10"/>
+      <c r="D88" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="12"/>
       <c r="F88" s="3" t="s">
         <v>841</v>
       </c>
@@ -20289,10 +20372,10 @@
       <c r="C89" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="D89" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="10"/>
+      <c r="D89" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="12"/>
       <c r="F89" s="1" t="s">
         <v>843</v>
       </c>
@@ -20307,10 +20390,10 @@
       <c r="C90" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="D90" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="10"/>
+      <c r="D90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="12"/>
       <c r="F90" s="1" t="s">
         <v>845</v>
       </c>
@@ -20325,10 +20408,10 @@
       <c r="C91" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="D91" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="10"/>
+      <c r="D91" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="12"/>
       <c r="F91" s="3" t="s">
         <v>568</v>
       </c>
@@ -20343,10 +20426,10 @@
       <c r="C92" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="D92" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="10"/>
+      <c r="D92" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="12"/>
       <c r="F92" s="3" t="s">
         <v>568</v>
       </c>
@@ -20361,10 +20444,10 @@
       <c r="C93" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="D93" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="10"/>
+      <c r="D93" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="12"/>
       <c r="F93" s="3" t="s">
         <v>14</v>
       </c>
@@ -20379,10 +20462,10 @@
       <c r="C94" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D94" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="10"/>
+      <c r="D94" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="12"/>
       <c r="F94" s="1" t="s">
         <v>854</v>
       </c>
@@ -20397,10 +20480,10 @@
       <c r="C95" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="D95" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="10"/>
+      <c r="D95" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="12"/>
       <c r="F95" s="1" t="s">
         <v>162</v>
       </c>
@@ -20415,10 +20498,10 @@
       <c r="C96" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="D96" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="10"/>
+      <c r="D96" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="12"/>
       <c r="F96" s="3" t="s">
         <v>568</v>
       </c>
@@ -20433,10 +20516,10 @@
       <c r="C97" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="D97" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="10"/>
+      <c r="D97" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="12"/>
       <c r="F97" s="1" t="s">
         <v>859</v>
       </c>
@@ -20451,10 +20534,10 @@
       <c r="C98" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="D98" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="10"/>
+      <c r="D98" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="12"/>
       <c r="F98" s="3" t="s">
         <v>861</v>
       </c>
@@ -20469,10 +20552,10 @@
       <c r="C99" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="D99" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="10"/>
+      <c r="D99" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="12"/>
       <c r="F99" s="1" t="s">
         <v>863</v>
       </c>
@@ -20487,10 +20570,10 @@
       <c r="C100" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="D100" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="10"/>
+      <c r="D100" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="12"/>
       <c r="F100" s="1" t="s">
         <v>865</v>
       </c>
@@ -20505,10 +20588,10 @@
       <c r="C101" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="D101" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="10"/>
+      <c r="D101" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="12"/>
       <c r="F101" s="3" t="s">
         <v>568</v>
       </c>
@@ -20526,10 +20609,10 @@
       <c r="C102" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="D102" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="10"/>
+      <c r="D102" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="12"/>
       <c r="F102" s="3" t="s">
         <v>870</v>
       </c>
@@ -20547,10 +20630,10 @@
       <c r="C103" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D103" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="10"/>
+      <c r="D103" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="12"/>
       <c r="F103" s="3" t="s">
         <v>14</v>
       </c>
@@ -20565,10 +20648,10 @@
       <c r="C104" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="D104" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="10"/>
+      <c r="D104" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="12"/>
       <c r="F104" s="1" t="s">
         <v>875</v>
       </c>
@@ -20583,10 +20666,10 @@
       <c r="C105" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="D105" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="10"/>
+      <c r="D105" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="12"/>
       <c r="F105" s="1" t="s">
         <v>878</v>
       </c>
@@ -20601,10 +20684,10 @@
       <c r="C106" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="D106" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="10"/>
+      <c r="D106" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="12"/>
       <c r="F106" s="3" t="s">
         <v>14</v>
       </c>
@@ -20619,10 +20702,10 @@
       <c r="C107" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D107" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="10"/>
+      <c r="D107" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="12"/>
       <c r="F107" s="3" t="s">
         <v>882</v>
       </c>
@@ -20637,10 +20720,10 @@
       <c r="C108" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="D108" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="10"/>
+      <c r="D108" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="12"/>
       <c r="F108" s="1" t="s">
         <v>884</v>
       </c>
@@ -20655,10 +20738,10 @@
       <c r="C109" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="D109" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="10"/>
+      <c r="D109" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="12"/>
       <c r="F109" s="1" t="s">
         <v>886</v>
       </c>
@@ -20673,10 +20756,10 @@
       <c r="C110" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D110" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="10"/>
+      <c r="D110" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="12"/>
       <c r="F110" s="1" t="s">
         <v>162</v>
       </c>
@@ -20691,10 +20774,10 @@
       <c r="C111" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="D111" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="10"/>
+      <c r="D111" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="12"/>
       <c r="F111" s="3" t="s">
         <v>171</v>
       </c>
@@ -20709,10 +20792,10 @@
       <c r="C112" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D112" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="10"/>
+      <c r="D112" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="12"/>
       <c r="F112" s="1" t="s">
         <v>891</v>
       </c>
@@ -20730,10 +20813,10 @@
       <c r="C113" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="D113" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="10"/>
+      <c r="D113" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="12"/>
       <c r="F113" s="1" t="s">
         <v>893</v>
       </c>
@@ -20748,10 +20831,10 @@
       <c r="C114" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="D114" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="10"/>
+      <c r="D114" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="12"/>
       <c r="F114" s="3" t="s">
         <v>14</v>
       </c>
@@ -20766,10 +20849,10 @@
       <c r="C115" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="D115" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" s="10"/>
+      <c r="D115" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="12"/>
       <c r="F115" s="3" t="s">
         <v>14</v>
       </c>
@@ -20784,10 +20867,10 @@
       <c r="C116" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="D116" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" s="10"/>
+      <c r="D116" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="12"/>
       <c r="F116" s="3" t="s">
         <v>897</v>
       </c>
@@ -20802,10 +20885,10 @@
       <c r="C117" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="D117" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="10"/>
+      <c r="D117" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" s="12"/>
       <c r="F117" s="1" t="s">
         <v>900</v>
       </c>
@@ -20820,10 +20903,10 @@
       <c r="C118" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="D118" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="10"/>
+      <c r="D118" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="12"/>
       <c r="F118" s="1" t="s">
         <v>902</v>
       </c>
@@ -20838,10 +20921,10 @@
       <c r="C119" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="D119" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="10"/>
+      <c r="D119" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="12"/>
       <c r="F119" s="1" t="s">
         <v>905</v>
       </c>
@@ -20856,10 +20939,10 @@
       <c r="C120" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="D120" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E120" s="10"/>
+      <c r="D120" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="12"/>
       <c r="F120" s="2" t="s">
         <v>411</v>
       </c>
@@ -20874,10 +20957,10 @@
       <c r="C121" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="D121" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="10"/>
+      <c r="D121" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="12"/>
       <c r="F121" s="2" t="s">
         <v>234</v>
       </c>
@@ -20892,10 +20975,10 @@
       <c r="C122" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="D122" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="10"/>
+      <c r="D122" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="12"/>
       <c r="F122" s="3" t="s">
         <v>912</v>
       </c>
@@ -20910,10 +20993,10 @@
       <c r="C123" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="D123" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="10"/>
+      <c r="D123" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="12"/>
       <c r="F123" s="3" t="s">
         <v>915</v>
       </c>
@@ -20928,10 +21011,10 @@
       <c r="C124" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="D124" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="10"/>
+      <c r="D124" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="12"/>
       <c r="F124" s="1" t="s">
         <v>918</v>
       </c>
@@ -20946,10 +21029,10 @@
       <c r="C125" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="D125" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="10"/>
+      <c r="D125" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="12"/>
       <c r="F125" s="3" t="s">
         <v>422</v>
       </c>
@@ -20964,10 +21047,10 @@
       <c r="C126" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="D126" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="10"/>
+      <c r="D126" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="12"/>
       <c r="F126" s="3" t="s">
         <v>882</v>
       </c>
@@ -20982,10 +21065,10 @@
       <c r="C127" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D127" s="10" t="s">
+      <c r="D127" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E127" s="10"/>
+      <c r="E127" s="12"/>
       <c r="F127" s="1" t="s">
         <v>925</v>
       </c>
@@ -21000,10 +21083,10 @@
       <c r="C128" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D128" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E128" s="10"/>
+      <c r="D128" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="12"/>
       <c r="F128" s="3" t="s">
         <v>168</v>
       </c>
@@ -21018,10 +21101,10 @@
       <c r="C129" s="3" t="s">
         <v>926</v>
       </c>
-      <c r="D129" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E129" s="10"/>
+      <c r="D129" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="12"/>
       <c r="F129" s="1" t="s">
         <v>927</v>
       </c>
@@ -21036,10 +21119,10 @@
       <c r="C130" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="D130" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E130" s="10"/>
+      <c r="D130" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" s="12"/>
       <c r="F130" s="3" t="s">
         <v>171</v>
       </c>
@@ -21054,10 +21137,10 @@
       <c r="C131" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="D131" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" s="10"/>
+      <c r="D131" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="12"/>
       <c r="F131" s="3" t="s">
         <v>566</v>
       </c>
@@ -21072,10 +21155,10 @@
       <c r="C132" s="3" t="s">
         <v>930</v>
       </c>
-      <c r="D132" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E132" s="10"/>
+      <c r="D132" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="12"/>
       <c r="F132" s="1" t="s">
         <v>162</v>
       </c>
@@ -21090,10 +21173,10 @@
       <c r="C133" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="D133" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133" s="10"/>
+      <c r="D133" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="12"/>
       <c r="F133" s="1" t="s">
         <v>933</v>
       </c>
@@ -21108,10 +21191,10 @@
       <c r="C134" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="D134" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="10"/>
+      <c r="D134" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="12"/>
       <c r="F134" s="1" t="s">
         <v>936</v>
       </c>
@@ -21129,10 +21212,10 @@
       <c r="C135" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="D135" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="10"/>
+      <c r="D135" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" s="12"/>
       <c r="F135" s="1" t="s">
         <v>938</v>
       </c>
@@ -21147,10 +21230,10 @@
       <c r="C136" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D136" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" s="10"/>
+      <c r="D136" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" s="12"/>
       <c r="F136" s="1" t="s">
         <v>940</v>
       </c>
@@ -21165,10 +21248,10 @@
       <c r="C137" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D137" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E137" s="10"/>
+      <c r="D137" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" s="12"/>
       <c r="F137" s="1" t="s">
         <v>942</v>
       </c>
@@ -21183,10 +21266,10 @@
       <c r="C138" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D138" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="10"/>
+      <c r="D138" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="12"/>
       <c r="F138" s="1" t="s">
         <v>943</v>
       </c>
@@ -21201,10 +21284,10 @@
       <c r="C139" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="D139" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="10"/>
+      <c r="D139" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="12"/>
       <c r="F139" s="1" t="s">
         <v>826</v>
       </c>
@@ -21219,10 +21302,10 @@
       <c r="C140" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="D140" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E140" s="10"/>
+      <c r="D140" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" s="12"/>
       <c r="F140" s="4" t="s">
         <v>947</v>
       </c>
@@ -21237,10 +21320,10 @@
       <c r="C141" s="7" t="s">
         <v>955</v>
       </c>
-      <c r="D141" s="10" t="s">
+      <c r="D141" s="12" t="s">
         <v>950</v>
       </c>
-      <c r="E141" s="10"/>
+      <c r="E141" s="12"/>
       <c r="F141" s="7" t="s">
         <v>954</v>
       </c>
@@ -21255,10 +21338,10 @@
       <c r="C142" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="D142" s="10" t="s">
+      <c r="D142" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E142" s="10"/>
+      <c r="E142" s="12"/>
       <c r="F142" s="7" t="s">
         <v>953</v>
       </c>
@@ -21273,10 +21356,10 @@
       <c r="C143" s="7" t="s">
         <v>958</v>
       </c>
-      <c r="D143" s="10" t="s">
+      <c r="D143" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E143" s="10"/>
+      <c r="E143" s="12"/>
       <c r="F143" s="7" t="s">
         <v>960</v>
       </c>
@@ -21291,10 +21374,10 @@
       <c r="C144" s="7" t="s">
         <v>961</v>
       </c>
-      <c r="D144" s="10" t="s">
+      <c r="D144" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E144" s="10"/>
+      <c r="E144" s="12"/>
       <c r="F144" s="7" t="s">
         <v>962</v>
       </c>
@@ -21312,10 +21395,10 @@
       <c r="C145" s="7" t="s">
         <v>964</v>
       </c>
-      <c r="D145" s="10" t="s">
+      <c r="D145" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E145" s="10"/>
+      <c r="E145" s="12"/>
       <c r="F145" s="3" t="s">
         <v>965</v>
       </c>
@@ -21330,10 +21413,10 @@
       <c r="C146" s="7" t="s">
         <v>966</v>
       </c>
-      <c r="D146" s="10" t="s">
+      <c r="D146" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E146" s="10"/>
+      <c r="E146" s="12"/>
       <c r="F146" s="3" t="s">
         <v>967</v>
       </c>
@@ -21348,10 +21431,10 @@
       <c r="C147" s="7" t="s">
         <v>968</v>
       </c>
-      <c r="D147" s="10" t="s">
+      <c r="D147" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E147" s="10"/>
+      <c r="E147" s="12"/>
       <c r="F147" s="7" t="s">
         <v>969</v>
       </c>
@@ -21369,10 +21452,10 @@
       <c r="C148" s="7" t="s">
         <v>970</v>
       </c>
-      <c r="D148" s="10" t="s">
+      <c r="D148" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E148" s="10"/>
+      <c r="E148" s="12"/>
       <c r="F148" s="7" t="s">
         <v>971</v>
       </c>
@@ -21390,10 +21473,10 @@
       <c r="C149" s="7" t="s">
         <v>972</v>
       </c>
-      <c r="D149" s="10" t="s">
+      <c r="D149" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E149" s="10"/>
+      <c r="E149" s="12"/>
       <c r="F149" s="7" t="s">
         <v>974</v>
       </c>
@@ -21408,10 +21491,10 @@
       <c r="C150" s="7" t="s">
         <v>973</v>
       </c>
-      <c r="D150" s="10" t="s">
+      <c r="D150" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E150" s="10"/>
+      <c r="E150" s="12"/>
       <c r="F150" s="7" t="s">
         <v>975</v>
       </c>
@@ -21426,10 +21509,10 @@
       <c r="C151" s="3" t="s">
         <v>976</v>
       </c>
-      <c r="D151" s="10" t="s">
+      <c r="D151" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E151" s="10"/>
+      <c r="E151" s="12"/>
       <c r="F151" s="7" t="s">
         <v>980</v>
       </c>
@@ -21444,10 +21527,10 @@
       <c r="C152" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="D152" s="10" t="s">
+      <c r="D152" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E152" s="10"/>
+      <c r="E152" s="12"/>
       <c r="F152" s="7" t="s">
         <v>981</v>
       </c>
@@ -21462,10 +21545,10 @@
       <c r="C153" s="7" t="s">
         <v>978</v>
       </c>
-      <c r="D153" s="10" t="s">
+      <c r="D153" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E153" s="10"/>
+      <c r="E153" s="12"/>
       <c r="F153" s="7" t="s">
         <v>982</v>
       </c>
@@ -21480,10 +21563,10 @@
       <c r="C154" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="D154" s="10" t="s">
+      <c r="D154" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E154" s="10"/>
+      <c r="E154" s="12"/>
       <c r="F154" s="7" t="s">
         <v>983</v>
       </c>
@@ -21498,10 +21581,10 @@
       <c r="C155" s="7" t="s">
         <v>984</v>
       </c>
-      <c r="D155" s="10" t="s">
+      <c r="D155" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E155" s="10"/>
+      <c r="E155" s="12"/>
       <c r="F155" s="7" t="s">
         <v>981</v>
       </c>
@@ -21516,10 +21599,10 @@
       <c r="C156" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="D156" s="10" t="s">
+      <c r="D156" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E156" s="10"/>
+      <c r="E156" s="12"/>
       <c r="F156" s="7" t="s">
         <v>986</v>
       </c>
@@ -21534,10 +21617,10 @@
       <c r="C157" s="7" t="s">
         <v>987</v>
       </c>
-      <c r="D157" s="10" t="s">
+      <c r="D157" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E157" s="10"/>
+      <c r="E157" s="12"/>
       <c r="F157" s="3" t="s">
         <v>988</v>
       </c>
@@ -21552,10 +21635,10 @@
       <c r="C158" s="7" t="s">
         <v>989</v>
       </c>
-      <c r="D158" s="10" t="s">
+      <c r="D158" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="E158" s="10"/>
+      <c r="E158" s="12"/>
       <c r="F158" s="7" t="s">
         <v>983</v>
       </c>
@@ -21570,10 +21653,10 @@
       <c r="C159" s="8" t="s">
         <v>991</v>
       </c>
-      <c r="D159" s="10" t="s">
+      <c r="D159" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E159" s="10"/>
+      <c r="E159" s="12"/>
       <c r="F159" s="3" t="s">
         <v>995</v>
       </c>
@@ -21591,10 +21674,10 @@
       <c r="C160" s="8" t="s">
         <v>993</v>
       </c>
-      <c r="D160" s="10" t="s">
+      <c r="D160" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E160" s="10"/>
+      <c r="E160" s="12"/>
       <c r="F160" s="3" t="s">
         <v>996</v>
       </c>
@@ -21609,10 +21692,10 @@
       <c r="C161" s="8" t="s">
         <v>994</v>
       </c>
-      <c r="D161" s="10" t="s">
+      <c r="D161" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E161" s="10"/>
+      <c r="E161" s="12"/>
       <c r="F161" s="8" t="s">
         <v>997</v>
       </c>
@@ -21627,10 +21710,10 @@
       <c r="C162" s="8" t="s">
         <v>998</v>
       </c>
-      <c r="D162" s="10" t="s">
+      <c r="D162" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E162" s="10"/>
+      <c r="E162" s="12"/>
       <c r="F162" s="3" t="s">
         <v>999</v>
       </c>
@@ -21645,10 +21728,10 @@
       <c r="C163" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="D163" s="10" t="s">
+      <c r="D163" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E163" s="10"/>
+      <c r="E163" s="12"/>
       <c r="F163" s="8" t="s">
         <v>1001</v>
       </c>
@@ -21663,10 +21746,10 @@
       <c r="C164" s="8" t="s">
         <v>1002</v>
       </c>
-      <c r="D164" s="10" t="s">
+      <c r="D164" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E164" s="10"/>
+      <c r="E164" s="12"/>
       <c r="F164" s="8" t="s">
         <v>1003</v>
       </c>
@@ -21681,10 +21764,10 @@
       <c r="C165" s="8" t="s">
         <v>1005</v>
       </c>
-      <c r="D165" s="10" t="s">
+      <c r="D165" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E165" s="10"/>
+      <c r="E165" s="12"/>
       <c r="F165" s="9" t="s">
         <v>1017</v>
       </c>
@@ -21699,10 +21782,10 @@
       <c r="C166" s="8" t="s">
         <v>1006</v>
       </c>
-      <c r="D166" s="10" t="s">
+      <c r="D166" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E166" s="10"/>
+      <c r="E166" s="12"/>
       <c r="F166" s="9" t="s">
         <v>1007</v>
       </c>
@@ -21720,10 +21803,10 @@
       <c r="C167" s="9" t="s">
         <v>1014</v>
       </c>
-      <c r="D167" s="10" t="s">
+      <c r="D167" s="12" t="s">
         <v>1010</v>
       </c>
-      <c r="E167" s="10"/>
+      <c r="E167" s="12"/>
       <c r="F167" s="9" t="s">
         <v>1013</v>
       </c>
@@ -21738,10 +21821,10 @@
       <c r="C168" s="9" t="s">
         <v>1015</v>
       </c>
-      <c r="D168" s="10" t="s">
+      <c r="D168" s="12" t="s">
         <v>1012</v>
       </c>
-      <c r="E168" s="10"/>
+      <c r="E168" s="12"/>
       <c r="F168" s="9" t="s">
         <v>1016</v>
       </c>
@@ -21756,93 +21839,124 @@
       <c r="C169" s="9" t="s">
         <v>1009</v>
       </c>
-      <c r="D169" s="10" t="s">
+      <c r="D169" s="12" t="s">
         <v>1010</v>
       </c>
-      <c r="E169" s="10"/>
+      <c r="E169" s="12"/>
       <c r="F169" s="9" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="18" customHeight="1">
-      <c r="D170" s="10"/>
-      <c r="E170" s="10"/>
+      <c r="A170" s="10" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B170" s="1">
+        <v>6428</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D170" s="12" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E170" s="12"/>
+      <c r="F170" s="10" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G170" s="10" t="s">
+        <v>1022</v>
+      </c>
     </row>
     <row r="171" spans="1:7" ht="18" customHeight="1">
-      <c r="D171" s="10"/>
-      <c r="E171" s="10"/>
+      <c r="A171" s="11" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B171" s="1">
+        <v>6429</v>
+      </c>
+      <c r="C171" s="11" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D171" s="12" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E171" s="12"/>
+      <c r="F171" s="11" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="172" spans="1:7" ht="18" customHeight="1">
-      <c r="D172" s="10"/>
-      <c r="E172" s="10"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
     </row>
     <row r="173" spans="1:7" ht="18" customHeight="1">
-      <c r="D173" s="10"/>
-      <c r="E173" s="10"/>
+      <c r="D173" s="12"/>
+      <c r="E173" s="12"/>
     </row>
     <row r="174" spans="1:7" ht="18" customHeight="1">
-      <c r="D174" s="10"/>
-      <c r="E174" s="10"/>
+      <c r="D174" s="12"/>
+      <c r="E174" s="12"/>
     </row>
     <row r="175" spans="1:7" ht="18" customHeight="1">
-      <c r="D175" s="10"/>
-      <c r="E175" s="10"/>
+      <c r="D175" s="12"/>
+      <c r="E175" s="12"/>
     </row>
     <row r="176" spans="1:7" ht="18" customHeight="1">
-      <c r="D176" s="10"/>
-      <c r="E176" s="10"/>
+      <c r="D176" s="12"/>
+      <c r="E176" s="12"/>
     </row>
     <row r="177" spans="4:5" ht="18" customHeight="1">
-      <c r="D177" s="10"/>
-      <c r="E177" s="10"/>
+      <c r="D177" s="12"/>
+      <c r="E177" s="12"/>
     </row>
     <row r="178" spans="4:5" ht="18" customHeight="1">
-      <c r="D178" s="10"/>
-      <c r="E178" s="10"/>
+      <c r="D178" s="12"/>
+      <c r="E178" s="12"/>
     </row>
     <row r="179" spans="4:5" ht="18" customHeight="1">
-      <c r="D179" s="10"/>
-      <c r="E179" s="10"/>
+      <c r="D179" s="12"/>
+      <c r="E179" s="12"/>
     </row>
     <row r="180" spans="4:5" ht="18" customHeight="1">
-      <c r="D180" s="10"/>
-      <c r="E180" s="10"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
     </row>
     <row r="181" spans="4:5" ht="18" customHeight="1">
-      <c r="D181" s="10"/>
-      <c r="E181" s="10"/>
+      <c r="D181" s="12"/>
+      <c r="E181" s="12"/>
     </row>
     <row r="182" spans="4:5" ht="18" customHeight="1">
-      <c r="D182" s="10"/>
-      <c r="E182" s="10"/>
+      <c r="D182" s="12"/>
+      <c r="E182" s="12"/>
     </row>
     <row r="183" spans="4:5" ht="18" customHeight="1">
-      <c r="D183" s="10"/>
-      <c r="E183" s="10"/>
+      <c r="D183" s="12"/>
+      <c r="E183" s="12"/>
     </row>
     <row r="184" spans="4:5" ht="18" customHeight="1">
-      <c r="D184" s="10"/>
-      <c r="E184" s="10"/>
+      <c r="D184" s="12"/>
+      <c r="E184" s="12"/>
     </row>
     <row r="185" spans="4:5" ht="18" customHeight="1">
-      <c r="D185" s="10"/>
-      <c r="E185" s="10"/>
+      <c r="D185" s="12"/>
+      <c r="E185" s="12"/>
     </row>
     <row r="186" spans="4:5" ht="18" customHeight="1">
-      <c r="D186" s="10"/>
-      <c r="E186" s="10"/>
+      <c r="D186" s="12"/>
+      <c r="E186" s="12"/>
     </row>
     <row r="187" spans="4:5" ht="18" customHeight="1">
-      <c r="D187" s="10"/>
-      <c r="E187" s="10"/>
+      <c r="D187" s="12"/>
+      <c r="E187" s="12"/>
     </row>
     <row r="188" spans="4:5" ht="18" customHeight="1">
-      <c r="D188" s="10"/>
-      <c r="E188" s="10"/>
+      <c r="D188" s="12"/>
+      <c r="E188" s="12"/>
     </row>
     <row r="189" spans="4:5" ht="18" customHeight="1">
-      <c r="D189" s="10"/>
-      <c r="E189" s="10"/>
+      <c r="D189" s="12"/>
+      <c r="E189" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G169"/>

</xml_diff>

<commit_message>
add cf338e(unfinished) and cf878c
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="1041">
   <si>
     <t>OJ</t>
   </si>
@@ -12371,6 +12371,68 @@
   </si>
   <si>
     <t>数学</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>878C</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tournament</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>图论</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>并查集</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>链表</t>
+    </r>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -12473,7 +12535,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -12494,6 +12556,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -18800,8 +18865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G173" sqref="G173"/>
+    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
@@ -19254,10 +19319,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="14"/>
+      <c r="D26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="15"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -19275,10 +19340,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="14"/>
+      <c r="D27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="15"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -19296,10 +19361,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="14"/>
+      <c r="D28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="15"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -19317,10 +19382,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="14"/>
+      <c r="D29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="15"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -19338,10 +19403,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="14"/>
+      <c r="D30" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="15"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -19356,10 +19421,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="14"/>
+      <c r="D31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="15"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -19374,10 +19439,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="14"/>
+      <c r="D32" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="15"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -19392,10 +19457,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="14"/>
+      <c r="D33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="15"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -19413,10 +19478,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="15">
         <v>97</v>
       </c>
-      <c r="E34" s="14"/>
+      <c r="E34" s="15"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -19431,10 +19496,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="14"/>
+      <c r="D35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="15"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -19449,10 +19514,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="14"/>
+      <c r="D36" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="15"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -19467,10 +19532,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="14"/>
+      <c r="D37" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="15"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -19485,10 +19550,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="14"/>
+      <c r="D38" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="15"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -19506,10 +19571,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="14"/>
+      <c r="D39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="15"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -19527,10 +19592,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="14"/>
+      <c r="D40" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="15"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -19545,10 +19610,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="14"/>
+      <c r="D41" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="15"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -19566,10 +19631,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="14"/>
+      <c r="D42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="15"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -19584,10 +19649,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="14"/>
+      <c r="D43" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="15"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -19605,10 +19670,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="14"/>
+      <c r="D44" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="15"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -19623,10 +19688,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="14"/>
+      <c r="D45" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="15"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -19641,10 +19706,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="14"/>
+      <c r="D46" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="15"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -19659,10 +19724,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="14"/>
+      <c r="D47" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="15"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -19680,10 +19745,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="14"/>
+      <c r="D48" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="15"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -19698,10 +19763,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="14"/>
+      <c r="D49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="15"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -19719,10 +19784,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="14"/>
+      <c r="D50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="15"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -19740,10 +19805,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="14"/>
+      <c r="D51" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="15"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -19758,10 +19823,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="14"/>
+      <c r="D52" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="15"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -19776,10 +19841,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="14"/>
+      <c r="D53" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="15"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -19794,10 +19859,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="14"/>
+      <c r="D54" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="15"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -19812,10 +19877,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="14"/>
+      <c r="D55" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="15"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -19830,10 +19895,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="14"/>
+      <c r="D56" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="15"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -19848,10 +19913,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="14"/>
+      <c r="D57" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="15"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -19866,10 +19931,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="14"/>
+      <c r="D58" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="15"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -19884,10 +19949,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="14"/>
+      <c r="D59" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="15"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -19905,10 +19970,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="14"/>
+      <c r="D60" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="15"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -19923,10 +19988,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="14"/>
+      <c r="D61" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="15"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -19944,10 +20009,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="14"/>
+      <c r="D62" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="15"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -19962,10 +20027,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="14"/>
+      <c r="D63" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="15"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -19980,10 +20045,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="14"/>
+      <c r="D64" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="15"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -19998,10 +20063,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="14"/>
+      <c r="D65" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="15"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -20016,10 +20081,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="14"/>
+      <c r="D66" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="15"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -20034,10 +20099,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="14"/>
+      <c r="D67" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="15"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -20052,10 +20117,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="14"/>
+      <c r="D68" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="15"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -20070,10 +20135,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="14"/>
+      <c r="D69" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="15"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -20088,10 +20153,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="14"/>
+      <c r="D70" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="15"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -20106,10 +20171,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="14"/>
+      <c r="D71" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="15"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -20124,10 +20189,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="14"/>
+      <c r="D72" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="15"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -20142,10 +20207,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="14"/>
+      <c r="D73" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="15"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -20160,10 +20225,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="14"/>
+      <c r="D74" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="15"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -20178,10 +20243,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="14"/>
+      <c r="D75" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="15"/>
       <c r="F75" s="3" t="s">
         <v>821</v>
       </c>
@@ -20196,10 +20261,10 @@
       <c r="C76" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D76" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="14"/>
+      <c r="D76" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="15"/>
       <c r="F76" s="1" t="s">
         <v>822</v>
       </c>
@@ -20214,10 +20279,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="14"/>
+      <c r="D77" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="15"/>
       <c r="F77" s="1" t="s">
         <v>824</v>
       </c>
@@ -20232,10 +20297,10 @@
       <c r="C78" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="D78" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="14"/>
+      <c r="D78" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="15"/>
       <c r="F78" s="1" t="s">
         <v>826</v>
       </c>
@@ -20250,10 +20315,10 @@
       <c r="C79" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="D79" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="14"/>
+      <c r="D79" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="15"/>
       <c r="F79" s="1" t="s">
         <v>818</v>
       </c>
@@ -20268,10 +20333,10 @@
       <c r="C80" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="D80" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="14"/>
+      <c r="D80" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="15"/>
       <c r="F80" s="3" t="s">
         <v>566</v>
       </c>
@@ -20286,10 +20351,10 @@
       <c r="C81" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="D81" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="14"/>
+      <c r="D81" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="15"/>
       <c r="F81" s="3" t="s">
         <v>14</v>
       </c>
@@ -20304,10 +20369,10 @@
       <c r="C82" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="D82" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="14"/>
+      <c r="D82" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="15"/>
       <c r="F82" s="3" t="s">
         <v>831</v>
       </c>
@@ -20322,10 +20387,10 @@
       <c r="C83" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="D83" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="14"/>
+      <c r="D83" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="15"/>
       <c r="F83" s="1" t="s">
         <v>833</v>
       </c>
@@ -20340,10 +20405,10 @@
       <c r="C84" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D84" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="14"/>
+      <c r="D84" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="15"/>
       <c r="F84" s="3" t="s">
         <v>568</v>
       </c>
@@ -20358,10 +20423,10 @@
       <c r="C85" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="D85" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="14"/>
+      <c r="D85" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="15"/>
       <c r="F85" s="1" t="s">
         <v>836</v>
       </c>
@@ -20376,10 +20441,10 @@
       <c r="C86" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="D86" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="14"/>
+      <c r="D86" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="15"/>
       <c r="F86" s="1" t="s">
         <v>806</v>
       </c>
@@ -20394,10 +20459,10 @@
       <c r="C87" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D87" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="14"/>
+      <c r="D87" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="15"/>
       <c r="F87" s="3" t="s">
         <v>839</v>
       </c>
@@ -20412,10 +20477,10 @@
       <c r="C88" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="D88" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="14"/>
+      <c r="D88" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="15"/>
       <c r="F88" s="3" t="s">
         <v>841</v>
       </c>
@@ -20430,10 +20495,10 @@
       <c r="C89" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="D89" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="14"/>
+      <c r="D89" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="15"/>
       <c r="F89" s="1" t="s">
         <v>843</v>
       </c>
@@ -20448,10 +20513,10 @@
       <c r="C90" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="D90" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="14"/>
+      <c r="D90" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="15"/>
       <c r="F90" s="1" t="s">
         <v>845</v>
       </c>
@@ -20466,10 +20531,10 @@
       <c r="C91" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="D91" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="14"/>
+      <c r="D91" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="15"/>
       <c r="F91" s="3" t="s">
         <v>568</v>
       </c>
@@ -20484,10 +20549,10 @@
       <c r="C92" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="D92" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="14"/>
+      <c r="D92" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="15"/>
       <c r="F92" s="3" t="s">
         <v>568</v>
       </c>
@@ -20502,10 +20567,10 @@
       <c r="C93" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="D93" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="14"/>
+      <c r="D93" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="15"/>
       <c r="F93" s="3" t="s">
         <v>14</v>
       </c>
@@ -20520,10 +20585,10 @@
       <c r="C94" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D94" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="14"/>
+      <c r="D94" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="15"/>
       <c r="F94" s="1" t="s">
         <v>854</v>
       </c>
@@ -20538,10 +20603,10 @@
       <c r="C95" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="D95" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="14"/>
+      <c r="D95" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="15"/>
       <c r="F95" s="1" t="s">
         <v>162</v>
       </c>
@@ -20556,10 +20621,10 @@
       <c r="C96" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="D96" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="14"/>
+      <c r="D96" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="15"/>
       <c r="F96" s="3" t="s">
         <v>568</v>
       </c>
@@ -20574,10 +20639,10 @@
       <c r="C97" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="D97" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="14"/>
+      <c r="D97" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="15"/>
       <c r="F97" s="1" t="s">
         <v>859</v>
       </c>
@@ -20592,10 +20657,10 @@
       <c r="C98" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="D98" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="14"/>
+      <c r="D98" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="15"/>
       <c r="F98" s="3" t="s">
         <v>861</v>
       </c>
@@ -20610,10 +20675,10 @@
       <c r="C99" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="D99" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="14"/>
+      <c r="D99" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="15"/>
       <c r="F99" s="1" t="s">
         <v>863</v>
       </c>
@@ -20628,10 +20693,10 @@
       <c r="C100" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="D100" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="14"/>
+      <c r="D100" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="15"/>
       <c r="F100" s="1" t="s">
         <v>865</v>
       </c>
@@ -20646,10 +20711,10 @@
       <c r="C101" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="D101" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="14"/>
+      <c r="D101" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="15"/>
       <c r="F101" s="3" t="s">
         <v>568</v>
       </c>
@@ -20667,10 +20732,10 @@
       <c r="C102" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="D102" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="14"/>
+      <c r="D102" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="15"/>
       <c r="F102" s="3" t="s">
         <v>870</v>
       </c>
@@ -20688,10 +20753,10 @@
       <c r="C103" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D103" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="14"/>
+      <c r="D103" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="15"/>
       <c r="F103" s="3" t="s">
         <v>14</v>
       </c>
@@ -20706,10 +20771,10 @@
       <c r="C104" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="D104" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="14"/>
+      <c r="D104" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="15"/>
       <c r="F104" s="1" t="s">
         <v>875</v>
       </c>
@@ -20724,10 +20789,10 @@
       <c r="C105" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="D105" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="14"/>
+      <c r="D105" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="15"/>
       <c r="F105" s="1" t="s">
         <v>878</v>
       </c>
@@ -20742,10 +20807,10 @@
       <c r="C106" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="D106" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="14"/>
+      <c r="D106" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="15"/>
       <c r="F106" s="3" t="s">
         <v>14</v>
       </c>
@@ -20760,10 +20825,10 @@
       <c r="C107" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D107" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="14"/>
+      <c r="D107" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="15"/>
       <c r="F107" s="3" t="s">
         <v>882</v>
       </c>
@@ -20778,10 +20843,10 @@
       <c r="C108" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="D108" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="14"/>
+      <c r="D108" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="15"/>
       <c r="F108" s="1" t="s">
         <v>884</v>
       </c>
@@ -20796,10 +20861,10 @@
       <c r="C109" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="D109" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="14"/>
+      <c r="D109" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="15"/>
       <c r="F109" s="1" t="s">
         <v>886</v>
       </c>
@@ -20814,10 +20879,10 @@
       <c r="C110" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D110" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="14"/>
+      <c r="D110" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="15"/>
       <c r="F110" s="1" t="s">
         <v>162</v>
       </c>
@@ -20832,10 +20897,10 @@
       <c r="C111" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="D111" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="14"/>
+      <c r="D111" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="15"/>
       <c r="F111" s="3" t="s">
         <v>171</v>
       </c>
@@ -20850,10 +20915,10 @@
       <c r="C112" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D112" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="14"/>
+      <c r="D112" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="15"/>
       <c r="F112" s="1" t="s">
         <v>891</v>
       </c>
@@ -20871,10 +20936,10 @@
       <c r="C113" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="D113" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="14"/>
+      <c r="D113" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="15"/>
       <c r="F113" s="1" t="s">
         <v>893</v>
       </c>
@@ -20889,10 +20954,10 @@
       <c r="C114" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="D114" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="14"/>
+      <c r="D114" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="15"/>
       <c r="F114" s="3" t="s">
         <v>14</v>
       </c>
@@ -20907,10 +20972,10 @@
       <c r="C115" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="D115" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" s="14"/>
+      <c r="D115" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="15"/>
       <c r="F115" s="3" t="s">
         <v>14</v>
       </c>
@@ -20925,10 +20990,10 @@
       <c r="C116" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="D116" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" s="14"/>
+      <c r="D116" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="15"/>
       <c r="F116" s="3" t="s">
         <v>897</v>
       </c>
@@ -20943,10 +21008,10 @@
       <c r="C117" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="D117" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="14"/>
+      <c r="D117" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" s="15"/>
       <c r="F117" s="1" t="s">
         <v>900</v>
       </c>
@@ -20961,10 +21026,10 @@
       <c r="C118" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="D118" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="14"/>
+      <c r="D118" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="15"/>
       <c r="F118" s="1" t="s">
         <v>902</v>
       </c>
@@ -20979,10 +21044,10 @@
       <c r="C119" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="D119" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="14"/>
+      <c r="D119" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="15"/>
       <c r="F119" s="1" t="s">
         <v>905</v>
       </c>
@@ -20997,10 +21062,10 @@
       <c r="C120" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="D120" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E120" s="14"/>
+      <c r="D120" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="15"/>
       <c r="F120" s="2" t="s">
         <v>411</v>
       </c>
@@ -21015,10 +21080,10 @@
       <c r="C121" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="D121" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="14"/>
+      <c r="D121" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="15"/>
       <c r="F121" s="2" t="s">
         <v>234</v>
       </c>
@@ -21033,10 +21098,10 @@
       <c r="C122" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="D122" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="14"/>
+      <c r="D122" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="15"/>
       <c r="F122" s="3" t="s">
         <v>912</v>
       </c>
@@ -21051,10 +21116,10 @@
       <c r="C123" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="D123" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="14"/>
+      <c r="D123" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="15"/>
       <c r="F123" s="3" t="s">
         <v>915</v>
       </c>
@@ -21069,10 +21134,10 @@
       <c r="C124" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="D124" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="14"/>
+      <c r="D124" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="15"/>
       <c r="F124" s="1" t="s">
         <v>918</v>
       </c>
@@ -21087,10 +21152,10 @@
       <c r="C125" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="D125" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="14"/>
+      <c r="D125" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="15"/>
       <c r="F125" s="3" t="s">
         <v>422</v>
       </c>
@@ -21105,10 +21170,10 @@
       <c r="C126" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="D126" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="14"/>
+      <c r="D126" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="15"/>
       <c r="F126" s="3" t="s">
         <v>882</v>
       </c>
@@ -21123,10 +21188,10 @@
       <c r="C127" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D127" s="14" t="s">
+      <c r="D127" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E127" s="14"/>
+      <c r="E127" s="15"/>
       <c r="F127" s="1" t="s">
         <v>925</v>
       </c>
@@ -21141,10 +21206,10 @@
       <c r="C128" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D128" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E128" s="14"/>
+      <c r="D128" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="15"/>
       <c r="F128" s="3" t="s">
         <v>168</v>
       </c>
@@ -21159,10 +21224,10 @@
       <c r="C129" s="3" t="s">
         <v>926</v>
       </c>
-      <c r="D129" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E129" s="14"/>
+      <c r="D129" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="15"/>
       <c r="F129" s="1" t="s">
         <v>927</v>
       </c>
@@ -21177,10 +21242,10 @@
       <c r="C130" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="D130" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E130" s="14"/>
+      <c r="D130" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" s="15"/>
       <c r="F130" s="3" t="s">
         <v>171</v>
       </c>
@@ -21195,10 +21260,10 @@
       <c r="C131" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="D131" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" s="14"/>
+      <c r="D131" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="15"/>
       <c r="F131" s="3" t="s">
         <v>566</v>
       </c>
@@ -21213,10 +21278,10 @@
       <c r="C132" s="3" t="s">
         <v>930</v>
       </c>
-      <c r="D132" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E132" s="14"/>
+      <c r="D132" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="15"/>
       <c r="F132" s="1" t="s">
         <v>162</v>
       </c>
@@ -21231,10 +21296,10 @@
       <c r="C133" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="D133" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133" s="14"/>
+      <c r="D133" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="15"/>
       <c r="F133" s="1" t="s">
         <v>933</v>
       </c>
@@ -21249,10 +21314,10 @@
       <c r="C134" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="D134" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="14"/>
+      <c r="D134" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="15"/>
       <c r="F134" s="1" t="s">
         <v>936</v>
       </c>
@@ -21270,10 +21335,10 @@
       <c r="C135" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="D135" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="14"/>
+      <c r="D135" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" s="15"/>
       <c r="F135" s="1" t="s">
         <v>938</v>
       </c>
@@ -21288,10 +21353,10 @@
       <c r="C136" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D136" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" s="14"/>
+      <c r="D136" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" s="15"/>
       <c r="F136" s="1" t="s">
         <v>940</v>
       </c>
@@ -21306,10 +21371,10 @@
       <c r="C137" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D137" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E137" s="14"/>
+      <c r="D137" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" s="15"/>
       <c r="F137" s="1" t="s">
         <v>942</v>
       </c>
@@ -21324,10 +21389,10 @@
       <c r="C138" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D138" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="14"/>
+      <c r="D138" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="15"/>
       <c r="F138" s="1" t="s">
         <v>943</v>
       </c>
@@ -21342,10 +21407,10 @@
       <c r="C139" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="D139" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="14"/>
+      <c r="D139" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="15"/>
       <c r="F139" s="1" t="s">
         <v>826</v>
       </c>
@@ -21360,10 +21425,10 @@
       <c r="C140" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="D140" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E140" s="14"/>
+      <c r="D140" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" s="15"/>
       <c r="F140" s="4" t="s">
         <v>947</v>
       </c>
@@ -21378,10 +21443,10 @@
       <c r="C141" s="7" t="s">
         <v>955</v>
       </c>
-      <c r="D141" s="14" t="s">
+      <c r="D141" s="15" t="s">
         <v>950</v>
       </c>
-      <c r="E141" s="14"/>
+      <c r="E141" s="15"/>
       <c r="F141" s="7" t="s">
         <v>954</v>
       </c>
@@ -21396,10 +21461,10 @@
       <c r="C142" s="7" t="s">
         <v>956</v>
       </c>
-      <c r="D142" s="14" t="s">
+      <c r="D142" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E142" s="14"/>
+      <c r="E142" s="15"/>
       <c r="F142" s="7" t="s">
         <v>953</v>
       </c>
@@ -21414,10 +21479,10 @@
       <c r="C143" s="7" t="s">
         <v>958</v>
       </c>
-      <c r="D143" s="14" t="s">
+      <c r="D143" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E143" s="14"/>
+      <c r="E143" s="15"/>
       <c r="F143" s="7" t="s">
         <v>960</v>
       </c>
@@ -21432,10 +21497,10 @@
       <c r="C144" s="7" t="s">
         <v>961</v>
       </c>
-      <c r="D144" s="14" t="s">
+      <c r="D144" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E144" s="14"/>
+      <c r="E144" s="15"/>
       <c r="F144" s="7" t="s">
         <v>962</v>
       </c>
@@ -21453,10 +21518,10 @@
       <c r="C145" s="7" t="s">
         <v>964</v>
       </c>
-      <c r="D145" s="14" t="s">
+      <c r="D145" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E145" s="14"/>
+      <c r="E145" s="15"/>
       <c r="F145" s="3" t="s">
         <v>965</v>
       </c>
@@ -21471,10 +21536,10 @@
       <c r="C146" s="7" t="s">
         <v>966</v>
       </c>
-      <c r="D146" s="14" t="s">
+      <c r="D146" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E146" s="14"/>
+      <c r="E146" s="15"/>
       <c r="F146" s="3" t="s">
         <v>967</v>
       </c>
@@ -21489,10 +21554,10 @@
       <c r="C147" s="7" t="s">
         <v>968</v>
       </c>
-      <c r="D147" s="14" t="s">
+      <c r="D147" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E147" s="14"/>
+      <c r="E147" s="15"/>
       <c r="F147" s="7" t="s">
         <v>969</v>
       </c>
@@ -21510,10 +21575,10 @@
       <c r="C148" s="7" t="s">
         <v>970</v>
       </c>
-      <c r="D148" s="14" t="s">
+      <c r="D148" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E148" s="14"/>
+      <c r="E148" s="15"/>
       <c r="F148" s="7" t="s">
         <v>971</v>
       </c>
@@ -21531,10 +21596,10 @@
       <c r="C149" s="7" t="s">
         <v>972</v>
       </c>
-      <c r="D149" s="14" t="s">
+      <c r="D149" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E149" s="14"/>
+      <c r="E149" s="15"/>
       <c r="F149" s="7" t="s">
         <v>974</v>
       </c>
@@ -21549,10 +21614,10 @@
       <c r="C150" s="7" t="s">
         <v>973</v>
       </c>
-      <c r="D150" s="14" t="s">
+      <c r="D150" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E150" s="14"/>
+      <c r="E150" s="15"/>
       <c r="F150" s="7" t="s">
         <v>975</v>
       </c>
@@ -21567,10 +21632,10 @@
       <c r="C151" s="3" t="s">
         <v>976</v>
       </c>
-      <c r="D151" s="14" t="s">
+      <c r="D151" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E151" s="14"/>
+      <c r="E151" s="15"/>
       <c r="F151" s="7" t="s">
         <v>980</v>
       </c>
@@ -21585,10 +21650,10 @@
       <c r="C152" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="D152" s="14" t="s">
+      <c r="D152" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E152" s="14"/>
+      <c r="E152" s="15"/>
       <c r="F152" s="7" t="s">
         <v>981</v>
       </c>
@@ -21603,10 +21668,10 @@
       <c r="C153" s="7" t="s">
         <v>978</v>
       </c>
-      <c r="D153" s="14" t="s">
+      <c r="D153" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E153" s="14"/>
+      <c r="E153" s="15"/>
       <c r="F153" s="7" t="s">
         <v>982</v>
       </c>
@@ -21621,10 +21686,10 @@
       <c r="C154" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="D154" s="14" t="s">
+      <c r="D154" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E154" s="14"/>
+      <c r="E154" s="15"/>
       <c r="F154" s="7" t="s">
         <v>983</v>
       </c>
@@ -21639,10 +21704,10 @@
       <c r="C155" s="7" t="s">
         <v>984</v>
       </c>
-      <c r="D155" s="14" t="s">
+      <c r="D155" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E155" s="14"/>
+      <c r="E155" s="15"/>
       <c r="F155" s="7" t="s">
         <v>981</v>
       </c>
@@ -21657,10 +21722,10 @@
       <c r="C156" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="D156" s="14" t="s">
+      <c r="D156" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E156" s="14"/>
+      <c r="E156" s="15"/>
       <c r="F156" s="7" t="s">
         <v>986</v>
       </c>
@@ -21675,10 +21740,10 @@
       <c r="C157" s="7" t="s">
         <v>987</v>
       </c>
-      <c r="D157" s="14" t="s">
+      <c r="D157" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E157" s="14"/>
+      <c r="E157" s="15"/>
       <c r="F157" s="3" t="s">
         <v>988</v>
       </c>
@@ -21693,10 +21758,10 @@
       <c r="C158" s="7" t="s">
         <v>989</v>
       </c>
-      <c r="D158" s="14" t="s">
+      <c r="D158" s="15" t="s">
         <v>959</v>
       </c>
-      <c r="E158" s="14"/>
+      <c r="E158" s="15"/>
       <c r="F158" s="7" t="s">
         <v>983</v>
       </c>
@@ -21711,10 +21776,10 @@
       <c r="C159" s="8" t="s">
         <v>991</v>
       </c>
-      <c r="D159" s="14" t="s">
+      <c r="D159" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E159" s="14"/>
+      <c r="E159" s="15"/>
       <c r="F159" s="3" t="s">
         <v>995</v>
       </c>
@@ -21732,10 +21797,10 @@
       <c r="C160" s="8" t="s">
         <v>993</v>
       </c>
-      <c r="D160" s="14" t="s">
+      <c r="D160" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E160" s="14"/>
+      <c r="E160" s="15"/>
       <c r="F160" s="3" t="s">
         <v>996</v>
       </c>
@@ -21750,10 +21815,10 @@
       <c r="C161" s="8" t="s">
         <v>994</v>
       </c>
-      <c r="D161" s="14" t="s">
+      <c r="D161" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E161" s="14"/>
+      <c r="E161" s="15"/>
       <c r="F161" s="8" t="s">
         <v>997</v>
       </c>
@@ -21768,10 +21833,10 @@
       <c r="C162" s="8" t="s">
         <v>998</v>
       </c>
-      <c r="D162" s="14" t="s">
+      <c r="D162" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E162" s="14"/>
+      <c r="E162" s="15"/>
       <c r="F162" s="3" t="s">
         <v>999</v>
       </c>
@@ -21786,10 +21851,10 @@
       <c r="C163" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="D163" s="14" t="s">
+      <c r="D163" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E163" s="14"/>
+      <c r="E163" s="15"/>
       <c r="F163" s="8" t="s">
         <v>1001</v>
       </c>
@@ -21804,10 +21869,10 @@
       <c r="C164" s="8" t="s">
         <v>1002</v>
       </c>
-      <c r="D164" s="14" t="s">
+      <c r="D164" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E164" s="14"/>
+      <c r="E164" s="15"/>
       <c r="F164" s="8" t="s">
         <v>1003</v>
       </c>
@@ -21822,10 +21887,10 @@
       <c r="C165" s="8" t="s">
         <v>1005</v>
       </c>
-      <c r="D165" s="14" t="s">
+      <c r="D165" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E165" s="14"/>
+      <c r="E165" s="15"/>
       <c r="F165" s="9" t="s">
         <v>1017</v>
       </c>
@@ -21840,10 +21905,10 @@
       <c r="C166" s="8" t="s">
         <v>1006</v>
       </c>
-      <c r="D166" s="14" t="s">
+      <c r="D166" s="15" t="s">
         <v>992</v>
       </c>
-      <c r="E166" s="14"/>
+      <c r="E166" s="15"/>
       <c r="F166" s="9" t="s">
         <v>1007</v>
       </c>
@@ -21861,10 +21926,10 @@
       <c r="C167" s="9" t="s">
         <v>1014</v>
       </c>
-      <c r="D167" s="14" t="s">
+      <c r="D167" s="15" t="s">
         <v>1010</v>
       </c>
-      <c r="E167" s="14"/>
+      <c r="E167" s="15"/>
       <c r="F167" s="9" t="s">
         <v>1013</v>
       </c>
@@ -21879,10 +21944,10 @@
       <c r="C168" s="9" t="s">
         <v>1015</v>
       </c>
-      <c r="D168" s="14" t="s">
+      <c r="D168" s="15" t="s">
         <v>1012</v>
       </c>
-      <c r="E168" s="14"/>
+      <c r="E168" s="15"/>
       <c r="F168" s="9" t="s">
         <v>1016</v>
       </c>
@@ -21897,10 +21962,10 @@
       <c r="C169" s="9" t="s">
         <v>1009</v>
       </c>
-      <c r="D169" s="14" t="s">
+      <c r="D169" s="15" t="s">
         <v>1010</v>
       </c>
-      <c r="E169" s="14"/>
+      <c r="E169" s="15"/>
       <c r="F169" s="9" t="s">
         <v>1011</v>
       </c>
@@ -21915,10 +21980,10 @@
       <c r="C170" s="10" t="s">
         <v>1019</v>
       </c>
-      <c r="D170" s="14" t="s">
+      <c r="D170" s="15" t="s">
         <v>1020</v>
       </c>
-      <c r="E170" s="14"/>
+      <c r="E170" s="15"/>
       <c r="F170" s="10" t="s">
         <v>1021</v>
       </c>
@@ -21936,10 +22001,10 @@
       <c r="C171" s="11" t="s">
         <v>1024</v>
       </c>
-      <c r="D171" s="14" t="s">
+      <c r="D171" s="15" t="s">
         <v>1025</v>
       </c>
-      <c r="E171" s="14"/>
+      <c r="E171" s="15"/>
       <c r="F171" s="11" t="s">
         <v>1026</v>
       </c>
@@ -21954,10 +22019,10 @@
       <c r="C172" s="12" t="s">
         <v>1028</v>
       </c>
-      <c r="D172" s="14" t="s">
+      <c r="D172" s="15" t="s">
         <v>1029</v>
       </c>
-      <c r="E172" s="14"/>
+      <c r="E172" s="15"/>
       <c r="F172" s="12" t="s">
         <v>1030</v>
       </c>
@@ -21975,234 +22040,95 @@
       <c r="C173" s="13" t="s">
         <v>1033</v>
       </c>
-      <c r="D173" s="14" t="s">
+      <c r="D173" s="15" t="s">
         <v>1034</v>
       </c>
-      <c r="E173" s="14"/>
+      <c r="E173" s="15"/>
       <c r="F173" s="3" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="18" customHeight="1">
-      <c r="D174" s="14"/>
-      <c r="E174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B174" s="14" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C174" s="14" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D174" s="15" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E174" s="15"/>
+      <c r="F174" s="14" t="s">
+        <v>1040</v>
+      </c>
     </row>
     <row r="175" spans="1:7" ht="18" customHeight="1">
-      <c r="D175" s="14"/>
-      <c r="E175" s="14"/>
+      <c r="D175" s="15"/>
+      <c r="E175" s="15"/>
     </row>
     <row r="176" spans="1:7" ht="18" customHeight="1">
-      <c r="D176" s="14"/>
-      <c r="E176" s="14"/>
+      <c r="D176" s="15"/>
+      <c r="E176" s="15"/>
     </row>
     <row r="177" spans="4:5" ht="18" customHeight="1">
-      <c r="D177" s="14"/>
-      <c r="E177" s="14"/>
+      <c r="D177" s="15"/>
+      <c r="E177" s="15"/>
     </row>
     <row r="178" spans="4:5" ht="18" customHeight="1">
-      <c r="D178" s="14"/>
-      <c r="E178" s="14"/>
+      <c r="D178" s="15"/>
+      <c r="E178" s="15"/>
     </row>
     <row r="179" spans="4:5" ht="18" customHeight="1">
-      <c r="D179" s="14"/>
-      <c r="E179" s="14"/>
+      <c r="D179" s="15"/>
+      <c r="E179" s="15"/>
     </row>
     <row r="180" spans="4:5" ht="18" customHeight="1">
-      <c r="D180" s="14"/>
-      <c r="E180" s="14"/>
+      <c r="D180" s="15"/>
+      <c r="E180" s="15"/>
     </row>
     <row r="181" spans="4:5" ht="18" customHeight="1">
-      <c r="D181" s="14"/>
-      <c r="E181" s="14"/>
+      <c r="D181" s="15"/>
+      <c r="E181" s="15"/>
     </row>
     <row r="182" spans="4:5" ht="18" customHeight="1">
-      <c r="D182" s="14"/>
-      <c r="E182" s="14"/>
+      <c r="D182" s="15"/>
+      <c r="E182" s="15"/>
     </row>
     <row r="183" spans="4:5" ht="18" customHeight="1">
-      <c r="D183" s="14"/>
-      <c r="E183" s="14"/>
+      <c r="D183" s="15"/>
+      <c r="E183" s="15"/>
     </row>
     <row r="184" spans="4:5" ht="18" customHeight="1">
-      <c r="D184" s="14"/>
-      <c r="E184" s="14"/>
+      <c r="D184" s="15"/>
+      <c r="E184" s="15"/>
     </row>
     <row r="185" spans="4:5" ht="18" customHeight="1">
-      <c r="D185" s="14"/>
-      <c r="E185" s="14"/>
+      <c r="D185" s="15"/>
+      <c r="E185" s="15"/>
     </row>
     <row r="186" spans="4:5" ht="18" customHeight="1">
-      <c r="D186" s="14"/>
-      <c r="E186" s="14"/>
+      <c r="D186" s="15"/>
+      <c r="E186" s="15"/>
     </row>
     <row r="187" spans="4:5" ht="18" customHeight="1">
-      <c r="D187" s="14"/>
-      <c r="E187" s="14"/>
+      <c r="D187" s="15"/>
+      <c r="E187" s="15"/>
     </row>
     <row r="188" spans="4:5" ht="18" customHeight="1">
-      <c r="D188" s="14"/>
-      <c r="E188" s="14"/>
+      <c r="D188" s="15"/>
+      <c r="E188" s="15"/>
     </row>
     <row r="189" spans="4:5" ht="18" customHeight="1">
-      <c r="D189" s="14"/>
-      <c r="E189" s="14"/>
+      <c r="D189" s="15"/>
+      <c r="E189" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G169"/>
   <mergeCells count="164">
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -22214,6 +22140,159 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
add cf118c,agc009e and Zigzag MST
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19605" windowHeight="8595" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19605" windowHeight="8595" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2018寒假" sheetId="1" r:id="rId1"/>
     <sheet name="2018春季" sheetId="2" r:id="rId2"/>
     <sheet name="2018暑假" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="1036">
   <si>
     <t>OJ</t>
   </si>
@@ -12229,6 +12230,194 @@
         <charset val="134"/>
       </rPr>
       <t>均摊分析</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alkane</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>多项式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;Polya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>定理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生成函数</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>题号</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>名称</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>状态</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>标签</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>博客状态</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtCoder</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code Festival 2016 Final B</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zigzag MST</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>kruskal;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>118C</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fancy Numbers</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>贪心</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGC</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>009E</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eternal Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp</t>
     </r>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -12237,7 +12426,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="宋体"/>
@@ -12297,6 +12486,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Apple Garamond"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Apple Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -12335,7 +12539,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -12359,6 +12563,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -18642,9 +18858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="G176" sqref="G176"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="18" customHeight="1"/>
   <cols>
@@ -19096,10 +19310,10 @@
       <c r="C26" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="7"/>
+      <c r="D26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="F26" s="1" t="s">
         <v>728</v>
       </c>
@@ -19117,10 +19331,10 @@
       <c r="C27" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7"/>
+      <c r="D27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="1" t="s">
         <v>730</v>
       </c>
@@ -19138,10 +19352,10 @@
       <c r="C28" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="D28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="10"/>
       <c r="F28" s="1" t="s">
         <v>14</v>
       </c>
@@ -19159,10 +19373,10 @@
       <c r="C29" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="7"/>
+      <c r="D29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="10"/>
       <c r="F29" s="1" t="s">
         <v>735</v>
       </c>
@@ -19180,10 +19394,10 @@
       <c r="C30" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="7"/>
+      <c r="D30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="F30" s="1" t="s">
         <v>737</v>
       </c>
@@ -19198,10 +19412,10 @@
       <c r="C31" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="7"/>
+      <c r="D31" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="10"/>
       <c r="F31" s="1" t="s">
         <v>739</v>
       </c>
@@ -19216,10 +19430,10 @@
       <c r="C32" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="7"/>
+      <c r="D32" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="10"/>
       <c r="F32" s="1" t="s">
         <v>741</v>
       </c>
@@ -19234,10 +19448,10 @@
       <c r="C33" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="7"/>
+      <c r="D33" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="10"/>
       <c r="F33" s="1" t="s">
         <v>743</v>
       </c>
@@ -19255,10 +19469,10 @@
       <c r="C34" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="10">
         <v>97</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="1" t="s">
         <v>745</v>
       </c>
@@ -19273,10 +19487,10 @@
       <c r="C35" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="7"/>
+      <c r="D35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="F35" s="1" t="s">
         <v>747</v>
       </c>
@@ -19291,10 +19505,10 @@
       <c r="C36" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="7"/>
+      <c r="D36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10"/>
       <c r="F36" s="1" t="s">
         <v>701</v>
       </c>
@@ -19309,10 +19523,10 @@
       <c r="C37" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="7"/>
+      <c r="D37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="10"/>
       <c r="F37" s="1" t="s">
         <v>750</v>
       </c>
@@ -19327,10 +19541,10 @@
       <c r="C38" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="7"/>
+      <c r="D38" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="10"/>
       <c r="F38" s="1" t="s">
         <v>753</v>
       </c>
@@ -19348,10 +19562,10 @@
       <c r="C39" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="7"/>
+      <c r="D39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="10"/>
       <c r="F39" s="1" t="s">
         <v>755</v>
       </c>
@@ -19369,10 +19583,10 @@
       <c r="C40" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="7"/>
+      <c r="D40" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="10"/>
       <c r="F40" s="1" t="s">
         <v>756</v>
       </c>
@@ -19387,10 +19601,10 @@
       <c r="C41" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="7"/>
+      <c r="D41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="10"/>
       <c r="F41" s="1" t="s">
         <v>758</v>
       </c>
@@ -19408,10 +19622,10 @@
       <c r="C42" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="7"/>
+      <c r="D42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="10"/>
       <c r="F42" s="1" t="s">
         <v>760</v>
       </c>
@@ -19426,10 +19640,10 @@
       <c r="C43" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="7"/>
+      <c r="D43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="10"/>
       <c r="F43" s="1" t="s">
         <v>762</v>
       </c>
@@ -19447,10 +19661,10 @@
       <c r="C44" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="7"/>
+      <c r="D44" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="10"/>
       <c r="F44" s="1" t="s">
         <v>764</v>
       </c>
@@ -19465,10 +19679,10 @@
       <c r="C45" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="7"/>
+      <c r="D45" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="10"/>
       <c r="F45" s="1" t="s">
         <v>766</v>
       </c>
@@ -19483,10 +19697,10 @@
       <c r="C46" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="7"/>
+      <c r="D46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="10"/>
       <c r="F46" s="1" t="s">
         <v>767</v>
       </c>
@@ -19501,10 +19715,10 @@
       <c r="C47" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="7"/>
+      <c r="D47" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="10"/>
       <c r="F47" s="2" t="s">
         <v>769</v>
       </c>
@@ -19522,10 +19736,10 @@
       <c r="C48" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="7"/>
+      <c r="D48" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="10"/>
       <c r="F48" s="2" t="s">
         <v>771</v>
       </c>
@@ -19540,10 +19754,10 @@
       <c r="C49" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="7"/>
+      <c r="D49" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="10"/>
       <c r="F49" s="2" t="s">
         <v>773</v>
       </c>
@@ -19561,10 +19775,10 @@
       <c r="C50" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="7"/>
+      <c r="D50" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>775</v>
       </c>
@@ -19582,10 +19796,10 @@
       <c r="C51" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="7"/>
+      <c r="D51" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="10"/>
       <c r="F51" s="1" t="s">
         <v>777</v>
       </c>
@@ -19600,10 +19814,10 @@
       <c r="C52" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="7"/>
+      <c r="D52" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="10"/>
       <c r="F52" s="2" t="s">
         <v>779</v>
       </c>
@@ -19618,10 +19832,10 @@
       <c r="C53" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="7"/>
+      <c r="D53" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="10"/>
       <c r="F53" s="1" t="s">
         <v>781</v>
       </c>
@@ -19636,10 +19850,10 @@
       <c r="C54" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="7"/>
+      <c r="D54" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="10"/>
       <c r="F54" s="2" t="s">
         <v>783</v>
       </c>
@@ -19654,10 +19868,10 @@
       <c r="C55" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="7"/>
+      <c r="D55" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="10"/>
       <c r="F55" s="2" t="s">
         <v>785</v>
       </c>
@@ -19672,10 +19886,10 @@
       <c r="C56" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="7"/>
+      <c r="D56" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="10"/>
       <c r="F56" s="2" t="s">
         <v>783</v>
       </c>
@@ -19690,10 +19904,10 @@
       <c r="C57" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="7"/>
+      <c r="D57" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="10"/>
       <c r="F57" s="2" t="s">
         <v>788</v>
       </c>
@@ -19708,10 +19922,10 @@
       <c r="C58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="7"/>
+      <c r="D58" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="10"/>
       <c r="F58" s="1" t="s">
         <v>789</v>
       </c>
@@ -19726,10 +19940,10 @@
       <c r="C59" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="7"/>
+      <c r="D59" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="10"/>
       <c r="F59" s="1" t="s">
         <v>789</v>
       </c>
@@ -19747,10 +19961,10 @@
       <c r="C60" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="7"/>
+      <c r="D60" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="10"/>
       <c r="F60" s="1" t="s">
         <v>794</v>
       </c>
@@ -19765,10 +19979,10 @@
       <c r="C61" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="7"/>
+      <c r="D61" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="10"/>
       <c r="F61" s="1" t="s">
         <v>789</v>
       </c>
@@ -19786,10 +20000,10 @@
       <c r="C62" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="7"/>
+      <c r="D62" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="10"/>
       <c r="F62" s="1" t="s">
         <v>798</v>
       </c>
@@ -19804,10 +20018,10 @@
       <c r="C63" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="7"/>
+      <c r="D63" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="10"/>
       <c r="F63" s="1" t="s">
         <v>800</v>
       </c>
@@ -19822,10 +20036,10 @@
       <c r="C64" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="7"/>
+      <c r="D64" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="10"/>
       <c r="F64" s="3" t="s">
         <v>802</v>
       </c>
@@ -19840,10 +20054,10 @@
       <c r="C65" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="7"/>
+      <c r="D65" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="10"/>
       <c r="F65" s="1" t="s">
         <v>804</v>
       </c>
@@ -19858,10 +20072,10 @@
       <c r="C66" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="7"/>
+      <c r="D66" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="10"/>
       <c r="F66" s="1" t="s">
         <v>806</v>
       </c>
@@ -19876,10 +20090,10 @@
       <c r="C67" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="7"/>
+      <c r="D67" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="10"/>
       <c r="F67" s="1" t="s">
         <v>808</v>
       </c>
@@ -19894,10 +20108,10 @@
       <c r="C68" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="7"/>
+      <c r="D68" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="10"/>
       <c r="F68" s="3" t="s">
         <v>422</v>
       </c>
@@ -19912,10 +20126,10 @@
       <c r="C69" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="7"/>
+      <c r="D69" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="10"/>
       <c r="F69" s="1" t="s">
         <v>798</v>
       </c>
@@ -19930,10 +20144,10 @@
       <c r="C70" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="7"/>
+      <c r="D70" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="10"/>
       <c r="F70" s="3" t="s">
         <v>14</v>
       </c>
@@ -19948,10 +20162,10 @@
       <c r="C71" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="7"/>
+      <c r="D71" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="10"/>
       <c r="F71" s="1" t="s">
         <v>813</v>
       </c>
@@ -19966,10 +20180,10 @@
       <c r="C72" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="7"/>
+      <c r="D72" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="10"/>
       <c r="F72" s="3" t="s">
         <v>568</v>
       </c>
@@ -19984,10 +20198,10 @@
       <c r="C73" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="7"/>
+      <c r="D73" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="10"/>
       <c r="F73" s="1" t="s">
         <v>816</v>
       </c>
@@ -20002,10 +20216,10 @@
       <c r="C74" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="7"/>
+      <c r="D74" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="10"/>
       <c r="F74" s="1" t="s">
         <v>818</v>
       </c>
@@ -20020,10 +20234,10 @@
       <c r="C75" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="7"/>
+      <c r="D75" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="10"/>
       <c r="F75" s="3" t="s">
         <v>821</v>
       </c>
@@ -20038,10 +20252,10 @@
       <c r="C76" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="7"/>
+      <c r="D76" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="10"/>
       <c r="F76" s="1" t="s">
         <v>822</v>
       </c>
@@ -20056,10 +20270,10 @@
       <c r="C77" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="7"/>
+      <c r="D77" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="10"/>
       <c r="F77" s="1" t="s">
         <v>824</v>
       </c>
@@ -20074,10 +20288,10 @@
       <c r="C78" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="7"/>
+      <c r="D78" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="10"/>
       <c r="F78" s="1" t="s">
         <v>826</v>
       </c>
@@ -20092,10 +20306,10 @@
       <c r="C79" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="7"/>
+      <c r="D79" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="10"/>
       <c r="F79" s="1" t="s">
         <v>818</v>
       </c>
@@ -20110,10 +20324,10 @@
       <c r="C80" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="7"/>
+      <c r="D80" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="10"/>
       <c r="F80" s="3" t="s">
         <v>566</v>
       </c>
@@ -20128,10 +20342,10 @@
       <c r="C81" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="7"/>
+      <c r="D81" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="10"/>
       <c r="F81" s="3" t="s">
         <v>14</v>
       </c>
@@ -20146,10 +20360,10 @@
       <c r="C82" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="7"/>
+      <c r="D82" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="10"/>
       <c r="F82" s="3" t="s">
         <v>831</v>
       </c>
@@ -20164,10 +20378,10 @@
       <c r="C83" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="7"/>
+      <c r="D83" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="10"/>
       <c r="F83" s="1" t="s">
         <v>833</v>
       </c>
@@ -20182,10 +20396,10 @@
       <c r="C84" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="7"/>
+      <c r="D84" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="10"/>
       <c r="F84" s="3" t="s">
         <v>568</v>
       </c>
@@ -20200,10 +20414,10 @@
       <c r="C85" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="D85" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="7"/>
+      <c r="D85" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="10"/>
       <c r="F85" s="1" t="s">
         <v>836</v>
       </c>
@@ -20218,10 +20432,10 @@
       <c r="C86" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="7"/>
+      <c r="D86" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="10"/>
       <c r="F86" s="1" t="s">
         <v>806</v>
       </c>
@@ -20236,10 +20450,10 @@
       <c r="C87" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="7"/>
+      <c r="D87" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="10"/>
       <c r="F87" s="3" t="s">
         <v>839</v>
       </c>
@@ -20254,10 +20468,10 @@
       <c r="C88" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="7"/>
+      <c r="D88" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="10"/>
       <c r="F88" s="3" t="s">
         <v>841</v>
       </c>
@@ -20272,10 +20486,10 @@
       <c r="C89" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="D89" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="7"/>
+      <c r="D89" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="10"/>
       <c r="F89" s="1" t="s">
         <v>843</v>
       </c>
@@ -20290,10 +20504,10 @@
       <c r="C90" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="7"/>
+      <c r="D90" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="10"/>
       <c r="F90" s="1" t="s">
         <v>845</v>
       </c>
@@ -20308,10 +20522,10 @@
       <c r="C91" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="7"/>
+      <c r="D91" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="10"/>
       <c r="F91" s="3" t="s">
         <v>568</v>
       </c>
@@ -20326,10 +20540,10 @@
       <c r="C92" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="7"/>
+      <c r="D92" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="10"/>
       <c r="F92" s="3" t="s">
         <v>568</v>
       </c>
@@ -20344,10 +20558,10 @@
       <c r="C93" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="7"/>
+      <c r="D93" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="10"/>
       <c r="F93" s="3" t="s">
         <v>14</v>
       </c>
@@ -20362,10 +20576,10 @@
       <c r="C94" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D94" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="7"/>
+      <c r="D94" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="10"/>
       <c r="F94" s="1" t="s">
         <v>854</v>
       </c>
@@ -20380,10 +20594,10 @@
       <c r="C95" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="D95" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="7"/>
+      <c r="D95" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="10"/>
       <c r="F95" s="1" t="s">
         <v>162</v>
       </c>
@@ -20398,10 +20612,10 @@
       <c r="C96" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="D96" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="7"/>
+      <c r="D96" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="10"/>
       <c r="F96" s="3" t="s">
         <v>568</v>
       </c>
@@ -20416,10 +20630,10 @@
       <c r="C97" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="D97" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="7"/>
+      <c r="D97" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="10"/>
       <c r="F97" s="1" t="s">
         <v>859</v>
       </c>
@@ -20434,10 +20648,10 @@
       <c r="C98" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="7"/>
+      <c r="D98" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="10"/>
       <c r="F98" s="3" t="s">
         <v>861</v>
       </c>
@@ -20452,10 +20666,10 @@
       <c r="C99" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="D99" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="7"/>
+      <c r="D99" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="10"/>
       <c r="F99" s="1" t="s">
         <v>863</v>
       </c>
@@ -20470,10 +20684,10 @@
       <c r="C100" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="7"/>
+      <c r="D100" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="10"/>
       <c r="F100" s="1" t="s">
         <v>865</v>
       </c>
@@ -20488,10 +20702,10 @@
       <c r="C101" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="D101" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="7"/>
+      <c r="D101" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="10"/>
       <c r="F101" s="3" t="s">
         <v>568</v>
       </c>
@@ -20509,10 +20723,10 @@
       <c r="C102" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="7"/>
+      <c r="D102" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="10"/>
       <c r="F102" s="3" t="s">
         <v>870</v>
       </c>
@@ -20530,10 +20744,10 @@
       <c r="C103" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="7"/>
+      <c r="D103" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="10"/>
       <c r="F103" s="3" t="s">
         <v>14</v>
       </c>
@@ -20548,10 +20762,10 @@
       <c r="C104" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="7"/>
+      <c r="D104" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" s="10"/>
       <c r="F104" s="1" t="s">
         <v>875</v>
       </c>
@@ -20566,10 +20780,10 @@
       <c r="C105" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="7"/>
+      <c r="D105" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="10"/>
       <c r="F105" s="1" t="s">
         <v>878</v>
       </c>
@@ -20584,10 +20798,10 @@
       <c r="C106" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="7"/>
+      <c r="D106" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="10"/>
       <c r="F106" s="3" t="s">
         <v>14</v>
       </c>
@@ -20602,10 +20816,10 @@
       <c r="C107" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D107" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="7"/>
+      <c r="D107" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" s="10"/>
       <c r="F107" s="3" t="s">
         <v>882</v>
       </c>
@@ -20620,10 +20834,10 @@
       <c r="C108" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="D108" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="7"/>
+      <c r="D108" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="10"/>
       <c r="F108" s="1" t="s">
         <v>884</v>
       </c>
@@ -20638,10 +20852,10 @@
       <c r="C109" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="D109" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="7"/>
+      <c r="D109" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="10"/>
       <c r="F109" s="1" t="s">
         <v>886</v>
       </c>
@@ -20656,10 +20870,10 @@
       <c r="C110" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D110" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="7"/>
+      <c r="D110" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" s="10"/>
       <c r="F110" s="1" t="s">
         <v>162</v>
       </c>
@@ -20674,10 +20888,10 @@
       <c r="C111" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="D111" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="7"/>
+      <c r="D111" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="10"/>
       <c r="F111" s="3" t="s">
         <v>171</v>
       </c>
@@ -20692,10 +20906,10 @@
       <c r="C112" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="D112" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="7"/>
+      <c r="D112" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" s="10"/>
       <c r="F112" s="1" t="s">
         <v>891</v>
       </c>
@@ -20713,10 +20927,10 @@
       <c r="C113" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="7"/>
+      <c r="D113" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="10"/>
       <c r="F113" s="1" t="s">
         <v>893</v>
       </c>
@@ -20731,10 +20945,10 @@
       <c r="C114" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" s="7"/>
+      <c r="D114" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="10"/>
       <c r="F114" s="3" t="s">
         <v>14</v>
       </c>
@@ -20749,10 +20963,10 @@
       <c r="C115" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="D115" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E115" s="7"/>
+      <c r="D115" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="10"/>
       <c r="F115" s="3" t="s">
         <v>14</v>
       </c>
@@ -20767,10 +20981,10 @@
       <c r="C116" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="D116" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E116" s="7"/>
+      <c r="D116" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="10"/>
       <c r="F116" s="3" t="s">
         <v>897</v>
       </c>
@@ -20785,10 +20999,10 @@
       <c r="C117" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="D117" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E117" s="7"/>
+      <c r="D117" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" s="10"/>
       <c r="F117" s="1" t="s">
         <v>900</v>
       </c>
@@ -20803,10 +21017,10 @@
       <c r="C118" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="D118" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="7"/>
+      <c r="D118" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="10"/>
       <c r="F118" s="1" t="s">
         <v>902</v>
       </c>
@@ -20821,10 +21035,10 @@
       <c r="C119" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="D119" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E119" s="7"/>
+      <c r="D119" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" s="10"/>
       <c r="F119" s="1" t="s">
         <v>905</v>
       </c>
@@ -20839,10 +21053,10 @@
       <c r="C120" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="D120" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E120" s="7"/>
+      <c r="D120" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="10"/>
       <c r="F120" s="2" t="s">
         <v>411</v>
       </c>
@@ -20857,10 +21071,10 @@
       <c r="C121" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="D121" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E121" s="7"/>
+      <c r="D121" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" s="10"/>
       <c r="F121" s="2" t="s">
         <v>234</v>
       </c>
@@ -20875,10 +21089,10 @@
       <c r="C122" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="D122" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="7"/>
+      <c r="D122" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="10"/>
       <c r="F122" s="3" t="s">
         <v>912</v>
       </c>
@@ -20893,10 +21107,10 @@
       <c r="C123" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="D123" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E123" s="7"/>
+      <c r="D123" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="10"/>
       <c r="F123" s="3" t="s">
         <v>915</v>
       </c>
@@ -20911,10 +21125,10 @@
       <c r="C124" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="D124" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E124" s="7"/>
+      <c r="D124" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="10"/>
       <c r="F124" s="1" t="s">
         <v>918</v>
       </c>
@@ -20929,10 +21143,10 @@
       <c r="C125" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="D125" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E125" s="7"/>
+      <c r="D125" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="10"/>
       <c r="F125" s="3" t="s">
         <v>422</v>
       </c>
@@ -20947,10 +21161,10 @@
       <c r="C126" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="D126" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E126" s="7"/>
+      <c r="D126" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="10"/>
       <c r="F126" s="3" t="s">
         <v>882</v>
       </c>
@@ -20965,10 +21179,10 @@
       <c r="C127" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D127" s="7" t="s">
+      <c r="D127" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E127" s="7"/>
+      <c r="E127" s="10"/>
       <c r="F127" s="1" t="s">
         <v>925</v>
       </c>
@@ -20983,10 +21197,10 @@
       <c r="C128" s="1" t="s">
         <v>924</v>
       </c>
-      <c r="D128" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E128" s="7"/>
+      <c r="D128" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="10"/>
       <c r="F128" s="3" t="s">
         <v>168</v>
       </c>
@@ -21001,10 +21215,10 @@
       <c r="C129" s="3" t="s">
         <v>926</v>
       </c>
-      <c r="D129" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E129" s="7"/>
+      <c r="D129" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="10"/>
       <c r="F129" s="1" t="s">
         <v>927</v>
       </c>
@@ -21019,10 +21233,10 @@
       <c r="C130" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="D130" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E130" s="7"/>
+      <c r="D130" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" s="10"/>
       <c r="F130" s="3" t="s">
         <v>171</v>
       </c>
@@ -21037,10 +21251,10 @@
       <c r="C131" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="D131" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E131" s="7"/>
+      <c r="D131" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="10"/>
       <c r="F131" s="3" t="s">
         <v>566</v>
       </c>
@@ -21055,10 +21269,10 @@
       <c r="C132" s="3" t="s">
         <v>930</v>
       </c>
-      <c r="D132" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E132" s="7"/>
+      <c r="D132" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="10"/>
       <c r="F132" s="1" t="s">
         <v>162</v>
       </c>
@@ -21073,10 +21287,10 @@
       <c r="C133" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="D133" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E133" s="7"/>
+      <c r="D133" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="10"/>
       <c r="F133" s="1" t="s">
         <v>933</v>
       </c>
@@ -21091,10 +21305,10 @@
       <c r="C134" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="D134" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E134" s="7"/>
+      <c r="D134" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="10"/>
       <c r="F134" s="1" t="s">
         <v>936</v>
       </c>
@@ -21112,10 +21326,10 @@
       <c r="C135" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="D135" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E135" s="7"/>
+      <c r="D135" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" s="10"/>
       <c r="F135" s="1" t="s">
         <v>938</v>
       </c>
@@ -21130,10 +21344,10 @@
       <c r="C136" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D136" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E136" s="7"/>
+      <c r="D136" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" s="10"/>
       <c r="F136" s="1" t="s">
         <v>940</v>
       </c>
@@ -21148,10 +21362,10 @@
       <c r="C137" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D137" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E137" s="7"/>
+      <c r="D137" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" s="10"/>
       <c r="F137" s="1" t="s">
         <v>942</v>
       </c>
@@ -21166,10 +21380,10 @@
       <c r="C138" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D138" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="7"/>
+      <c r="D138" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="10"/>
       <c r="F138" s="1" t="s">
         <v>943</v>
       </c>
@@ -21184,10 +21398,10 @@
       <c r="C139" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="D139" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E139" s="7"/>
+      <c r="D139" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="10"/>
       <c r="F139" s="1" t="s">
         <v>826</v>
       </c>
@@ -21202,10 +21416,10 @@
       <c r="C140" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="D140" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E140" s="7"/>
+      <c r="D140" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" s="10"/>
       <c r="F140" s="3" t="s">
         <v>947</v>
       </c>
@@ -21220,10 +21434,10 @@
       <c r="C141" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="D141" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E141" s="7"/>
+      <c r="D141" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E141" s="10"/>
       <c r="F141" s="1" t="s">
         <v>950</v>
       </c>
@@ -21238,10 +21452,10 @@
       <c r="C142" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="D142" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E142" s="7"/>
+      <c r="D142" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E142" s="10"/>
       <c r="F142" s="1" t="s">
         <v>950</v>
       </c>
@@ -21256,10 +21470,10 @@
       <c r="C143" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="D143" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E143" s="7"/>
+      <c r="D143" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E143" s="10"/>
       <c r="F143" s="1" t="s">
         <v>953</v>
       </c>
@@ -21274,10 +21488,10 @@
       <c r="C144" s="1" t="s">
         <v>954</v>
       </c>
-      <c r="D144" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E144" s="7"/>
+      <c r="D144" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E144" s="10"/>
       <c r="F144" s="1" t="s">
         <v>955</v>
       </c>
@@ -21295,10 +21509,10 @@
       <c r="C145" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="D145" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E145" s="7"/>
+      <c r="D145" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E145" s="10"/>
       <c r="F145" s="3" t="s">
         <v>957</v>
       </c>
@@ -21313,10 +21527,10 @@
       <c r="C146" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="D146" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E146" s="7"/>
+      <c r="D146" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E146" s="10"/>
       <c r="F146" s="3" t="s">
         <v>568</v>
       </c>
@@ -21331,10 +21545,10 @@
       <c r="C147" s="1" t="s">
         <v>959</v>
       </c>
-      <c r="D147" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E147" s="7"/>
+      <c r="D147" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E147" s="10"/>
       <c r="F147" s="1" t="s">
         <v>960</v>
       </c>
@@ -21352,10 +21566,10 @@
       <c r="C148" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="D148" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E148" s="7"/>
+      <c r="D148" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E148" s="10"/>
       <c r="F148" s="1" t="s">
         <v>962</v>
       </c>
@@ -21373,10 +21587,10 @@
       <c r="C149" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="D149" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E149" s="7"/>
+      <c r="D149" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E149" s="10"/>
       <c r="F149" s="1" t="s">
         <v>964</v>
       </c>
@@ -21391,10 +21605,10 @@
       <c r="C150" s="1" t="s">
         <v>965</v>
       </c>
-      <c r="D150" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E150" s="7"/>
+      <c r="D150" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E150" s="10"/>
       <c r="F150" s="1" t="s">
         <v>966</v>
       </c>
@@ -21409,10 +21623,10 @@
       <c r="C151" s="3" t="s">
         <v>967</v>
       </c>
-      <c r="D151" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E151" s="7"/>
+      <c r="D151" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E151" s="10"/>
       <c r="F151" s="1" t="s">
         <v>968</v>
       </c>
@@ -21427,10 +21641,10 @@
       <c r="C152" s="3" t="s">
         <v>969</v>
       </c>
-      <c r="D152" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E152" s="7"/>
+      <c r="D152" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152" s="10"/>
       <c r="F152" s="1" t="s">
         <v>162</v>
       </c>
@@ -21445,10 +21659,10 @@
       <c r="C153" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="D153" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E153" s="7"/>
+      <c r="D153" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153" s="10"/>
       <c r="F153" s="1" t="s">
         <v>971</v>
       </c>
@@ -21463,10 +21677,10 @@
       <c r="C154" s="3" t="s">
         <v>972</v>
       </c>
-      <c r="D154" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E154" s="7"/>
+      <c r="D154" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E154" s="10"/>
       <c r="F154" s="1" t="s">
         <v>798</v>
       </c>
@@ -21481,10 +21695,10 @@
       <c r="C155" s="1" t="s">
         <v>973</v>
       </c>
-      <c r="D155" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E155" s="7"/>
+      <c r="D155" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E155" s="10"/>
       <c r="F155" s="1" t="s">
         <v>162</v>
       </c>
@@ -21499,10 +21713,10 @@
       <c r="C156" s="1" t="s">
         <v>974</v>
       </c>
-      <c r="D156" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E156" s="7"/>
+      <c r="D156" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E156" s="10"/>
       <c r="F156" s="1" t="s">
         <v>806</v>
       </c>
@@ -21517,10 +21731,10 @@
       <c r="C157" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="D157" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E157" s="7"/>
+      <c r="D157" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E157" s="10"/>
       <c r="F157" s="3" t="s">
         <v>976</v>
       </c>
@@ -21535,10 +21749,10 @@
       <c r="C158" s="1" t="s">
         <v>977</v>
       </c>
-      <c r="D158" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E158" s="7"/>
+      <c r="D158" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158" s="10"/>
       <c r="F158" s="1" t="s">
         <v>798</v>
       </c>
@@ -21553,10 +21767,10 @@
       <c r="C159" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="D159" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E159" s="7"/>
+      <c r="D159" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E159" s="10"/>
       <c r="F159" s="3" t="s">
         <v>979</v>
       </c>
@@ -21574,10 +21788,10 @@
       <c r="C160" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="D160" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E160" s="7"/>
+      <c r="D160" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E160" s="10"/>
       <c r="F160" s="3" t="s">
         <v>14</v>
       </c>
@@ -21592,10 +21806,10 @@
       <c r="C161" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="D161" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E161" s="7"/>
+      <c r="D161" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161" s="10"/>
       <c r="F161" s="1" t="s">
         <v>982</v>
       </c>
@@ -21610,10 +21824,10 @@
       <c r="C162" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="D162" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E162" s="7"/>
+      <c r="D162" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162" s="10"/>
       <c r="F162" s="3" t="s">
         <v>566</v>
       </c>
@@ -21628,10 +21842,10 @@
       <c r="C163" s="3" t="s">
         <v>984</v>
       </c>
-      <c r="D163" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E163" s="7"/>
+      <c r="D163" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163" s="10"/>
       <c r="F163" s="1" t="s">
         <v>985</v>
       </c>
@@ -21646,10 +21860,10 @@
       <c r="C164" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="D164" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E164" s="7"/>
+      <c r="D164" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E164" s="10"/>
       <c r="F164" s="1" t="s">
         <v>987</v>
       </c>
@@ -21664,10 +21878,10 @@
       <c r="C165" s="1" t="s">
         <v>988</v>
       </c>
-      <c r="D165" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E165" s="7"/>
+      <c r="D165" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E165" s="10"/>
       <c r="F165" s="1" t="s">
         <v>989</v>
       </c>
@@ -21682,10 +21896,10 @@
       <c r="C166" s="1" t="s">
         <v>990</v>
       </c>
-      <c r="D166" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E166" s="7"/>
+      <c r="D166" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166" s="10"/>
       <c r="F166" s="1" t="s">
         <v>991</v>
       </c>
@@ -21703,10 +21917,10 @@
       <c r="C167" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="D167" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E167" s="7"/>
+      <c r="D167" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167" s="10"/>
       <c r="F167" s="1" t="s">
         <v>993</v>
       </c>
@@ -21721,10 +21935,10 @@
       <c r="C168" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="D168" s="7" t="s">
+      <c r="D168" s="10" t="s">
         <v>619</v>
       </c>
-      <c r="E168" s="7"/>
+      <c r="E168" s="10"/>
       <c r="F168" s="1" t="s">
         <v>994</v>
       </c>
@@ -21739,10 +21953,10 @@
       <c r="C169" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="D169" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E169" s="7"/>
+      <c r="D169" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169" s="10"/>
       <c r="F169" s="1" t="s">
         <v>996</v>
       </c>
@@ -21757,10 +21971,10 @@
       <c r="C170" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="D170" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E170" s="7"/>
+      <c r="D170" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E170" s="10"/>
       <c r="F170" s="1" t="s">
         <v>998</v>
       </c>
@@ -21778,10 +21992,10 @@
       <c r="C171" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="D171" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E171" s="7"/>
+      <c r="D171" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171" s="10"/>
       <c r="F171" s="1" t="s">
         <v>798</v>
       </c>
@@ -21796,10 +22010,10 @@
       <c r="C172" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="D172" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E172" s="7"/>
+      <c r="D172" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172" s="10"/>
       <c r="F172" s="1" t="s">
         <v>1001</v>
       </c>
@@ -21817,10 +22031,10 @@
       <c r="C173" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="D173" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E173" s="7"/>
+      <c r="D173" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E173" s="10"/>
       <c r="F173" s="3" t="s">
         <v>575</v>
       </c>
@@ -21835,10 +22049,10 @@
       <c r="C174" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="D174" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E174" s="7"/>
+      <c r="D174" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E174" s="10"/>
       <c r="F174" s="1" t="s">
         <v>1005</v>
       </c>
@@ -21853,10 +22067,10 @@
       <c r="C175" s="1" t="s">
         <v>1007</v>
       </c>
-      <c r="D175" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E175" s="7"/>
+      <c r="D175" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E175" s="10"/>
       <c r="F175" s="3" t="s">
         <v>1008</v>
       </c>
@@ -21874,65 +22088,79 @@
       <c r="C176" s="6" t="s">
         <v>1012</v>
       </c>
-      <c r="D176" s="7" t="s">
+      <c r="D176" s="10" t="s">
         <v>1013</v>
       </c>
-      <c r="E176" s="7"/>
+      <c r="E176" s="10"/>
       <c r="F176" s="6" t="s">
         <v>1014</v>
       </c>
     </row>
-    <row r="177" spans="4:5" ht="18" customHeight="1">
-      <c r="D177" s="7"/>
-      <c r="E177" s="7"/>
-    </row>
-    <row r="178" spans="4:5" ht="18" customHeight="1">
-      <c r="D178" s="7"/>
-      <c r="E178" s="7"/>
-    </row>
-    <row r="179" spans="4:5" ht="18" customHeight="1">
-      <c r="D179" s="7"/>
-      <c r="E179" s="7"/>
-    </row>
-    <row r="180" spans="4:5" ht="18" customHeight="1">
-      <c r="D180" s="7"/>
-      <c r="E180" s="7"/>
-    </row>
-    <row r="181" spans="4:5" ht="18" customHeight="1">
-      <c r="D181" s="7"/>
-      <c r="E181" s="7"/>
-    </row>
-    <row r="182" spans="4:5" ht="18" customHeight="1">
-      <c r="D182" s="7"/>
-      <c r="E182" s="7"/>
-    </row>
-    <row r="183" spans="4:5" ht="18" customHeight="1">
-      <c r="D183" s="7"/>
-      <c r="E183" s="7"/>
-    </row>
-    <row r="184" spans="4:5" ht="18" customHeight="1">
-      <c r="D184" s="7"/>
-      <c r="E184" s="7"/>
-    </row>
-    <row r="185" spans="4:5" ht="18" customHeight="1">
-      <c r="D185" s="7"/>
-      <c r="E185" s="7"/>
-    </row>
-    <row r="186" spans="4:5" ht="18" customHeight="1">
-      <c r="D186" s="7"/>
-      <c r="E186" s="7"/>
-    </row>
-    <row r="187" spans="4:5" ht="18" customHeight="1">
-      <c r="D187" s="7"/>
-      <c r="E187" s="7"/>
-    </row>
-    <row r="188" spans="4:5" ht="18" customHeight="1">
-      <c r="D188" s="7"/>
-      <c r="E188" s="7"/>
-    </row>
-    <row r="189" spans="4:5" ht="18" customHeight="1">
-      <c r="D189" s="7"/>
-      <c r="E189" s="7"/>
+    <row r="177" spans="1:6" ht="18" customHeight="1">
+      <c r="A177" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B177" s="1">
+        <v>6426</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D177" s="10" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E177" s="10"/>
+      <c r="F177" s="7" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="18" customHeight="1">
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
+    </row>
+    <row r="179" spans="1:6" ht="18" customHeight="1">
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
+    </row>
+    <row r="180" spans="1:6" ht="18" customHeight="1">
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
+    </row>
+    <row r="181" spans="1:6" ht="18" customHeight="1">
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
+    </row>
+    <row r="182" spans="1:6" ht="18" customHeight="1">
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
+    </row>
+    <row r="183" spans="1:6" ht="18" customHeight="1">
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
+    </row>
+    <row r="184" spans="1:6" ht="18" customHeight="1">
+      <c r="D184" s="10"/>
+      <c r="E184" s="10"/>
+    </row>
+    <row r="185" spans="1:6" ht="18" customHeight="1">
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
+    </row>
+    <row r="186" spans="1:6" ht="18" customHeight="1">
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
+    </row>
+    <row r="187" spans="1:6" ht="18" customHeight="1">
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
+    </row>
+    <row r="188" spans="1:6" ht="18" customHeight="1">
+      <c r="D188" s="10"/>
+      <c r="E188" s="10"/>
+    </row>
+    <row r="189" spans="1:6" ht="18" customHeight="1">
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G174"/>
@@ -22106,4 +22334,100 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="9"/>
+    <col min="2" max="2" width="35.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="9"/>
+    <col min="5" max="5" width="33.140625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="17.7109375" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="9" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="9" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add cf1045c and cf1045i
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19605" windowHeight="8595" tabRatio="500" activeTab="3"/>
+    <workbookView windowWidth="19605" windowHeight="8595" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2018寒假" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076">
   <si>
     <t>OJ</t>
   </si>
@@ -12315,6 +12315,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>复杂度分析</t>
     </r>
     <r>
@@ -12351,6 +12356,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>思维</t>
     </r>
     <r>
@@ -12364,9 +12374,38 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>搜索</t>
+    </r>
+  </si>
+  <si>
+    <t>1045C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyperspace Highways </t>
+  </si>
+  <si>
+    <t>圆方树</t>
+  </si>
+  <si>
+    <t>1045I</t>
+  </si>
+  <si>
+    <t>Palindrome Pairs</t>
+  </si>
+  <si>
+    <r>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;map</t>
     </r>
   </si>
 </sst>
@@ -12375,9 +12414,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
@@ -12427,14 +12466,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -12452,7 +12483,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12460,7 +12491,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12473,15 +12504,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -12496,31 +12520,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12535,28 +12537,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12569,16 +12610,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="14"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -12593,19 +12632,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12617,25 +12650,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12647,13 +12674,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12671,85 +12734,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12767,13 +12752,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12784,21 +12823,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -12826,26 +12850,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -12861,11 +12865,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12884,6 +12905,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -12895,169 +12934,169 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -13098,8 +13137,8 @@
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 6" xfId="1"/>
-    <cellStyle name="常规 9" xfId="2"/>
+    <cellStyle name="常规 9" xfId="1"/>
+    <cellStyle name="常规 6" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -14181,8 +14220,8 @@
   <sheetPr/>
   <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="D256" sqref="D256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="5"/>
@@ -22729,10 +22768,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -23036,7 +23075,7 @@
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>1063</v>
       </c>
     </row>
@@ -23053,7 +23092,7 @@
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>1066</v>
       </c>
     </row>
@@ -23070,7 +23109,7 @@
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>566</v>
       </c>
     </row>
@@ -23087,8 +23126,42 @@
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>1069</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>1075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cf1045a,cf1045h and uva1063
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2506" uniqueCount="1101">
   <si>
     <t>OJ</t>
   </si>
@@ -12356,9 +12356,6 @@
   </si>
   <si>
     <t>AtCoder</t>
-  </si>
-  <si>
-    <t>Code Festival 2016 Final B</t>
   </si>
   <si>
     <t>Zigzag MST</t>
@@ -12976,6 +12973,133 @@
         <family val="1"/>
       </rPr>
       <t>dp</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>1045H</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-exploration</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>组合数学</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code Festival 2016 Final G</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>1045A</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last Chance</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uva</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marble Games</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索;大模拟</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网络流</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>贪心</t>
     </r>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -22750,6 +22874,159 @@
   </sheetData>
   <autoFilter ref="A1:G178"/>
   <mergeCells count="164">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -22761,159 +23038,6 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -22923,17 +23047,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="1"/>
     <col min="2" max="2" width="35.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1"/>
     <col min="5" max="5" width="33.140625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="17.7109375" style="1"/>
@@ -22964,16 +23088,19 @@
         <v>1022</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1023</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1024</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1025</v>
+      <c r="F2" s="1" t="s">
+        <v>1092</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -22981,10 +23108,10 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1026</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1027</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -22998,16 +23125,16 @@
         <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>1029</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -23018,13 +23145,13 @@
         <v>3569</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>1031</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -23035,13 +23162,13 @@
         <v>4230</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -23049,16 +23176,16 @@
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>1035</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -23066,16 +23193,16 @@
         <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>1037</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>1038</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -23083,16 +23210,16 @@
         <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>1041</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>1042</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>19</v>
@@ -23103,30 +23230,30 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>1044</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>1046</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>1047</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -23134,16 +23261,16 @@
         <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>1050</v>
-      </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -23151,16 +23278,16 @@
         <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>1052</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -23168,16 +23295,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>1055</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -23188,13 +23315,13 @@
         <v>6130</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>1057</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21">
@@ -23205,61 +23332,61 @@
         <v>4934</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>1059</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>1060</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="21">
+    <row r="17" spans="1:6" ht="21">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>1061</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>1062</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="21">
+    </row>
+    <row r="18" spans="1:6" ht="21">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>1064</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>1065</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="21">
+    </row>
+    <row r="19" spans="1:6" ht="21">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>1067</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1068</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -23268,106 +23395,160 @@
         <v>566</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="21">
+    <row r="20" spans="1:6" ht="21">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>1067</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>1068</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>1070</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>1073</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
         <v>1075</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>1077</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>1081</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>1076</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E24" s="1" t="s">
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
         <v>1086</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>1076</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1080</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1082</v>
+      <c r="B26" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1063</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add nflsoj260, gym101617a and gym101617b
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$131</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303">
   <si>
     <t>OJ</t>
   </si>
@@ -15658,6 +15658,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>思维</t>
     </r>
     <r>
@@ -15671,6 +15676,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>贪心</t>
@@ -15681,6 +15687,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>思维</t>
     </r>
     <r>
@@ -15694,6 +15705,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>随机</t>
@@ -15709,6 +15721,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>二维</t>
@@ -15724,11 +15737,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
       <t>[</t>
     </r>
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>六校联合训练</t>
@@ -15744,6 +15763,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>树</t>
@@ -15751,11 +15771,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
       <t>[</t>
     </r>
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>六校联合训练</t>
@@ -15771,6 +15797,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>环</t>
@@ -15778,11 +15805,37 @@
   </si>
   <si>
     <r>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>容斥</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
       <t>[</t>
     </r>
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>六校联合训练</t>
@@ -15798,6 +15851,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>礼物</t>
@@ -15805,6 +15859,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>组合数</t>
     </r>
     <r>
@@ -15818,6 +15877,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>思维</t>
@@ -15833,6 +15893,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>根号暴力</t>
@@ -15843,11 +15904,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
       <t>dp;</t>
     </r>
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>凸壳</t>
@@ -15863,6 +15930,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>思维</t>
@@ -15886,6 +15954,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>套</t>
@@ -15907,6 +15976,18 @@
   </si>
   <si>
     <t>upit</t>
+  </si>
+  <si>
+    <t>101617A</t>
+  </si>
+  <si>
+    <t>Ducks in a Row</t>
+  </si>
+  <si>
+    <t>101617B</t>
+  </si>
+  <si>
+    <t>Exciting Finish</t>
   </si>
 </sst>
 </file>
@@ -15914,12 +15995,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -15973,17 +16054,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -15995,9 +16084,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16012,14 +16108,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16029,6 +16141,12 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -16058,15 +16176,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16079,53 +16196,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -16138,7 +16213,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16150,7 +16291,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16162,85 +16375,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16252,73 +16387,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16346,6 +16421,32 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -16380,17 +16481,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -16414,216 +16504,201 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="66">
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -26308,8 +26383,8 @@
   <sheetPr/>
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="B119" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -28302,58 +28377,58 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="121" ht="21" spans="1:5">
+    <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B121" s="1">
         <v>256</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="C121" s="3" t="s">
         <v>1283</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E121" s="5" t="s">
+      <c r="E121" s="3" t="s">
         <v>1284</v>
       </c>
     </row>
-    <row r="122" ht="21" spans="1:5">
+    <row r="122" spans="1:5">
       <c r="A122" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B122" s="1">
         <v>257</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C122" s="3" t="s">
         <v>724</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E122" s="5" t="s">
+      <c r="E122" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="123" ht="21" spans="1:5">
+    <row r="123" spans="1:5">
       <c r="A123" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B123" s="1">
         <v>258</v>
       </c>
-      <c r="C123" s="5" t="s">
+      <c r="C123" s="3" t="s">
         <v>1285</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E123" s="5" t="s">
+      <c r="E123" s="3" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="124" ht="21" spans="1:5">
+    <row r="124" spans="1:5">
       <c r="A124" s="1" t="s">
         <v>212</v>
       </c>
@@ -28366,7 +28441,7 @@
       <c r="D124" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E124" s="5" t="s">
+      <c r="E124" s="3" t="s">
         <v>1248</v>
       </c>
     </row>
@@ -28381,11 +28456,13 @@
         <v>1288</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E125" s="5"/>
-    </row>
-    <row r="126" ht="21" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="1" t="s">
         <v>212</v>
       </c>
@@ -28393,30 +28470,30 @@
         <v>261</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E126" s="5" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="127" ht="21" spans="1:5">
+      <c r="E126" s="3" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B127" s="1">
         <v>262</v>
       </c>
-      <c r="C127" s="5" t="s">
-        <v>1291</v>
+      <c r="C127" s="3" t="s">
+        <v>1292</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="128" ht="21" spans="1:5">
@@ -28426,34 +28503,34 @@
       <c r="B128" s="1">
         <v>263</v>
       </c>
-      <c r="C128" s="5" t="s">
-        <v>1293</v>
+      <c r="C128" s="3" t="s">
+        <v>1294</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="129" ht="21" spans="1:5">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B129" s="1">
         <v>264</v>
       </c>
-      <c r="C129" s="5" t="s">
-        <v>1295</v>
+      <c r="C129" s="3" t="s">
+        <v>1296</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E129" s="5" t="s">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="130" ht="21" spans="1:5">
+      <c r="E129" s="3" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
         <v>1277</v>
       </c>
@@ -28461,18 +28538,51 @@
         <v>4018</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E130" s="5" t="s">
+      <c r="E130" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="132" ht="12"/>
+    <row r="131" spans="1:5">
+      <c r="A131" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F120"/>
+  <autoFilter ref="A1:F131"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add bzoj3189 and scu141
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$132</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307">
   <si>
     <t>OJ</t>
   </si>
@@ -15805,6 +15805,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>思维</t>
     </r>
     <r>
@@ -15818,6 +15823,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>容斥</t>
@@ -15941,6 +15947,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>数位</t>
     </r>
     <r>
@@ -15988,6 +15999,18 @@
   </si>
   <si>
     <t>Exciting Finish</t>
+  </si>
+  <si>
+    <t>Jumping Joe</t>
+  </si>
+  <si>
+    <t>扩展欧几里得</t>
+  </si>
+  <si>
+    <t>[COCI2011]Slika</t>
+  </si>
+  <si>
+    <t>并查集</t>
   </si>
 </sst>
 </file>
@@ -15995,10 +16018,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -16047,13 +16070,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -16069,23 +16085,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -16099,68 +16115,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16176,7 +16132,81 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16189,18 +16219,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -16219,13 +16242,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16237,7 +16290,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16249,13 +16332,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16267,85 +16398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16357,43 +16410,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16425,6 +16448,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -16436,32 +16468,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -16481,6 +16487,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -16496,11 +16513,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -16527,181 +16550,181 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -16742,12 +16765,12 @@
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 9" xfId="1"/>
-    <cellStyle name="常规 6" xfId="2"/>
-    <cellStyle name="常规 16" xfId="3"/>
-    <cellStyle name="常规 15" xfId="4"/>
-    <cellStyle name="常规 13" xfId="5"/>
-    <cellStyle name="常规 11" xfId="6"/>
+    <cellStyle name="常规 11" xfId="1"/>
+    <cellStyle name="常规 13" xfId="2"/>
+    <cellStyle name="常规 15" xfId="3"/>
+    <cellStyle name="常规 16" xfId="4"/>
+    <cellStyle name="常规 6" xfId="5"/>
+    <cellStyle name="常规 9" xfId="6"/>
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="8" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="9" builtinId="48"/>
@@ -26381,10 +26404,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B119" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -28445,7 +28468,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="125" ht="21" spans="1:5">
+    <row r="125" spans="1:5">
       <c r="A125" s="1" t="s">
         <v>212</v>
       </c>
@@ -28458,7 +28481,7 @@
       <c r="D125" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="5" t="s">
+      <c r="E125" s="3" t="s">
         <v>1289</v>
       </c>
     </row>
@@ -28496,7 +28519,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="128" ht="21" spans="1:5">
+    <row r="128" spans="1:5">
       <c r="A128" s="1" t="s">
         <v>212</v>
       </c>
@@ -28509,7 +28532,7 @@
       <c r="D128" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E128" s="5" t="s">
+      <c r="E128" s="3" t="s">
         <v>1295</v>
       </c>
     </row>
@@ -28581,8 +28604,59 @@
         <v>162</v>
       </c>
     </row>
+    <row r="133" ht="21" spans="1:5">
+      <c r="A133" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B133" s="1">
+        <v>141</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="134" ht="21" spans="1:5">
+      <c r="A134" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B134" s="1">
+        <v>3189</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="135" ht="21" spans="1:5">
+      <c r="A135" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B135" s="1">
+        <v>3189</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>1306</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F131"/>
+  <autoFilter ref="A1:F132"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
modify some filenames and add nflsoj274,nflsoj283 and nflsoj284
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$156</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351">
   <si>
     <t>OJ</t>
   </si>
@@ -16503,6 +16503,173 @@
   </si>
   <si>
     <t>KMP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>六校联合训练</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> #13]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>石子</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>博弈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>找规律</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>六校联合训练</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> #13]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>矩阵</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>链表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>大模拟</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>六校联合训练</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> #11]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>白色糖果</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>矩阵快速幂</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -16510,10 +16677,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -16562,14 +16729,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -16577,9 +16736,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16589,21 +16756,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -16622,14 +16774,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -16639,7 +16783,57 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16653,23 +16847,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16683,12 +16870,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -16696,24 +16878,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -16728,25 +16895,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16758,13 +16913,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16776,25 +16955,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16806,43 +16991,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16854,31 +17015,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16896,19 +17033,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -16922,21 +17089,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -16946,11 +17098,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -16981,17 +17139,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -17011,11 +17172,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -17045,187 +17212,187 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -26908,10 +27075,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" topLeftCell="B148" workbookViewId="0">
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -29445,7 +29612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" ht="21" spans="1:5">
+    <row r="153" spans="1:5">
       <c r="A153" s="1" t="s">
         <v>15</v>
       </c>
@@ -29458,7 +29625,7 @@
       <c r="D153" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E153" s="5" t="s">
+      <c r="E153" s="3" t="s">
         <v>1341</v>
       </c>
     </row>
@@ -29479,8 +29646,59 @@
         <v>1344</v>
       </c>
     </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B155" s="1">
+        <v>283</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B156" s="1">
+        <v>284</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="157" ht="21" spans="1:5">
+      <c r="A157" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B157" s="1">
+        <v>274</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>1350</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F154"/>
+  <autoFilter ref="A1:F156"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add nflsoj292 and nflsoj293
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$175</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387">
   <si>
     <t>OJ</t>
   </si>
@@ -17246,11 +17246,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
       <t>Fairy(</t>
     </r>
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>树链剖分</t>
@@ -17266,11 +17272,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
       <t>dfs</t>
     </r>
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>树</t>
@@ -17286,6 +17298,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>树链剖分</t>
@@ -17301,6 +17314,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>思维</t>
@@ -17311,6 +17325,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>贪心</t>
     </r>
     <r>
@@ -17324,6 +17343,7 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>三分</t>
@@ -17334,6 +17354,19 @@
   </si>
   <si>
     <t>Unambiguous Arithmetic Expression</t>
+  </si>
+  <si>
+    <r>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;set</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -17342,11 +17375,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -17400,9 +17433,137 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -17421,140 +17582,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -17565,7 +17592,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17577,13 +17640,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17595,7 +17670,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17607,13 +17688,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17625,79 +17754,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17709,43 +17772,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17759,35 +17786,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -17839,6 +17842,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -17851,203 +17863,209 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="71">
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -18056,16 +18074,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -18109,14 +18136,14 @@
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 9" xfId="1"/>
-    <cellStyle name="常规 6" xfId="2"/>
-    <cellStyle name="常规 21" xfId="3"/>
-    <cellStyle name="常规 16" xfId="4"/>
-    <cellStyle name="常规 20" xfId="5"/>
-    <cellStyle name="常规 15" xfId="6"/>
-    <cellStyle name="常规 13" xfId="7"/>
-    <cellStyle name="常规 11" xfId="8"/>
+    <cellStyle name="常规 11" xfId="1"/>
+    <cellStyle name="常规 13" xfId="2"/>
+    <cellStyle name="常规 15" xfId="3"/>
+    <cellStyle name="常规 20" xfId="4"/>
+    <cellStyle name="常规 16" xfId="5"/>
+    <cellStyle name="常规 21" xfId="6"/>
+    <cellStyle name="常规 6" xfId="7"/>
+    <cellStyle name="常规 9" xfId="8"/>
     <cellStyle name="60% - Accent6" xfId="9" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="10" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="11" builtinId="48"/>
@@ -18144,8 +18171,8 @@
     <cellStyle name="Accent1" xfId="33" builtinId="29"/>
     <cellStyle name="Comma[0]" xfId="34" builtinId="6"/>
     <cellStyle name="Neutral" xfId="35" builtinId="28"/>
-    <cellStyle name="常规 22" xfId="36"/>
-    <cellStyle name="常规 17" xfId="37"/>
+    <cellStyle name="常规 17" xfId="36"/>
+    <cellStyle name="常规 22" xfId="37"/>
     <cellStyle name="60% - Accent1" xfId="38" builtinId="32"/>
     <cellStyle name="Bad" xfId="39" builtinId="27"/>
     <cellStyle name="20% - Accent4" xfId="40" builtinId="42"/>
@@ -27753,10 +27780,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B165" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -30639,7 +30666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" ht="21" spans="1:6">
+    <row r="173" spans="1:6">
       <c r="A173" s="1" t="s">
         <v>15</v>
       </c>
@@ -30659,7 +30686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" ht="21" spans="1:6">
+    <row r="174" spans="1:6">
       <c r="A174" s="1" t="s">
         <v>15</v>
       </c>
@@ -30672,7 +30699,7 @@
       <c r="D174" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E174" s="5" t="s">
+      <c r="E174" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F174" s="1" t="s">
@@ -30699,8 +30726,42 @@
         <v>19</v>
       </c>
     </row>
+    <row r="176" ht="21" spans="1:5">
+      <c r="A176" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B176" s="1">
+        <v>292</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B177" s="1">
+        <v>293</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F172"/>
+  <autoFilter ref="A1:F175"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add cf20c,24b,455a,592c and nflsoj294, modify .gitignore
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$177</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388">
   <si>
     <t>OJ</t>
   </si>
@@ -17357,6 +17357,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>思维</t>
     </r>
     <r>
@@ -17366,6 +17371,26 @@
         <charset val="134"/>
       </rPr>
       <t>;set</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>树上莫队</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分块</t>
     </r>
   </si>
 </sst>
@@ -17374,10 +17399,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -17433,42 +17458,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -17486,16 +17479,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -17516,36 +17502,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -17559,11 +17517,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -17575,9 +17540,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -17592,7 +17617,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17604,19 +17629,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17628,25 +17647,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17658,7 +17659,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17676,13 +17689,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17694,85 +17797,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -17790,7 +17815,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -17825,6 +17850,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -17845,41 +17905,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -17912,85 +17937,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -17999,97 +18024,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -18136,14 +18161,14 @@
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 11" xfId="1"/>
-    <cellStyle name="常规 13" xfId="2"/>
-    <cellStyle name="常规 15" xfId="3"/>
-    <cellStyle name="常规 20" xfId="4"/>
-    <cellStyle name="常规 16" xfId="5"/>
-    <cellStyle name="常规 21" xfId="6"/>
-    <cellStyle name="常规 6" xfId="7"/>
-    <cellStyle name="常规 9" xfId="8"/>
+    <cellStyle name="常规 9" xfId="1"/>
+    <cellStyle name="常规 6" xfId="2"/>
+    <cellStyle name="常规 21" xfId="3"/>
+    <cellStyle name="常规 16" xfId="4"/>
+    <cellStyle name="常规 20" xfId="5"/>
+    <cellStyle name="常规 15" xfId="6"/>
+    <cellStyle name="常规 13" xfId="7"/>
+    <cellStyle name="常规 11" xfId="8"/>
     <cellStyle name="60% - Accent6" xfId="9" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="10" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="11" builtinId="48"/>
@@ -18171,8 +18196,8 @@
     <cellStyle name="Accent1" xfId="33" builtinId="29"/>
     <cellStyle name="Comma[0]" xfId="34" builtinId="6"/>
     <cellStyle name="Neutral" xfId="35" builtinId="28"/>
-    <cellStyle name="常规 17" xfId="36"/>
-    <cellStyle name="常规 22" xfId="37"/>
+    <cellStyle name="常规 22" xfId="36"/>
+    <cellStyle name="常规 17" xfId="37"/>
     <cellStyle name="60% - Accent1" xfId="38" builtinId="32"/>
     <cellStyle name="Bad" xfId="39" builtinId="27"/>
     <cellStyle name="20% - Accent4" xfId="40" builtinId="42"/>
@@ -27780,10 +27805,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F177"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="E177" sqref="E177"/>
+      <selection activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -30726,7 +30751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="176" ht="21" spans="1:5">
+    <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
         <v>212</v>
       </c>
@@ -30739,7 +30764,7 @@
       <c r="D176" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E176" s="5" t="s">
+      <c r="E176" s="3" t="s">
         <v>1386</v>
       </c>
     </row>
@@ -30760,8 +30785,25 @@
         <v>162</v>
       </c>
     </row>
+    <row r="178" ht="21" spans="1:5">
+      <c r="A178" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B178" s="1">
+        <v>294</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>1387</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F175"/>
+  <autoFilter ref="A1:F177"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add nflsoj270,uoj262 and uoj264
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3238" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3246" uniqueCount="1426">
   <si>
     <t>OJ</t>
   </si>
@@ -18364,6 +18364,110 @@
   </si>
   <si>
     <t>高斯消元</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>UOJ</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2016]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>蚯蚓</t>
+    </r>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>队列</t>
+    </r>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2016]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>换教室</t>
+    </r>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最短路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>概率</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -28199,6 +28303,159 @@
   </sheetData>
   <autoFilter ref="A1:G178"/>
   <mergeCells count="164">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -28210,159 +28467,6 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -28372,10 +28476,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F192"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E193" sqref="E193"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
@@ -30756,7 +30860,7 @@
         <v>1321</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>11</v>
+        <v>1422</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>1322</v>
@@ -31611,6 +31715,40 @@
       </c>
       <c r="E192" s="4" t="s">
         <v>1419</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B193" s="1">
+        <v>264</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B194" s="1">
+        <v>262</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>1425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add apc001G(unfinished),2 solutions of nflspc #1 and tcsrm726div1&2c
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3316" uniqueCount="1454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3361" uniqueCount="1486">
   <si>
     <t>OJ</t>
   </si>
@@ -19043,6 +19043,379 @@
   </si>
   <si>
     <t>计算几何</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFLSoj</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Jiangsu Training Contest #5]Graph</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Jiangsu Training Contest #5]Palindrome</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>离线</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>并查集</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树合并</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>AC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>自动机</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>复杂度分析</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">NFLSoj </t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Jiangsu Training Contest #5]Bishop</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>容斥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;NTT;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Jiangsu Training Contest #6]Decompose</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>拉格朗日插值</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>取石子游戏</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>博弈</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPOJ</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIVCNT3</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>CodeChef</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDGEST</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edges in Spanning Tree</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>差分</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>搜索</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;BIT</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountingDivisors(cube)</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>洲阁筛</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOJ</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单的函数</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unfinished</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>TopCoder</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRM726DIV2C</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRM726DIV1C</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>HeroicScheduled2</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>HeroicSchedule</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>贪心</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>状压</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>拟阵</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>贪心</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
@@ -29073,17 +29446,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F210"/>
+  <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F206" sqref="F206"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1"/>
     <col min="5" max="5" width="50.42578125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="17.7109375" style="1"/>
@@ -29923,7 +30296,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
         <v>6</v>
       </c>
@@ -29940,7 +30313,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
         <v>6</v>
       </c>
@@ -29957,7 +30330,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -29974,7 +30347,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -29991,7 +30364,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -30008,7 +30381,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
         <v>6</v>
       </c>
@@ -30025,7 +30398,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
@@ -30041,8 +30414,11 @@
       <c r="E55" s="1" t="s">
         <v>1147</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="1" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -30059,7 +30435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
         <v>260</v>
       </c>
@@ -30076,7 +30452,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
         <v>260</v>
       </c>
@@ -30093,7 +30469,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:6">
       <c r="B59" s="1" t="s">
         <v>1154</v>
       </c>
@@ -30107,7 +30483,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:6">
       <c r="B60" s="1" t="s">
         <v>1156</v>
       </c>
@@ -30121,7 +30497,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:6">
       <c r="B61" s="1" t="s">
         <v>1159</v>
       </c>
@@ -30135,7 +30511,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:6">
       <c r="B62" s="1" t="s">
         <v>1162</v>
       </c>
@@ -30149,7 +30525,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:6">
       <c r="B63" s="1" t="s">
         <v>1164</v>
       </c>
@@ -30163,7 +30539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:6">
       <c r="B64" s="1" t="s">
         <v>1166</v>
       </c>
@@ -32633,6 +33009,176 @@
       </c>
       <c r="E210" s="4" t="s">
         <v>1452</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B211" s="1">
+        <v>322</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B212" s="1">
+        <v>323</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B213" s="1">
+        <v>324</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B214" s="1">
+        <v>325</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B215" s="1">
+        <v>331</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E215" s="4" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E216" s="4" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B218" s="1">
+        <v>6053</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="E218" s="4" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>1484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add atcoder4415,atcoder4417,gym101955a,nflsoj247,usaco2018 2 solutions
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -13,7 +13,7 @@
     <sheet name="2018-2019秋季" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$223</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$229</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3384" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1504">
   <si>
     <t>OJ</t>
   </si>
@@ -19463,6 +19463,221 @@
   </si>
   <si>
     <t>LCT;SAM</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>UOJ</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[NOI2014]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>魔法森林</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCT</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>组合数学</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtCoder</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>[JAGSC2018]Short LIS</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>[JAGSC2018]ADD DIV MAX RESTORE</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>GYM</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>101955A</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sockpuppets</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Trie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>树型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>树上背包</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>USACO</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018 December A</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Balanced Beam</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>凸包</t>
+    </r>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -29472,17 +29687,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F225"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E226" sqref="E226"/>
+    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E231" sqref="E231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1"/>
     <col min="5" max="5" width="50.42578125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="17.7109375" style="1"/>
@@ -31262,7 +31477,10 @@
         <v>1258</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>11</v>
+        <v>1486</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>1487</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -33277,8 +33495,11 @@
       <c r="E224" s="1" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="225" spans="1:5">
+      <c r="F224" s="1" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
       <c r="A225" s="1" t="s">
         <v>1479</v>
       </c>
@@ -33294,9 +33515,106 @@
       <c r="E225" s="1" t="s">
         <v>1482</v>
       </c>
+      <c r="F225" s="1" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B226" s="1">
+        <v>3</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D226" s="1">
+        <v>97</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B227" s="1">
+        <v>4417</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>1487</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B228" s="1">
+        <v>4415</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>1503</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F223"/>
+  <autoFilter ref="A1:F229"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modify agc029d and add uoj207
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$235</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$236</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510">
   <si>
     <t>OJ</t>
   </si>
@@ -18984,6 +18984,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>网络流</t>
     </r>
     <r>
@@ -18997,9 +19002,26 @@
     <r>
       <rPr>
         <sz val="16"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>思维</t>
+    </r>
+  </si>
+  <si>
+    <t>共价大爷游长沙</t>
+  </si>
+  <si>
+    <r>
+      <t>随机</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;LCT</t>
     </r>
   </si>
 </sst>
@@ -19008,10 +19030,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -19075,8 +19097,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19105,11 +19143,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19128,17 +19166,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19151,18 +19203,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19179,22 +19224,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -19204,14 +19233,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19227,18 +19249,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19262,7 +19272,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19274,7 +19296,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19286,7 +19344,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19298,73 +19410,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19376,37 +19428,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19444,15 +19466,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -19464,6 +19477,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19485,15 +19513,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -19503,17 +19522,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19552,58 +19574,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -19612,34 +19634,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -19648,55 +19670,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -19705,37 +19727,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -19788,15 +19810,15 @@
   </cellXfs>
   <cellStyles count="77">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 9" xfId="1"/>
-    <cellStyle name="常规 6" xfId="2"/>
-    <cellStyle name="常规 28" xfId="3"/>
-    <cellStyle name="常规 21" xfId="4"/>
+    <cellStyle name="常规 11" xfId="1"/>
+    <cellStyle name="常规 13" xfId="2"/>
+    <cellStyle name="常规 15" xfId="3"/>
+    <cellStyle name="常规 20" xfId="4"/>
     <cellStyle name="常规 16" xfId="5"/>
-    <cellStyle name="常规 20" xfId="6"/>
-    <cellStyle name="常规 15" xfId="7"/>
-    <cellStyle name="常规 13" xfId="8"/>
-    <cellStyle name="常规 11" xfId="9"/>
+    <cellStyle name="常规 21" xfId="6"/>
+    <cellStyle name="常规 28" xfId="7"/>
+    <cellStyle name="常规 6" xfId="8"/>
+    <cellStyle name="常规 9" xfId="9"/>
     <cellStyle name="常规 27" xfId="10"/>
     <cellStyle name="60% - Accent6" xfId="11" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="12" builtinId="51"/>
@@ -19816,8 +19838,8 @@
     <cellStyle name="Accent4" xfId="26" builtinId="41"/>
     <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39"/>
-    <cellStyle name="常规 23" xfId="29"/>
-    <cellStyle name="常规 18" xfId="30"/>
+    <cellStyle name="常规 18" xfId="29"/>
+    <cellStyle name="常规 23" xfId="30"/>
     <cellStyle name="60% - Accent2" xfId="31" builtinId="36"/>
     <cellStyle name="常规 2" xfId="32"/>
     <cellStyle name="Accent3" xfId="33" builtinId="37"/>
@@ -19828,8 +19850,8 @@
     <cellStyle name="Accent1" xfId="38" builtinId="29"/>
     <cellStyle name="Comma[0]" xfId="39" builtinId="6"/>
     <cellStyle name="Neutral" xfId="40" builtinId="28"/>
-    <cellStyle name="常规 22" xfId="41"/>
-    <cellStyle name="常规 17" xfId="42"/>
+    <cellStyle name="常规 17" xfId="41"/>
+    <cellStyle name="常规 22" xfId="42"/>
     <cellStyle name="60% - Accent1" xfId="43" builtinId="32"/>
     <cellStyle name="Bad" xfId="44" builtinId="27"/>
     <cellStyle name="20% - Accent4" xfId="45" builtinId="42"/>
@@ -19847,8 +19869,8 @@
     <cellStyle name="Good" xfId="57" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="58" builtinId="18"/>
     <cellStyle name="CExplanatory Text" xfId="59" builtinId="53"/>
-    <cellStyle name="常规 24" xfId="60"/>
-    <cellStyle name="常规 19" xfId="61"/>
+    <cellStyle name="常规 19" xfId="60"/>
+    <cellStyle name="常规 24" xfId="61"/>
     <cellStyle name="60% - Accent3" xfId="62" builtinId="40"/>
     <cellStyle name="Currency[0]" xfId="63" builtinId="7"/>
     <cellStyle name="Heading 1" xfId="64" builtinId="16"/>
@@ -29438,10 +29460,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F236"/>
+  <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C239" sqref="C239"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="E238" sqref="E238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -32850,7 +32872,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:6">
       <c r="A202" s="1" t="s">
         <v>473</v>
       </c>
@@ -32865,6 +32887,9 @@
       </c>
       <c r="E202" s="4" t="s">
         <v>1380</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -33452,7 +33477,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="236" ht="21" spans="1:5">
+    <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
         <v>83</v>
       </c>
@@ -33465,12 +33490,29 @@
       <c r="D236" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E236" s="5" t="s">
+      <c r="E236" s="3" t="s">
         <v>1507</v>
       </c>
     </row>
+    <row r="237" ht="21" spans="1:5">
+      <c r="A237" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B237" s="1">
+        <v>207</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E237" s="5" t="s">
+        <v>1509</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F235"/>
+  <autoFilter ref="A1:F236"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
modify nflsoj301,305 and add nflsoj312,313,314,315,342,343,344
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -16,14 +16,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018寒假'!$A$1:$F$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018春季'!$A$1:$F$262</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2018暑假'!$A$1:$G$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2018-2019秋季'!$A$1:$F$240</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524">
   <si>
     <t>OJ</t>
   </si>
@@ -19013,6 +19013,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>随机</t>
     </r>
     <r>
@@ -19022,6 +19027,254 @@
         <charset val="134"/>
       </rPr>
       <t>;LCT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[Jiangsu Training Contest #7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>偷吃巧克力</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>dp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[Jiangsu Training Contest #7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>卡片</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;dp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>背包</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[Jiangsu Training Contest #7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>连通</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分治</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树合并</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可撤销并查集</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2018]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>铺设道路</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2018]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>货币系统</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;dp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2018]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>赛道修建</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>二分答案</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <charset val="134"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>贪心</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2018]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>旅行</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2018]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>填数游戏</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[NOIP2018]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <charset val="134"/>
+      </rPr>
+      <t>保卫王国</t>
     </r>
   </si>
 </sst>
@@ -19030,10 +19283,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -19090,14 +19343,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -19105,9 +19350,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19121,25 +19365,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19152,7 +19381,67 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19167,22 +19456,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19197,45 +19471,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -19248,7 +19501,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19260,25 +19585,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19290,43 +19609,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19338,73 +19633,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19422,13 +19657,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19439,21 +19692,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -19482,6 +19720,45 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -19492,21 +19769,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19527,15 +19789,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19574,58 +19827,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -19634,34 +19887,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -19670,55 +19923,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -19727,43 +19980,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -29460,10 +29713,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F237"/>
+  <dimension ref="A1:F246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="E238" sqref="E238"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="E245" sqref="E245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7083333333333" defaultRowHeight="18.75" outlineLevelCol="5"/>
@@ -33392,7 +33645,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:6">
       <c r="A231" s="1" t="s">
         <v>83</v>
       </c>
@@ -33408,8 +33661,11 @@
       <c r="E231" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="232" spans="1:5">
+      <c r="F231" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
       <c r="A232" s="1" t="s">
         <v>83</v>
       </c>
@@ -33425,8 +33681,11 @@
       <c r="E232" s="3" t="s">
         <v>1496</v>
       </c>
-    </row>
-    <row r="233" spans="1:5">
+      <c r="F232" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
       <c r="A233" s="1" t="s">
         <v>83</v>
       </c>
@@ -33442,8 +33701,11 @@
       <c r="E233" s="3" t="s">
         <v>1499</v>
       </c>
-    </row>
-    <row r="234" spans="1:5">
+      <c r="F233" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
       <c r="A234" s="1" t="s">
         <v>83</v>
       </c>
@@ -33459,8 +33721,11 @@
       <c r="E234" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="235" spans="1:5">
+      <c r="F234" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
       <c r="A235" s="1" t="s">
         <v>83</v>
       </c>
@@ -33476,8 +33741,11 @@
       <c r="E235" s="3" t="s">
         <v>1504</v>
       </c>
-    </row>
-    <row r="236" spans="1:5">
+      <c r="F235" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
       <c r="A236" s="1" t="s">
         <v>83</v>
       </c>
@@ -33493,26 +33761,176 @@
       <c r="E236" s="3" t="s">
         <v>1507</v>
       </c>
-    </row>
-    <row r="237" ht="21" spans="1:5">
+      <c r="F236" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B237" s="1">
         <v>207</v>
       </c>
-      <c r="C237" s="5" t="s">
+      <c r="C237" s="3" t="s">
         <v>1508</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E237" s="5" t="s">
+      <c r="E237" s="3" t="s">
         <v>1509</v>
       </c>
     </row>
+    <row r="238" ht="21" spans="1:5">
+      <c r="A238" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B238" s="1">
+        <v>342</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="239" ht="21" spans="1:5">
+      <c r="A239" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B239" s="1">
+        <v>343</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E239" s="5" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B240" s="1">
+        <v>344</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="241" ht="21" spans="1:5">
+      <c r="A241" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B241" s="1">
+        <v>312</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E241" s="5" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="242" ht="21" spans="1:5">
+      <c r="A242" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B242" s="1">
+        <v>313</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E242" s="5" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="243" ht="21" spans="1:5">
+      <c r="A243" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B243" s="1">
+        <v>314</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E243" s="5" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="244" ht="21" spans="1:5">
+      <c r="A244" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B244" s="1">
+        <v>315</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E244" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="245" ht="21" spans="1:4">
+      <c r="A245" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B245" s="1">
+        <v>316</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="246" ht="21" spans="1:4">
+      <c r="A246" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B246" s="1">
+        <v>317</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F236"/>
+  <autoFilter ref="A1:F240"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add nflsoj346,347 and luogu4719
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3512" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3519" uniqueCount="1543">
   <si>
     <t>OJ</t>
   </si>
@@ -20280,7 +20280,138 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Unfinished</t>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;dp</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>莫比乌斯函数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数学</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>字符串</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>洛谷</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>【模板】动态</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>动态</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>dp</t>
+    </r>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -30130,6 +30261,159 @@
   </sheetData>
   <autoFilter ref="A1:G178"/>
   <mergeCells count="164">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -30141,159 +30425,6 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -30303,10 +30434,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F252"/>
+  <dimension ref="A1:F253"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A230" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A252" sqref="A252"/>
+      <selection activeCell="F253" sqref="F253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
@@ -34601,7 +34732,13 @@
         <v>1534</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1536</v>
+        <v>1532</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>1537</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>1538</v>
       </c>
     </row>
     <row r="252" spans="1:6">
@@ -34615,7 +34752,27 @@
         <v>1535</v>
       </c>
       <c r="D252" s="1" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E252" s="1" t="s">
         <v>1536</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6">
+      <c r="A253" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B253" s="1">
+        <v>4719</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>1542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cf700e,uoj79,hdu4687 and modify uoj80
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="1545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3544" uniqueCount="1556">
   <si>
     <t>OJ</t>
   </si>
@@ -20481,6 +20481,78 @@
       </rPr>
       <t>线段树合并</t>
     </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Codeforces</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>700E</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cool Slogans</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SAM;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线段树合并</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>UOJ</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般图最大匹配</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>带花树算法</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boke and Tsukkomi</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -30498,10 +30570,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F255"/>
+  <dimension ref="A1:F258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E256" sqref="E256"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E259" sqref="E259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
@@ -34882,6 +34954,57 @@
         <v>1544</v>
       </c>
     </row>
+    <row r="256" spans="1:6">
+      <c r="A256" s="1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B257" s="1">
+        <v>79</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E257" s="4" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B258" s="1">
+        <v>4687</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E258" s="4" t="s">
+        <v>1554</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F253"/>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
add hdu4690 and hdu4691
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3544" uniqueCount="1556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="1563">
   <si>
     <t>OJ</t>
   </si>
@@ -20553,6 +20553,34 @@
   </si>
   <si>
     <t>Boke and Tsukkomi</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDU</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>EBCDIC</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Front Compression</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>后缀数组</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -21826,8 +21854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -30397,6 +30425,159 @@
   </sheetData>
   <autoFilter ref="A1:G178"/>
   <mergeCells count="164">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -30408,159 +30589,6 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -30570,10 +30598,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F258"/>
+  <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E259" sqref="E259"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F256" sqref="F256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
@@ -34953,6 +34981,9 @@
       <c r="E255" s="1" t="s">
         <v>1544</v>
       </c>
+      <c r="F255" s="1" t="s">
+        <v>1562</v>
+      </c>
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="1" t="s">
@@ -35003,6 +35034,40 @@
       </c>
       <c r="E258" s="4" t="s">
         <v>1554</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B259" s="1">
+        <v>4690</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="E259" s="4" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B260" s="1">
+        <v>4691</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="E260" s="4" t="s">
+        <v>1561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a tle version of uoj422
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="1569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="1574">
   <si>
     <t>OJ</t>
   </si>
@@ -20685,6 +20685,51 @@
   </si>
   <si>
     <t>思维</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>TopCoder</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRM575DIV1C</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>TheTilesDivOne</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网络流</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大流</t>
+    </r>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -30529,6 +30574,159 @@
   </sheetData>
   <autoFilter ref="A1:G178"/>
   <mergeCells count="164">
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
     <mergeCell ref="D188:E188"/>
     <mergeCell ref="D189:E189"/>
     <mergeCell ref="D179:E179"/>
@@ -30540,159 +30738,6 @@
     <mergeCell ref="D185:E185"/>
     <mergeCell ref="D186:E186"/>
     <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -30702,10 +30747,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F262"/>
+  <dimension ref="A1:F263"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A241" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B263" sqref="B263"/>
+      <selection activeCell="E264" sqref="E264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
@@ -35202,6 +35247,23 @@
         <v>1568</v>
       </c>
     </row>
+    <row r="263" spans="1:5">
+      <c r="A263" s="1" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>1573</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F253"/>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
add bzoj3456,tsinsenA1493,tsinsenA1513,uoj118 and ural1469(unfinished)
</commit_message>
<xml_diff>
--- a/Problem List.xlsx
+++ b/Problem List.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="1589">
   <si>
     <t>OJ</t>
   </si>
@@ -21030,6 +21030,105 @@
       </rPr>
       <t>二分图最大权匹配</t>
     </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>TopCoder</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRM577DIV1C</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardPainting</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>思维</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二分图最大独立集</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大流</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Apple Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>网络流</t>
+    </r>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>BZOJ</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市规划</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accepted</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>多项式求逆</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -27568,7 +27667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -31064,10 +31163,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F271"/>
+  <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E271" sqref="E271"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E274" sqref="E274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="20.25"/>
@@ -31076,7 +31175,7 @@
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1"/>
-    <col min="5" max="5" width="50.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="17.7109375" style="1"/>
   </cols>
   <sheetData>
@@ -35721,6 +35820,43 @@
       </c>
       <c r="E271" s="1" t="s">
         <v>1578</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6">
+      <c r="A272" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>1583</v>
+      </c>
+      <c r="F272" s="1" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B273" s="1">
+        <v>3456</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E273" s="4" t="s">
+        <v>1588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>